<commit_message>
Atualização de bases das ligas, do dia: 2024-01-28 às 01-34
</commit_message>
<xml_diff>
--- a/Chile Primera Division/Chile Primera Division.xlsx
+++ b/Chile Primera Division/Chile Primera Division.xlsx
@@ -7042,7 +7042,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>3234177</v>
+        <v>3234974</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7054,73 +7054,73 @@
         <v>44240.77083333334</v>
       </c>
       <c r="F74" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K74">
-        <v>1.85</v>
+        <v>1.75</v>
       </c>
       <c r="L74">
+        <v>3.4</v>
+      </c>
+      <c r="M74">
+        <v>5</v>
+      </c>
+      <c r="N74">
+        <v>1.6</v>
+      </c>
+      <c r="O74">
         <v>3.6</v>
       </c>
-      <c r="M74">
-        <v>4</v>
-      </c>
-      <c r="N74">
-        <v>1.95</v>
-      </c>
-      <c r="O74">
-        <v>3.5</v>
-      </c>
       <c r="P74">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q74">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R74">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S74">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U74">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="V74">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA74">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -7131,7 +7131,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>3234974</v>
+        <v>3234177</v>
       </c>
       <c r="C75" t="s">
         <v>28</v>
@@ -7143,73 +7143,73 @@
         <v>44240.77083333334</v>
       </c>
       <c r="F75" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G75" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H75">
+        <v>2</v>
+      </c>
+      <c r="I75">
         <v>3</v>
       </c>
-      <c r="I75">
+      <c r="J75" t="s">
+        <v>53</v>
+      </c>
+      <c r="K75">
+        <v>1.85</v>
+      </c>
+      <c r="L75">
+        <v>3.6</v>
+      </c>
+      <c r="M75">
+        <v>4</v>
+      </c>
+      <c r="N75">
+        <v>1.95</v>
+      </c>
+      <c r="O75">
+        <v>3.5</v>
+      </c>
+      <c r="P75">
+        <v>4</v>
+      </c>
+      <c r="Q75">
+        <v>-0.5</v>
+      </c>
+      <c r="R75">
+        <v>1.925</v>
+      </c>
+      <c r="S75">
+        <v>1.875</v>
+      </c>
+      <c r="T75">
+        <v>3</v>
+      </c>
+      <c r="U75">
+        <v>2</v>
+      </c>
+      <c r="V75">
+        <v>1.8</v>
+      </c>
+      <c r="W75">
+        <v>-1</v>
+      </c>
+      <c r="X75">
+        <v>-1</v>
+      </c>
+      <c r="Y75">
+        <v>3</v>
+      </c>
+      <c r="Z75">
+        <v>-1</v>
+      </c>
+      <c r="AA75">
+        <v>0.875</v>
+      </c>
+      <c r="AB75">
         <v>1</v>
-      </c>
-      <c r="J75" t="s">
-        <v>52</v>
-      </c>
-      <c r="K75">
-        <v>1.75</v>
-      </c>
-      <c r="L75">
-        <v>3.4</v>
-      </c>
-      <c r="M75">
-        <v>5</v>
-      </c>
-      <c r="N75">
-        <v>1.6</v>
-      </c>
-      <c r="O75">
-        <v>3.6</v>
-      </c>
-      <c r="P75">
-        <v>6</v>
-      </c>
-      <c r="Q75">
-        <v>-0.75</v>
-      </c>
-      <c r="R75">
-        <v>1.8</v>
-      </c>
-      <c r="S75">
-        <v>2</v>
-      </c>
-      <c r="T75">
-        <v>2.75</v>
-      </c>
-      <c r="U75">
-        <v>1.8</v>
-      </c>
-      <c r="V75">
-        <v>2</v>
-      </c>
-      <c r="W75">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="X75">
-        <v>-1</v>
-      </c>
-      <c r="Y75">
-        <v>-1</v>
-      </c>
-      <c r="Z75">
-        <v>0.8</v>
-      </c>
-      <c r="AA75">
-        <v>-1</v>
-      </c>
-      <c r="AB75">
-        <v>0.8</v>
       </c>
       <c r="AC75">
         <v>-1</v>
@@ -31428,7 +31428,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>3898957</v>
+        <v>3899778</v>
       </c>
       <c r="C348" t="s">
         <v>28</v>
@@ -31440,55 +31440,55 @@
         <v>44534.75</v>
       </c>
       <c r="F348" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G348" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H348">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I348">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J348" t="s">
         <v>53</v>
       </c>
       <c r="K348">
-        <v>3.25</v>
+        <v>2.05</v>
       </c>
       <c r="L348">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="M348">
-        <v>2.05</v>
+        <v>3.1</v>
       </c>
       <c r="N348">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="O348">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="P348">
-        <v>2.1</v>
+        <v>3.6</v>
       </c>
       <c r="Q348">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R348">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="S348">
         <v>1.8</v>
       </c>
       <c r="T348">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U348">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="V348">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="W348">
         <v>-1</v>
@@ -31497,7 +31497,7 @@
         <v>-1</v>
       </c>
       <c r="Y348">
-        <v>1.1</v>
+        <v>2.6</v>
       </c>
       <c r="Z348">
         <v>-1</v>
@@ -31506,7 +31506,7 @@
         <v>0.8</v>
       </c>
       <c r="AB348">
-        <v>0.825</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC348">
         <v>-1</v>
@@ -31517,7 +31517,7 @@
         <v>347</v>
       </c>
       <c r="B349">
-        <v>3899778</v>
+        <v>3899774</v>
       </c>
       <c r="C349" t="s">
         <v>28</v>
@@ -31529,76 +31529,76 @@
         <v>44534.75</v>
       </c>
       <c r="F349" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G349" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H349">
         <v>1</v>
       </c>
       <c r="I349">
+        <v>0</v>
+      </c>
+      <c r="J349" t="s">
+        <v>52</v>
+      </c>
+      <c r="K349">
         <v>4</v>
-      </c>
-      <c r="J349" t="s">
-        <v>53</v>
-      </c>
-      <c r="K349">
-        <v>2.05</v>
       </c>
       <c r="L349">
         <v>3.4</v>
       </c>
       <c r="M349">
-        <v>3.1</v>
+        <v>1.8</v>
       </c>
       <c r="N349">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O349">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P349">
-        <v>3.6</v>
+        <v>1.363</v>
       </c>
       <c r="Q349">
-        <v>-0.5</v>
+        <v>1.5</v>
       </c>
       <c r="R349">
-        <v>2</v>
+        <v>1.775</v>
       </c>
       <c r="S349">
+        <v>2.025</v>
+      </c>
+      <c r="T349">
+        <v>2.5</v>
+      </c>
+      <c r="U349">
         <v>1.8</v>
       </c>
-      <c r="T349">
-        <v>2.75</v>
-      </c>
-      <c r="U349">
-        <v>1.85</v>
-      </c>
       <c r="V349">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W349">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="X349">
         <v>-1</v>
       </c>
       <c r="Y349">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z349">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA349">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB349">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC349">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350" spans="1:29">
@@ -31606,7 +31606,7 @@
         <v>348</v>
       </c>
       <c r="B350">
-        <v>3899774</v>
+        <v>3898957</v>
       </c>
       <c r="C350" t="s">
         <v>28</v>
@@ -31618,76 +31618,76 @@
         <v>44534.75</v>
       </c>
       <c r="F350" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G350" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H350">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I350">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J350" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K350">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="L350">
+        <v>3.25</v>
+      </c>
+      <c r="M350">
+        <v>2.05</v>
+      </c>
+      <c r="N350">
+        <v>3.5</v>
+      </c>
+      <c r="O350">
         <v>3.4</v>
       </c>
-      <c r="M350">
+      <c r="P350">
+        <v>2.1</v>
+      </c>
+      <c r="Q350">
+        <v>0.25</v>
+      </c>
+      <c r="R350">
+        <v>2.05</v>
+      </c>
+      <c r="S350">
         <v>1.8</v>
       </c>
-      <c r="N350">
-        <v>9</v>
-      </c>
-      <c r="O350">
-        <v>4.75</v>
-      </c>
-      <c r="P350">
-        <v>1.363</v>
-      </c>
-      <c r="Q350">
-        <v>1.5</v>
-      </c>
-      <c r="R350">
-        <v>1.775</v>
-      </c>
-      <c r="S350">
+      <c r="T350">
+        <v>2.25</v>
+      </c>
+      <c r="U350">
+        <v>1.825</v>
+      </c>
+      <c r="V350">
         <v>2.025</v>
       </c>
-      <c r="T350">
-        <v>2.5</v>
-      </c>
-      <c r="U350">
-        <v>1.8</v>
-      </c>
-      <c r="V350">
-        <v>2</v>
-      </c>
       <c r="W350">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="X350">
         <v>-1</v>
       </c>
       <c r="Y350">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="Z350">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA350">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB350">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC350">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="351" spans="1:29">
@@ -31784,7 +31784,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>3899436</v>
+        <v>3899777</v>
       </c>
       <c r="C352" t="s">
         <v>28</v>
@@ -31796,76 +31796,76 @@
         <v>44535.75</v>
       </c>
       <c r="F352" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G352" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H352">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I352">
         <v>1</v>
       </c>
       <c r="J352" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K352">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="L352">
-        <v>4.5</v>
+        <v>3.1</v>
       </c>
       <c r="M352">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N352">
-        <v>1.444</v>
+        <v>2.75</v>
       </c>
       <c r="O352">
-        <v>4.75</v>
+        <v>2.75</v>
       </c>
       <c r="P352">
-        <v>6.5</v>
+        <v>2.7</v>
       </c>
       <c r="Q352">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="R352">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S352">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="T352">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="U352">
-        <v>1.975</v>
+        <v>1.875</v>
       </c>
       <c r="V352">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="W352">
-        <v>0.444</v>
+        <v>-1</v>
       </c>
       <c r="X352">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y352">
         <v>-1</v>
       </c>
       <c r="Z352">
-        <v>1.025</v>
+        <v>0</v>
       </c>
       <c r="AA352">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB352">
-        <v>0.9750000000000001</v>
+        <v>0</v>
       </c>
       <c r="AC352">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="353" spans="1:29">
@@ -31873,7 +31873,7 @@
         <v>351</v>
       </c>
       <c r="B353">
-        <v>3899777</v>
+        <v>3899436</v>
       </c>
       <c r="C353" t="s">
         <v>28</v>
@@ -31885,76 +31885,76 @@
         <v>44535.75</v>
       </c>
       <c r="F353" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G353" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H353">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I353">
         <v>1</v>
       </c>
       <c r="J353" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K353">
-        <v>2.25</v>
+        <v>1.4</v>
       </c>
       <c r="L353">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="M353">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N353">
+        <v>1.444</v>
+      </c>
+      <c r="O353">
+        <v>4.75</v>
+      </c>
+      <c r="P353">
+        <v>6.5</v>
+      </c>
+      <c r="Q353">
+        <v>-1.25</v>
+      </c>
+      <c r="R353">
+        <v>2.025</v>
+      </c>
+      <c r="S353">
+        <v>1.825</v>
+      </c>
+      <c r="T353">
         <v>2.75</v>
       </c>
-      <c r="O353">
-        <v>2.75</v>
-      </c>
-      <c r="P353">
-        <v>2.7</v>
-      </c>
-      <c r="Q353">
-        <v>0</v>
-      </c>
-      <c r="R353">
-        <v>1.9</v>
-      </c>
-      <c r="S353">
-        <v>1.9</v>
-      </c>
-      <c r="T353">
-        <v>2</v>
-      </c>
       <c r="U353">
+        <v>1.975</v>
+      </c>
+      <c r="V353">
         <v>1.875</v>
       </c>
-      <c r="V353">
-        <v>1.925</v>
-      </c>
       <c r="W353">
-        <v>-1</v>
+        <v>0.444</v>
       </c>
       <c r="X353">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y353">
         <v>-1</v>
       </c>
       <c r="Z353">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="AA353">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB353">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC353">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="354" spans="1:29">
@@ -51542,7 +51542,7 @@
         <v>572</v>
       </c>
       <c r="B574">
-        <v>4617486</v>
+        <v>4614399</v>
       </c>
       <c r="C574" t="s">
         <v>28</v>
@@ -51554,40 +51554,40 @@
         <v>44857.625</v>
       </c>
       <c r="F574" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G574" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H574">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I574">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J574" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K574">
-        <v>2.1</v>
+        <v>5.25</v>
       </c>
       <c r="L574">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M574">
-        <v>3.25</v>
+        <v>1.615</v>
       </c>
       <c r="N574">
-        <v>1.909</v>
+        <v>5</v>
       </c>
       <c r="O574">
         <v>3.8</v>
       </c>
       <c r="P574">
-        <v>3.75</v>
+        <v>1.7</v>
       </c>
       <c r="Q574">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R574">
         <v>1.925</v>
@@ -51596,34 +51596,34 @@
         <v>1.925</v>
       </c>
       <c r="T574">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U574">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="V574">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W574">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X574">
         <v>-1</v>
       </c>
       <c r="Y574">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="Z574">
+        <v>-1</v>
+      </c>
+      <c r="AA574">
         <v>0.925</v>
       </c>
-      <c r="AA574">
-        <v>-1</v>
-      </c>
       <c r="AB574">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AC574">
-        <v>1</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="575" spans="1:29">
@@ -51631,7 +51631,7 @@
         <v>573</v>
       </c>
       <c r="B575">
-        <v>4614399</v>
+        <v>4617486</v>
       </c>
       <c r="C575" t="s">
         <v>28</v>
@@ -51643,40 +51643,40 @@
         <v>44857.625</v>
       </c>
       <c r="F575" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G575" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H575">
+        <v>2</v>
+      </c>
+      <c r="I575">
         <v>0</v>
       </c>
-      <c r="I575">
-        <v>2</v>
-      </c>
       <c r="J575" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K575">
-        <v>5.25</v>
+        <v>2.1</v>
       </c>
       <c r="L575">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M575">
-        <v>1.615</v>
+        <v>3.25</v>
       </c>
       <c r="N575">
-        <v>5</v>
+        <v>1.909</v>
       </c>
       <c r="O575">
         <v>3.8</v>
       </c>
       <c r="P575">
-        <v>1.7</v>
+        <v>3.75</v>
       </c>
       <c r="Q575">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R575">
         <v>1.925</v>
@@ -51685,34 +51685,34 @@
         <v>1.925</v>
       </c>
       <c r="T575">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U575">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V575">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W575">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X575">
         <v>-1</v>
       </c>
       <c r="Y575">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Z575">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA575">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AB575">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC575">
-        <v>0.4125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="576" spans="1:29">
@@ -52699,7 +52699,7 @@
         <v>585</v>
       </c>
       <c r="B587">
-        <v>4617491</v>
+        <v>4614405</v>
       </c>
       <c r="C587" t="s">
         <v>28</v>
@@ -52711,73 +52711,73 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F587" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G587" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H587">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I587">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J587" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K587">
-        <v>2.7</v>
+        <v>1.75</v>
       </c>
       <c r="L587">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M587">
-        <v>2.45</v>
+        <v>4.333</v>
       </c>
       <c r="N587">
-        <v>2.7</v>
+        <v>1.833</v>
       </c>
       <c r="O587">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P587">
-        <v>2.6</v>
+        <v>4.5</v>
       </c>
       <c r="Q587">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R587">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="S587">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="T587">
         <v>2.5</v>
       </c>
       <c r="U587">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="V587">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W587">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="X587">
         <v>-1</v>
       </c>
       <c r="Y587">
-        <v>1.6</v>
+        <v>-1</v>
       </c>
       <c r="Z587">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA587">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB587">
-        <v>0.8999999999999999</v>
+        <v>0.875</v>
       </c>
       <c r="AC587">
         <v>-1</v>
@@ -52788,7 +52788,7 @@
         <v>586</v>
       </c>
       <c r="B588">
-        <v>4617747</v>
+        <v>4617491</v>
       </c>
       <c r="C588" t="s">
         <v>28</v>
@@ -52800,76 +52800,76 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F588" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G588" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H588">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I588">
+        <v>4</v>
+      </c>
+      <c r="J588" t="s">
+        <v>53</v>
+      </c>
+      <c r="K588">
+        <v>2.7</v>
+      </c>
+      <c r="L588">
+        <v>3.3</v>
+      </c>
+      <c r="M588">
+        <v>2.45</v>
+      </c>
+      <c r="N588">
+        <v>2.7</v>
+      </c>
+      <c r="O588">
+        <v>3.4</v>
+      </c>
+      <c r="P588">
+        <v>2.6</v>
+      </c>
+      <c r="Q588">
         <v>0</v>
       </c>
-      <c r="J588" t="s">
-        <v>52</v>
-      </c>
-      <c r="K588">
-        <v>2.4</v>
-      </c>
-      <c r="L588">
-        <v>3.1</v>
-      </c>
-      <c r="M588">
-        <v>2.9</v>
-      </c>
-      <c r="N588">
-        <v>2.15</v>
-      </c>
-      <c r="O588">
-        <v>3.25</v>
-      </c>
-      <c r="P588">
-        <v>3.5</v>
-      </c>
-      <c r="Q588">
-        <v>-0.25</v>
-      </c>
       <c r="R588">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="S588">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T588">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U588">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="V588">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="W588">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X588">
         <v>-1</v>
       </c>
       <c r="Y588">
-        <v>-1</v>
+        <v>1.6</v>
       </c>
       <c r="Z588">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA588">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB588">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC588">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="589" spans="1:29">
@@ -52877,7 +52877,7 @@
         <v>587</v>
       </c>
       <c r="B589">
-        <v>4614405</v>
+        <v>4617747</v>
       </c>
       <c r="C589" t="s">
         <v>28</v>
@@ -52889,13 +52889,13 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F589" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G589" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H589">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I589">
         <v>0</v>
@@ -52904,43 +52904,43 @@
         <v>52</v>
       </c>
       <c r="K589">
-        <v>1.75</v>
+        <v>2.4</v>
       </c>
       <c r="L589">
+        <v>3.1</v>
+      </c>
+      <c r="M589">
+        <v>2.9</v>
+      </c>
+      <c r="N589">
+        <v>2.15</v>
+      </c>
+      <c r="O589">
+        <v>3.25</v>
+      </c>
+      <c r="P589">
         <v>3.5</v>
       </c>
-      <c r="M589">
-        <v>4.333</v>
-      </c>
-      <c r="N589">
-        <v>1.833</v>
-      </c>
-      <c r="O589">
-        <v>3.5</v>
-      </c>
-      <c r="P589">
-        <v>4.5</v>
-      </c>
       <c r="Q589">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R589">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="S589">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T589">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U589">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V589">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W589">
-        <v>0.833</v>
+        <v>1.15</v>
       </c>
       <c r="X589">
         <v>-1</v>
@@ -52949,16 +52949,16 @@
         <v>-1</v>
       </c>
       <c r="Z589">
-        <v>0.8</v>
+        <v>0.825</v>
       </c>
       <c r="AA589">
         <v>-1</v>
       </c>
       <c r="AB589">
-        <v>0.875</v>
+        <v>0</v>
       </c>
       <c r="AC589">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="590" spans="1:29">
@@ -55547,7 +55547,7 @@
         <v>617</v>
       </c>
       <c r="B619">
-        <v>6073146</v>
+        <v>6078853</v>
       </c>
       <c r="C619" t="s">
         <v>28</v>
@@ -55559,73 +55559,73 @@
         <v>44967.875</v>
       </c>
       <c r="F619" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G619" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H619">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I619">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J619" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K619">
-        <v>2.7</v>
+        <v>2.625</v>
       </c>
       <c r="L619">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="M619">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="N619">
-        <v>3.3</v>
+        <v>1.909</v>
       </c>
       <c r="O619">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="P619">
-        <v>2.25</v>
+        <v>4.2</v>
       </c>
       <c r="Q619">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R619">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="S619">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="T619">
         <v>2.5</v>
       </c>
       <c r="U619">
+        <v>1.925</v>
+      </c>
+      <c r="V619">
         <v>1.875</v>
       </c>
-      <c r="V619">
-        <v>1.925</v>
-      </c>
       <c r="W619">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X619">
         <v>-1</v>
       </c>
       <c r="Y619">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Z619">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA619">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB619">
-        <v>0.875</v>
+        <v>0.925</v>
       </c>
       <c r="AC619">
         <v>-1</v>
@@ -55636,7 +55636,7 @@
         <v>618</v>
       </c>
       <c r="B620">
-        <v>6078853</v>
+        <v>6073146</v>
       </c>
       <c r="C620" t="s">
         <v>28</v>
@@ -55648,73 +55648,73 @@
         <v>44967.875</v>
       </c>
       <c r="F620" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G620" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H620">
+        <v>1</v>
+      </c>
+      <c r="I620">
         <v>3</v>
       </c>
-      <c r="I620">
-        <v>2</v>
-      </c>
       <c r="J620" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K620">
-        <v>2.625</v>
+        <v>2.7</v>
       </c>
       <c r="L620">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="M620">
-        <v>2.4</v>
+        <v>2.45</v>
       </c>
       <c r="N620">
-        <v>1.909</v>
+        <v>3.3</v>
       </c>
       <c r="O620">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="P620">
-        <v>4.2</v>
+        <v>2.25</v>
       </c>
       <c r="Q620">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R620">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="S620">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="T620">
         <v>2.5</v>
       </c>
       <c r="U620">
+        <v>1.875</v>
+      </c>
+      <c r="V620">
         <v>1.925</v>
       </c>
-      <c r="V620">
-        <v>1.875</v>
-      </c>
       <c r="W620">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X620">
         <v>-1</v>
       </c>
       <c r="Y620">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="Z620">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA620">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB620">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AC620">
         <v>-1</v>
@@ -57238,7 +57238,7 @@
         <v>636</v>
       </c>
       <c r="B638">
-        <v>6078935</v>
+        <v>6073148</v>
       </c>
       <c r="C638" t="s">
         <v>28</v>
@@ -57250,73 +57250,73 @@
         <v>44984.85416666666</v>
       </c>
       <c r="F638" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G638" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H638">
+        <v>2</v>
+      </c>
+      <c r="I638">
+        <v>2</v>
+      </c>
+      <c r="J638" t="s">
+        <v>51</v>
+      </c>
+      <c r="K638">
+        <v>3.2</v>
+      </c>
+      <c r="L638">
+        <v>3.4</v>
+      </c>
+      <c r="M638">
+        <v>2.2</v>
+      </c>
+      <c r="N638">
+        <v>2.4</v>
+      </c>
+      <c r="O638">
+        <v>3.25</v>
+      </c>
+      <c r="P638">
         <v>3</v>
       </c>
-      <c r="I638">
-        <v>1</v>
-      </c>
-      <c r="J638" t="s">
-        <v>52</v>
-      </c>
-      <c r="K638">
-        <v>1.95</v>
-      </c>
-      <c r="L638">
-        <v>3.5</v>
-      </c>
-      <c r="M638">
-        <v>3.8</v>
-      </c>
-      <c r="N638">
+      <c r="Q638">
+        <v>-0.25</v>
+      </c>
+      <c r="R638">
+        <v>2.05</v>
+      </c>
+      <c r="S638">
         <v>1.75</v>
       </c>
-      <c r="O638">
-        <v>4</v>
-      </c>
-      <c r="P638">
-        <v>4.5</v>
-      </c>
-      <c r="Q638">
-        <v>-0.75</v>
-      </c>
-      <c r="R638">
-        <v>1.95</v>
-      </c>
-      <c r="S638">
-        <v>1.85</v>
-      </c>
       <c r="T638">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U638">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="V638">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W638">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="X638">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="Y638">
         <v>-1</v>
       </c>
       <c r="Z638">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="AA638">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AB638">
-        <v>0.925</v>
+        <v>0.8</v>
       </c>
       <c r="AC638">
         <v>-1</v>
@@ -57327,7 +57327,7 @@
         <v>637</v>
       </c>
       <c r="B639">
-        <v>6073148</v>
+        <v>6078935</v>
       </c>
       <c r="C639" t="s">
         <v>28</v>
@@ -57339,73 +57339,73 @@
         <v>44984.85416666666</v>
       </c>
       <c r="F639" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G639" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H639">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I639">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J639" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K639">
-        <v>3.2</v>
+        <v>1.95</v>
       </c>
       <c r="L639">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M639">
-        <v>2.2</v>
+        <v>3.8</v>
       </c>
       <c r="N639">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="O639">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="P639">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="Q639">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R639">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S639">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
       <c r="T639">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U639">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V639">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W639">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="X639">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="Y639">
         <v>-1</v>
       </c>
       <c r="Z639">
-        <v>-0.5</v>
+        <v>0.95</v>
       </c>
       <c r="AA639">
-        <v>0.375</v>
+        <v>-1</v>
       </c>
       <c r="AB639">
-        <v>0.8</v>
+        <v>0.925</v>
       </c>
       <c r="AC639">
         <v>-1</v>
@@ -61866,7 +61866,7 @@
         <v>688</v>
       </c>
       <c r="B690">
-        <v>6078876</v>
+        <v>6532619</v>
       </c>
       <c r="C690" t="s">
         <v>28</v>
@@ -61878,58 +61878,58 @@
         <v>45056.79166666666</v>
       </c>
       <c r="F690" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G690" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H690">
+        <v>2</v>
+      </c>
+      <c r="I690">
         <v>1</v>
-      </c>
-      <c r="I690">
-        <v>0</v>
       </c>
       <c r="J690" t="s">
         <v>52</v>
       </c>
       <c r="K690">
-        <v>1.85</v>
+        <v>2.55</v>
       </c>
       <c r="L690">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M690">
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
       <c r="N690">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="O690">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="P690">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="Q690">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R690">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="S690">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="T690">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U690">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V690">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="W690">
-        <v>0.909</v>
+        <v>1.45</v>
       </c>
       <c r="X690">
         <v>-1</v>
@@ -61938,16 +61938,16 @@
         <v>-1</v>
       </c>
       <c r="Z690">
-        <v>0.8500000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="AA690">
         <v>-1</v>
       </c>
       <c r="AB690">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC690">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="691" spans="1:29">
@@ -61955,7 +61955,7 @@
         <v>689</v>
       </c>
       <c r="B691">
-        <v>6532619</v>
+        <v>6078876</v>
       </c>
       <c r="C691" t="s">
         <v>28</v>
@@ -61967,58 +61967,58 @@
         <v>45056.79166666666</v>
       </c>
       <c r="F691" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G691" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H691">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I691">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J691" t="s">
         <v>52</v>
       </c>
       <c r="K691">
-        <v>2.55</v>
+        <v>1.85</v>
       </c>
       <c r="L691">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M691">
+        <v>3.75</v>
+      </c>
+      <c r="N691">
+        <v>1.909</v>
+      </c>
+      <c r="O691">
+        <v>3.6</v>
+      </c>
+      <c r="P691">
+        <v>4.2</v>
+      </c>
+      <c r="Q691">
+        <v>-0.5</v>
+      </c>
+      <c r="R691">
+        <v>1.85</v>
+      </c>
+      <c r="S691">
+        <v>1.95</v>
+      </c>
+      <c r="T691">
         <v>2.5</v>
       </c>
-      <c r="N691">
-        <v>2.45</v>
-      </c>
-      <c r="O691">
-        <v>3.3</v>
-      </c>
-      <c r="P691">
-        <v>3</v>
-      </c>
-      <c r="Q691">
-        <v>-0.25</v>
-      </c>
-      <c r="R691">
-        <v>2.05</v>
-      </c>
-      <c r="S691">
-        <v>1.75</v>
-      </c>
-      <c r="T691">
-        <v>2.25</v>
-      </c>
       <c r="U691">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="V691">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W691">
-        <v>1.45</v>
+        <v>0.909</v>
       </c>
       <c r="X691">
         <v>-1</v>
@@ -62027,16 +62027,16 @@
         <v>-1</v>
       </c>
       <c r="Z691">
-        <v>1.05</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA691">
         <v>-1</v>
       </c>
       <c r="AB691">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC691">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="692" spans="1:29">
@@ -69164,7 +69164,7 @@
         <v>770</v>
       </c>
       <c r="B772">
-        <v>7082624</v>
+        <v>7157967</v>
       </c>
       <c r="C772" t="s">
         <v>28</v>
@@ -69176,40 +69176,40 @@
         <v>45183.79166666666</v>
       </c>
       <c r="F772" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G772" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="H772">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I772">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J772" t="s">
         <v>51</v>
       </c>
       <c r="K772">
-        <v>1.333</v>
+        <v>2.375</v>
       </c>
       <c r="L772">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="M772">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N772">
-        <v>1.45</v>
+        <v>2.75</v>
       </c>
       <c r="O772">
-        <v>4.75</v>
+        <v>3.2</v>
       </c>
       <c r="P772">
-        <v>7</v>
+        <v>2.7</v>
       </c>
       <c r="Q772">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="R772">
         <v>1.925</v>
@@ -69218,34 +69218,34 @@
         <v>1.875</v>
       </c>
       <c r="T772">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U772">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V772">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="W772">
         <v>-1</v>
       </c>
       <c r="X772">
-        <v>3.75</v>
+        <v>2.2</v>
       </c>
       <c r="Y772">
         <v>-1</v>
       </c>
       <c r="Z772">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA772">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
       <c r="AB772">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC772">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="773" spans="1:29">
@@ -69253,7 +69253,7 @@
         <v>771</v>
       </c>
       <c r="B773">
-        <v>7157967</v>
+        <v>7082624</v>
       </c>
       <c r="C773" t="s">
         <v>28</v>
@@ -69265,40 +69265,40 @@
         <v>45183.79166666666</v>
       </c>
       <c r="F773" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G773" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="H773">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I773">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J773" t="s">
         <v>51</v>
       </c>
       <c r="K773">
-        <v>2.375</v>
+        <v>1.333</v>
       </c>
       <c r="L773">
-        <v>3.2</v>
+        <v>5</v>
       </c>
       <c r="M773">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N773">
-        <v>2.75</v>
+        <v>1.45</v>
       </c>
       <c r="O773">
-        <v>3.2</v>
+        <v>4.75</v>
       </c>
       <c r="P773">
-        <v>2.7</v>
+        <v>7</v>
       </c>
       <c r="Q773">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="R773">
         <v>1.925</v>
@@ -69307,34 +69307,34 @@
         <v>1.875</v>
       </c>
       <c r="T773">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U773">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="V773">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W773">
         <v>-1</v>
       </c>
       <c r="X773">
-        <v>2.2</v>
+        <v>3.75</v>
       </c>
       <c r="Y773">
         <v>-1</v>
       </c>
       <c r="Z773">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA773">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
       <c r="AB773">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC773">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="774" spans="1:29">
@@ -73080,7 +73080,7 @@
         <v>814</v>
       </c>
       <c r="B816">
-        <v>6078266</v>
+        <v>6078265</v>
       </c>
       <c r="C816" t="s">
         <v>28</v>
@@ -73092,76 +73092,76 @@
         <v>45262.75</v>
       </c>
       <c r="F816" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G816" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H816">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I816">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J816" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K816">
-        <v>1.533</v>
+        <v>1.666</v>
       </c>
       <c r="L816">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M816">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N816">
-        <v>1.363</v>
+        <v>2.25</v>
       </c>
       <c r="O816">
-        <v>4.75</v>
+        <v>3.3</v>
       </c>
       <c r="P816">
-        <v>7.5</v>
+        <v>3.3</v>
       </c>
       <c r="Q816">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R816">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="S816">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="T816">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U816">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V816">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W816">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="X816">
         <v>-1</v>
       </c>
       <c r="Y816">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z816">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA816">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB816">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC816">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="817" spans="1:29">
@@ -73169,7 +73169,7 @@
         <v>815</v>
       </c>
       <c r="B817">
-        <v>6077498</v>
+        <v>6078266</v>
       </c>
       <c r="C817" t="s">
         <v>28</v>
@@ -73181,73 +73181,73 @@
         <v>45262.75</v>
       </c>
       <c r="F817" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G817" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H817">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I817">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J817" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K817">
-        <v>1.65</v>
+        <v>1.533</v>
       </c>
       <c r="L817">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="M817">
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="N817">
-        <v>1.909</v>
+        <v>1.363</v>
       </c>
       <c r="O817">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P817">
-        <v>4.2</v>
+        <v>7.5</v>
       </c>
       <c r="Q817">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="R817">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="S817">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="T817">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U817">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V817">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W817">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="X817">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y817">
         <v>-1</v>
       </c>
       <c r="Z817">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA817">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB817">
-        <v>1.025</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC817">
         <v>-1</v>
@@ -73258,7 +73258,7 @@
         <v>816</v>
       </c>
       <c r="B818">
-        <v>6078265</v>
+        <v>6077498</v>
       </c>
       <c r="C818" t="s">
         <v>28</v>
@@ -73270,76 +73270,76 @@
         <v>45262.75</v>
       </c>
       <c r="F818" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G818" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H818">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I818">
         <v>2</v>
       </c>
       <c r="J818" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K818">
-        <v>1.666</v>
+        <v>1.65</v>
       </c>
       <c r="L818">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="M818">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="N818">
-        <v>2.25</v>
+        <v>1.909</v>
       </c>
       <c r="O818">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="P818">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="Q818">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R818">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="S818">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="T818">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U818">
-        <v>1.8</v>
+        <v>2.025</v>
       </c>
       <c r="V818">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W818">
         <v>-1</v>
       </c>
       <c r="X818">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y818">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z818">
         <v>-1</v>
       </c>
       <c r="AA818">
-        <v>0.8500000000000001</v>
+        <v>1</v>
       </c>
       <c r="AB818">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC818">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="819" spans="1:29">
@@ -73703,7 +73703,7 @@
         <v>821</v>
       </c>
       <c r="B823">
-        <v>6078997</v>
+        <v>6143704</v>
       </c>
       <c r="C823" t="s">
         <v>28</v>
@@ -73715,67 +73715,67 @@
         <v>45268.75</v>
       </c>
       <c r="F823" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G823" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H823">
+        <v>0</v>
+      </c>
+      <c r="I823">
         <v>1</v>
       </c>
-      <c r="I823">
-        <v>0</v>
-      </c>
       <c r="J823" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K823">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
       <c r="L823">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="M823">
-        <v>1.909</v>
+        <v>1.4</v>
       </c>
       <c r="N823">
-        <v>2.7</v>
+        <v>12</v>
       </c>
       <c r="O823">
-        <v>3.6</v>
+        <v>8.5</v>
       </c>
       <c r="P823">
-        <v>2.45</v>
+        <v>1.166</v>
       </c>
       <c r="Q823">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R823">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S823">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T823">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U823">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="V823">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W823">
-        <v>1.7</v>
+        <v>-1</v>
       </c>
       <c r="X823">
         <v>-1</v>
       </c>
       <c r="Y823">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="Z823">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="AA823">
         <v>-1</v>
@@ -73784,7 +73784,7 @@
         <v>-1</v>
       </c>
       <c r="AC823">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="824" spans="1:29">
@@ -73792,7 +73792,7 @@
         <v>822</v>
       </c>
       <c r="B824">
-        <v>6143704</v>
+        <v>6078997</v>
       </c>
       <c r="C824" t="s">
         <v>28</v>
@@ -73804,67 +73804,67 @@
         <v>45268.75</v>
       </c>
       <c r="F824" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G824" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H824">
+        <v>1</v>
+      </c>
+      <c r="I824">
         <v>0</v>
       </c>
-      <c r="I824">
-        <v>1</v>
-      </c>
       <c r="J824" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K824">
-        <v>6.5</v>
+        <v>3.8</v>
       </c>
       <c r="L824">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="M824">
-        <v>1.4</v>
+        <v>1.909</v>
       </c>
       <c r="N824">
-        <v>12</v>
+        <v>2.7</v>
       </c>
       <c r="O824">
-        <v>8.5</v>
+        <v>3.6</v>
       </c>
       <c r="P824">
-        <v>1.166</v>
+        <v>2.45</v>
       </c>
       <c r="Q824">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R824">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S824">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T824">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U824">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V824">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W824">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="X824">
         <v>-1</v>
       </c>
       <c r="Y824">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z824">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA824">
         <v>-1</v>
@@ -73873,7 +73873,7 @@
         <v>-1</v>
       </c>
       <c r="AC824">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="825" spans="1:29">
@@ -73970,7 +73970,7 @@
         <v>824</v>
       </c>
       <c r="B826">
-        <v>6078269</v>
+        <v>6078998</v>
       </c>
       <c r="C826" t="s">
         <v>28</v>
@@ -73982,73 +73982,73 @@
         <v>45269.75</v>
       </c>
       <c r="F826" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G826" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H826">
+        <v>2</v>
+      </c>
+      <c r="I826">
         <v>3</v>
       </c>
-      <c r="I826">
-        <v>1</v>
-      </c>
       <c r="J826" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K826">
+        <v>1.909</v>
+      </c>
+      <c r="L826">
+        <v>3.6</v>
+      </c>
+      <c r="M826">
+        <v>3.8</v>
+      </c>
+      <c r="N826">
+        <v>2.15</v>
+      </c>
+      <c r="O826">
+        <v>3.75</v>
+      </c>
+      <c r="P826">
+        <v>3.1</v>
+      </c>
+      <c r="Q826">
+        <v>-0.25</v>
+      </c>
+      <c r="R826">
         <v>1.85</v>
       </c>
-      <c r="L826">
-        <v>3.4</v>
-      </c>
-      <c r="M826">
-        <v>4.333</v>
-      </c>
-      <c r="N826">
-        <v>1.8</v>
-      </c>
-      <c r="O826">
-        <v>3.6</v>
-      </c>
-      <c r="P826">
-        <v>4.5</v>
-      </c>
-      <c r="Q826">
-        <v>-0.75</v>
-      </c>
-      <c r="R826">
-        <v>1.925</v>
-      </c>
       <c r="S826">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T826">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U826">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V826">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W826">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="X826">
         <v>-1</v>
       </c>
       <c r="Y826">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="Z826">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA826">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB826">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC826">
         <v>-1</v>
@@ -74059,7 +74059,7 @@
         <v>825</v>
       </c>
       <c r="B827">
-        <v>6078998</v>
+        <v>6077499</v>
       </c>
       <c r="C827" t="s">
         <v>28</v>
@@ -74071,76 +74071,76 @@
         <v>45269.75</v>
       </c>
       <c r="F827" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G827" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="H827">
         <v>2</v>
       </c>
       <c r="I827">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J827" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K827">
-        <v>1.909</v>
+        <v>2.1</v>
       </c>
       <c r="L827">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M827">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N827">
-        <v>2.15</v>
+        <v>2.9</v>
       </c>
       <c r="O827">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P827">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="Q827">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R827">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="S827">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="T827">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U827">
         <v>1.85</v>
       </c>
       <c r="V827">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W827">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="X827">
         <v>-1</v>
       </c>
       <c r="Y827">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z827">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA827">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB827">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC827">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="828" spans="1:29">
@@ -74148,7 +74148,7 @@
         <v>826</v>
       </c>
       <c r="B828">
-        <v>6077499</v>
+        <v>6077768</v>
       </c>
       <c r="C828" t="s">
         <v>28</v>
@@ -74160,76 +74160,76 @@
         <v>45269.75</v>
       </c>
       <c r="F828" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G828" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H828">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I828">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J828" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K828">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="L828">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M828">
         <v>3.4</v>
       </c>
       <c r="N828">
-        <v>2.9</v>
+        <v>2.05</v>
       </c>
       <c r="O828">
+        <v>3.6</v>
+      </c>
+      <c r="P828">
         <v>3.4</v>
       </c>
-      <c r="P828">
-        <v>2.4</v>
-      </c>
       <c r="Q828">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R828">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="S828">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="T828">
         <v>2.75</v>
       </c>
       <c r="U828">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V828">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W828">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="X828">
         <v>-1</v>
       </c>
       <c r="Y828">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z828">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA828">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB828">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AC828">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="829" spans="1:29">
@@ -74237,7 +74237,7 @@
         <v>827</v>
       </c>
       <c r="B829">
-        <v>6077768</v>
+        <v>6078269</v>
       </c>
       <c r="C829" t="s">
         <v>28</v>
@@ -74249,76 +74249,76 @@
         <v>45269.75</v>
       </c>
       <c r="F829" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G829" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H829">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I829">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J829" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K829">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="L829">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M829">
-        <v>3.4</v>
+        <v>4.333</v>
       </c>
       <c r="N829">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="O829">
         <v>3.6</v>
       </c>
       <c r="P829">
-        <v>3.4</v>
+        <v>4.5</v>
       </c>
       <c r="Q829">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R829">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S829">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="T829">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U829">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V829">
         <v>1.825</v>
       </c>
       <c r="W829">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X829">
         <v>-1</v>
       </c>
       <c r="Y829">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z829">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA829">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB829">
-        <v>0.4875</v>
+        <v>1.025</v>
       </c>
       <c r="AC829">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="830" spans="1:29">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-28 às 11-34
</commit_message>
<xml_diff>
--- a/Chile Primera Division/Chile Primera Division.xlsx
+++ b/Chile Primera Division/Chile Primera Division.xlsx
@@ -6597,7 +6597,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>3200931</v>
+        <v>3201281</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6609,76 +6609,76 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F69" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G69" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K69">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="L69">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="M69">
-        <v>3.3</v>
+        <v>2.375</v>
       </c>
       <c r="N69">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="O69">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="P69">
-        <v>3.6</v>
+        <v>2.15</v>
       </c>
       <c r="Q69">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R69">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S69">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="T69">
         <v>2.25</v>
       </c>
       <c r="U69">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="V69">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W69">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="X69">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y69">
         <v>-1</v>
       </c>
       <c r="Z69">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AA69">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB69">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC69">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -6686,7 +6686,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>3201269</v>
+        <v>3201280</v>
       </c>
       <c r="C70" t="s">
         <v>28</v>
@@ -6698,10 +6698,10 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F70" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G70" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -6713,31 +6713,31 @@
         <v>51</v>
       </c>
       <c r="K70">
-        <v>2</v>
+        <v>1.833</v>
       </c>
       <c r="L70">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="M70">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N70">
-        <v>2.3</v>
+        <v>2</v>
       </c>
       <c r="O70">
         <v>3.5</v>
       </c>
       <c r="P70">
-        <v>2.875</v>
+        <v>3.5</v>
       </c>
       <c r="Q70">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R70">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
       <c r="S70">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="T70">
         <v>2.5</v>
@@ -6758,10 +6758,10 @@
         <v>-1</v>
       </c>
       <c r="Z70">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AA70">
-        <v>-0</v>
+        <v>0.475</v>
       </c>
       <c r="AB70">
         <v>-1</v>
@@ -6775,7 +6775,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>3201280</v>
+        <v>3200931</v>
       </c>
       <c r="C71" t="s">
         <v>28</v>
@@ -6787,61 +6787,61 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F71" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G71" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J71" t="s">
         <v>51</v>
       </c>
       <c r="K71">
-        <v>1.833</v>
+        <v>2.2</v>
       </c>
       <c r="L71">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="M71">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="N71">
         <v>2</v>
       </c>
       <c r="O71">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P71">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="Q71">
         <v>-0.25</v>
       </c>
       <c r="R71">
+        <v>1.8</v>
+      </c>
+      <c r="S71">
+        <v>2</v>
+      </c>
+      <c r="T71">
+        <v>2.25</v>
+      </c>
+      <c r="U71">
         <v>1.85</v>
       </c>
-      <c r="S71">
+      <c r="V71">
         <v>1.95</v>
       </c>
-      <c r="T71">
-        <v>2.5</v>
-      </c>
-      <c r="U71">
-        <v>1.825</v>
-      </c>
-      <c r="V71">
-        <v>1.975</v>
-      </c>
       <c r="W71">
         <v>-1</v>
       </c>
       <c r="X71">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="Y71">
         <v>-1</v>
@@ -6850,13 +6850,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA71">
-        <v>0.475</v>
+        <v>0.5</v>
       </c>
       <c r="AB71">
         <v>-1</v>
       </c>
       <c r="AC71">
-        <v>0.9750000000000001</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="72" spans="1:29">
@@ -6864,7 +6864,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>3201281</v>
+        <v>3201269</v>
       </c>
       <c r="C72" t="s">
         <v>28</v>
@@ -6876,76 +6876,76 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F72" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G72" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H72">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72" t="s">
+        <v>51</v>
+      </c>
+      <c r="K72">
+        <v>2</v>
+      </c>
+      <c r="L72">
+        <v>3.5</v>
+      </c>
+      <c r="M72">
+        <v>3.6</v>
+      </c>
+      <c r="N72">
+        <v>2.3</v>
+      </c>
+      <c r="O72">
+        <v>3.5</v>
+      </c>
+      <c r="P72">
+        <v>2.875</v>
+      </c>
+      <c r="Q72">
         <v>0</v>
       </c>
-      <c r="J72" t="s">
-        <v>52</v>
-      </c>
-      <c r="K72">
-        <v>3</v>
-      </c>
-      <c r="L72">
-        <v>3.2</v>
-      </c>
-      <c r="M72">
-        <v>2.375</v>
-      </c>
-      <c r="N72">
-        <v>3.5</v>
-      </c>
-      <c r="O72">
-        <v>3.2</v>
-      </c>
-      <c r="P72">
-        <v>2.15</v>
-      </c>
-      <c r="Q72">
-        <v>0.25</v>
-      </c>
       <c r="R72">
-        <v>1.925</v>
+        <v>1.75</v>
       </c>
       <c r="S72">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="T72">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U72">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="V72">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W72">
+        <v>-1</v>
+      </c>
+      <c r="X72">
         <v>2.5</v>
       </c>
-      <c r="X72">
-        <v>-1</v>
-      </c>
       <c r="Y72">
         <v>-1</v>
       </c>
       <c r="Z72">
-        <v>0.925</v>
+        <v>0</v>
       </c>
       <c r="AA72">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB72">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC72">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:29">
@@ -7042,7 +7042,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>3234974</v>
+        <v>3234177</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7054,73 +7054,73 @@
         <v>44240.77083333334</v>
       </c>
       <c r="F74" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G74" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
         <v>3</v>
       </c>
-      <c r="I74">
+      <c r="J74" t="s">
+        <v>53</v>
+      </c>
+      <c r="K74">
+        <v>1.85</v>
+      </c>
+      <c r="L74">
+        <v>3.6</v>
+      </c>
+      <c r="M74">
+        <v>4</v>
+      </c>
+      <c r="N74">
+        <v>1.95</v>
+      </c>
+      <c r="O74">
+        <v>3.5</v>
+      </c>
+      <c r="P74">
+        <v>4</v>
+      </c>
+      <c r="Q74">
+        <v>-0.5</v>
+      </c>
+      <c r="R74">
+        <v>1.925</v>
+      </c>
+      <c r="S74">
+        <v>1.875</v>
+      </c>
+      <c r="T74">
+        <v>3</v>
+      </c>
+      <c r="U74">
+        <v>2</v>
+      </c>
+      <c r="V74">
+        <v>1.8</v>
+      </c>
+      <c r="W74">
+        <v>-1</v>
+      </c>
+      <c r="X74">
+        <v>-1</v>
+      </c>
+      <c r="Y74">
+        <v>3</v>
+      </c>
+      <c r="Z74">
+        <v>-1</v>
+      </c>
+      <c r="AA74">
+        <v>0.875</v>
+      </c>
+      <c r="AB74">
         <v>1</v>
-      </c>
-      <c r="J74" t="s">
-        <v>52</v>
-      </c>
-      <c r="K74">
-        <v>1.75</v>
-      </c>
-      <c r="L74">
-        <v>3.4</v>
-      </c>
-      <c r="M74">
-        <v>5</v>
-      </c>
-      <c r="N74">
-        <v>1.6</v>
-      </c>
-      <c r="O74">
-        <v>3.6</v>
-      </c>
-      <c r="P74">
-        <v>6</v>
-      </c>
-      <c r="Q74">
-        <v>-0.75</v>
-      </c>
-      <c r="R74">
-        <v>1.8</v>
-      </c>
-      <c r="S74">
-        <v>2</v>
-      </c>
-      <c r="T74">
-        <v>2.75</v>
-      </c>
-      <c r="U74">
-        <v>1.8</v>
-      </c>
-      <c r="V74">
-        <v>2</v>
-      </c>
-      <c r="W74">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="X74">
-        <v>-1</v>
-      </c>
-      <c r="Y74">
-        <v>-1</v>
-      </c>
-      <c r="Z74">
-        <v>0.8</v>
-      </c>
-      <c r="AA74">
-        <v>-1</v>
-      </c>
-      <c r="AB74">
-        <v>0.8</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -7131,7 +7131,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>3234177</v>
+        <v>3234974</v>
       </c>
       <c r="C75" t="s">
         <v>28</v>
@@ -7143,73 +7143,73 @@
         <v>44240.77083333334</v>
       </c>
       <c r="F75" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G75" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J75" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K75">
-        <v>1.85</v>
+        <v>1.75</v>
       </c>
       <c r="L75">
+        <v>3.4</v>
+      </c>
+      <c r="M75">
+        <v>5</v>
+      </c>
+      <c r="N75">
+        <v>1.6</v>
+      </c>
+      <c r="O75">
         <v>3.6</v>
       </c>
-      <c r="M75">
-        <v>4</v>
-      </c>
-      <c r="N75">
-        <v>1.95</v>
-      </c>
-      <c r="O75">
-        <v>3.5</v>
-      </c>
       <c r="P75">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q75">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R75">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S75">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="T75">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U75">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="V75">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="W75">
-        <v>-1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="X75">
         <v>-1</v>
       </c>
       <c r="Y75">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z75">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA75">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB75">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AC75">
         <v>-1</v>
@@ -31250,7 +31250,7 @@
         <v>344</v>
       </c>
       <c r="B346">
-        <v>4365259</v>
+        <v>3898955</v>
       </c>
       <c r="C346" t="s">
         <v>28</v>
@@ -31262,76 +31262,76 @@
         <v>44528.75</v>
       </c>
       <c r="F346" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G346" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H346">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I346">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J346" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K346">
-        <v>2.45</v>
+        <v>1.5</v>
       </c>
       <c r="L346">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="M346">
-        <v>2.625</v>
+        <v>5.5</v>
       </c>
       <c r="N346">
-        <v>2.25</v>
+        <v>1.65</v>
       </c>
       <c r="O346">
-        <v>3.25</v>
+        <v>3.6</v>
       </c>
       <c r="P346">
-        <v>2.9</v>
+        <v>4.5</v>
       </c>
       <c r="Q346">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R346">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="S346">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="T346">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U346">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V346">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="W346">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="X346">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="Y346">
         <v>-1</v>
       </c>
       <c r="Z346">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AA346">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AB346">
         <v>-1</v>
       </c>
       <c r="AC346">
-        <v>0.875</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="347" spans="1:29">
@@ -31339,7 +31339,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>3898955</v>
+        <v>4365259</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31351,76 +31351,76 @@
         <v>44528.75</v>
       </c>
       <c r="F347" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G347" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H347">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I347">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J347" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K347">
-        <v>1.5</v>
+        <v>2.45</v>
       </c>
       <c r="L347">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="M347">
-        <v>5.5</v>
+        <v>2.625</v>
       </c>
       <c r="N347">
-        <v>1.65</v>
+        <v>2.25</v>
       </c>
       <c r="O347">
-        <v>3.6</v>
+        <v>3.25</v>
       </c>
       <c r="P347">
-        <v>4.5</v>
+        <v>2.9</v>
       </c>
       <c r="Q347">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R347">
+        <v>1.95</v>
+      </c>
+      <c r="S347">
+        <v>1.85</v>
+      </c>
+      <c r="T347">
+        <v>2.5</v>
+      </c>
+      <c r="U347">
         <v>1.925</v>
       </c>
-      <c r="S347">
+      <c r="V347">
         <v>1.875</v>
       </c>
-      <c r="T347">
-        <v>2.75</v>
-      </c>
-      <c r="U347">
-        <v>2</v>
-      </c>
-      <c r="V347">
-        <v>1.8</v>
-      </c>
       <c r="W347">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X347">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="Y347">
         <v>-1</v>
       </c>
       <c r="Z347">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AA347">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AB347">
         <v>-1</v>
       </c>
       <c r="AC347">
-        <v>0.8</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="348" spans="1:29">
@@ -31428,7 +31428,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>3899778</v>
+        <v>3899776</v>
       </c>
       <c r="C348" t="s">
         <v>28</v>
@@ -31440,49 +31440,49 @@
         <v>44534.75</v>
       </c>
       <c r="F348" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G348" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H348">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I348">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J348" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K348">
-        <v>2.05</v>
+        <v>1.666</v>
       </c>
       <c r="L348">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M348">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="N348">
-        <v>2</v>
+        <v>1.333</v>
       </c>
       <c r="O348">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P348">
-        <v>3.6</v>
+        <v>9.5</v>
       </c>
       <c r="Q348">
-        <v>-0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R348">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="S348">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="T348">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U348">
         <v>1.85</v>
@@ -31494,22 +31494,22 @@
         <v>-1</v>
       </c>
       <c r="X348">
-        <v>-1</v>
+        <v>3.75</v>
       </c>
       <c r="Y348">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z348">
         <v>-1</v>
       </c>
       <c r="AA348">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AB348">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC348">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="349" spans="1:29">
@@ -31517,7 +31517,7 @@
         <v>347</v>
       </c>
       <c r="B349">
-        <v>3899774</v>
+        <v>3898957</v>
       </c>
       <c r="C349" t="s">
         <v>28</v>
@@ -31529,76 +31529,76 @@
         <v>44534.75</v>
       </c>
       <c r="F349" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G349" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H349">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I349">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J349" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K349">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="L349">
+        <v>3.25</v>
+      </c>
+      <c r="M349">
+        <v>2.05</v>
+      </c>
+      <c r="N349">
+        <v>3.5</v>
+      </c>
+      <c r="O349">
         <v>3.4</v>
       </c>
-      <c r="M349">
+      <c r="P349">
+        <v>2.1</v>
+      </c>
+      <c r="Q349">
+        <v>0.25</v>
+      </c>
+      <c r="R349">
+        <v>2.05</v>
+      </c>
+      <c r="S349">
         <v>1.8</v>
       </c>
-      <c r="N349">
-        <v>9</v>
-      </c>
-      <c r="O349">
-        <v>4.75</v>
-      </c>
-      <c r="P349">
-        <v>1.363</v>
-      </c>
-      <c r="Q349">
-        <v>1.5</v>
-      </c>
-      <c r="R349">
-        <v>1.775</v>
-      </c>
-      <c r="S349">
+      <c r="T349">
+        <v>2.25</v>
+      </c>
+      <c r="U349">
+        <v>1.825</v>
+      </c>
+      <c r="V349">
         <v>2.025</v>
       </c>
-      <c r="T349">
-        <v>2.5</v>
-      </c>
-      <c r="U349">
-        <v>1.8</v>
-      </c>
-      <c r="V349">
-        <v>2</v>
-      </c>
       <c r="W349">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="X349">
         <v>-1</v>
       </c>
       <c r="Y349">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="Z349">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA349">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB349">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC349">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="350" spans="1:29">
@@ -31606,7 +31606,7 @@
         <v>348</v>
       </c>
       <c r="B350">
-        <v>3898957</v>
+        <v>3899774</v>
       </c>
       <c r="C350" t="s">
         <v>28</v>
@@ -31618,76 +31618,76 @@
         <v>44534.75</v>
       </c>
       <c r="F350" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G350" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H350">
+        <v>1</v>
+      </c>
+      <c r="I350">
         <v>0</v>
       </c>
-      <c r="I350">
-        <v>3</v>
-      </c>
       <c r="J350" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K350">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="L350">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="M350">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="N350">
-        <v>3.5</v>
+        <v>9</v>
       </c>
       <c r="O350">
-        <v>3.4</v>
+        <v>4.75</v>
       </c>
       <c r="P350">
-        <v>2.1</v>
+        <v>1.363</v>
       </c>
       <c r="Q350">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="R350">
-        <v>2.05</v>
+        <v>1.775</v>
       </c>
       <c r="S350">
+        <v>2.025</v>
+      </c>
+      <c r="T350">
+        <v>2.5</v>
+      </c>
+      <c r="U350">
         <v>1.8</v>
       </c>
-      <c r="T350">
-        <v>2.25</v>
-      </c>
-      <c r="U350">
-        <v>1.825</v>
-      </c>
       <c r="V350">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W350">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="X350">
         <v>-1</v>
       </c>
       <c r="Y350">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="Z350">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA350">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB350">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC350">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="351" spans="1:29">
@@ -31695,7 +31695,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>3899776</v>
+        <v>3899778</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31707,49 +31707,49 @@
         <v>44534.75</v>
       </c>
       <c r="F351" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G351" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H351">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I351">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J351" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K351">
-        <v>1.666</v>
+        <v>2.05</v>
       </c>
       <c r="L351">
+        <v>3.4</v>
+      </c>
+      <c r="M351">
+        <v>3.1</v>
+      </c>
+      <c r="N351">
+        <v>2</v>
+      </c>
+      <c r="O351">
         <v>3.6</v>
       </c>
-      <c r="M351">
-        <v>4.5</v>
-      </c>
-      <c r="N351">
-        <v>1.333</v>
-      </c>
-      <c r="O351">
-        <v>4.75</v>
-      </c>
       <c r="P351">
-        <v>9.5</v>
+        <v>3.6</v>
       </c>
       <c r="Q351">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R351">
+        <v>2</v>
+      </c>
+      <c r="S351">
         <v>1.8</v>
       </c>
-      <c r="S351">
-        <v>2</v>
-      </c>
       <c r="T351">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U351">
         <v>1.85</v>
@@ -31761,22 +31761,22 @@
         <v>-1</v>
       </c>
       <c r="X351">
-        <v>3.75</v>
+        <v>-1</v>
       </c>
       <c r="Y351">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Z351">
         <v>-1</v>
       </c>
       <c r="AA351">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AB351">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC351">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="352" spans="1:29">
@@ -52699,7 +52699,7 @@
         <v>585</v>
       </c>
       <c r="B587">
-        <v>4614405</v>
+        <v>4617491</v>
       </c>
       <c r="C587" t="s">
         <v>28</v>
@@ -52711,73 +52711,73 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F587" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G587" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H587">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I587">
+        <v>4</v>
+      </c>
+      <c r="J587" t="s">
+        <v>53</v>
+      </c>
+      <c r="K587">
+        <v>2.7</v>
+      </c>
+      <c r="L587">
+        <v>3.3</v>
+      </c>
+      <c r="M587">
+        <v>2.45</v>
+      </c>
+      <c r="N587">
+        <v>2.7</v>
+      </c>
+      <c r="O587">
+        <v>3.4</v>
+      </c>
+      <c r="P587">
+        <v>2.6</v>
+      </c>
+      <c r="Q587">
         <v>0</v>
       </c>
-      <c r="J587" t="s">
-        <v>52</v>
-      </c>
-      <c r="K587">
-        <v>1.75</v>
-      </c>
-      <c r="L587">
-        <v>3.5</v>
-      </c>
-      <c r="M587">
-        <v>4.333</v>
-      </c>
-      <c r="N587">
-        <v>1.833</v>
-      </c>
-      <c r="O587">
-        <v>3.5</v>
-      </c>
-      <c r="P587">
-        <v>4.5</v>
-      </c>
-      <c r="Q587">
-        <v>-0.5</v>
-      </c>
       <c r="R587">
+        <v>2</v>
+      </c>
+      <c r="S587">
         <v>1.8</v>
-      </c>
-      <c r="S587">
-        <v>2</v>
       </c>
       <c r="T587">
         <v>2.5</v>
       </c>
       <c r="U587">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="V587">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W587">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="X587">
         <v>-1</v>
       </c>
       <c r="Y587">
-        <v>-1</v>
+        <v>1.6</v>
       </c>
       <c r="Z587">
+        <v>-1</v>
+      </c>
+      <c r="AA587">
         <v>0.8</v>
       </c>
-      <c r="AA587">
-        <v>-1</v>
-      </c>
       <c r="AB587">
-        <v>0.875</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC587">
         <v>-1</v>
@@ -52788,7 +52788,7 @@
         <v>586</v>
       </c>
       <c r="B588">
-        <v>4617491</v>
+        <v>4617747</v>
       </c>
       <c r="C588" t="s">
         <v>28</v>
@@ -52800,76 +52800,76 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F588" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G588" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H588">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I588">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J588" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K588">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
       <c r="L588">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="M588">
-        <v>2.45</v>
+        <v>2.9</v>
       </c>
       <c r="N588">
-        <v>2.7</v>
+        <v>2.15</v>
       </c>
       <c r="O588">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="P588">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
       <c r="Q588">
+        <v>-0.25</v>
+      </c>
+      <c r="R588">
+        <v>1.825</v>
+      </c>
+      <c r="S588">
+        <v>1.975</v>
+      </c>
+      <c r="T588">
+        <v>2</v>
+      </c>
+      <c r="U588">
+        <v>1.775</v>
+      </c>
+      <c r="V588">
+        <v>2.025</v>
+      </c>
+      <c r="W588">
+        <v>1.15</v>
+      </c>
+      <c r="X588">
+        <v>-1</v>
+      </c>
+      <c r="Y588">
+        <v>-1</v>
+      </c>
+      <c r="Z588">
+        <v>0.825</v>
+      </c>
+      <c r="AA588">
+        <v>-1</v>
+      </c>
+      <c r="AB588">
         <v>0</v>
       </c>
-      <c r="R588">
-        <v>2</v>
-      </c>
-      <c r="S588">
-        <v>1.8</v>
-      </c>
-      <c r="T588">
-        <v>2.5</v>
-      </c>
-      <c r="U588">
-        <v>1.9</v>
-      </c>
-      <c r="V588">
-        <v>1.9</v>
-      </c>
-      <c r="W588">
-        <v>-1</v>
-      </c>
-      <c r="X588">
-        <v>-1</v>
-      </c>
-      <c r="Y588">
-        <v>1.6</v>
-      </c>
-      <c r="Z588">
-        <v>-1</v>
-      </c>
-      <c r="AA588">
-        <v>0.8</v>
-      </c>
-      <c r="AB588">
-        <v>0.8999999999999999</v>
-      </c>
       <c r="AC588">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="589" spans="1:29">
@@ -52877,7 +52877,7 @@
         <v>587</v>
       </c>
       <c r="B589">
-        <v>4617747</v>
+        <v>4614405</v>
       </c>
       <c r="C589" t="s">
         <v>28</v>
@@ -52889,13 +52889,13 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F589" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G589" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H589">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I589">
         <v>0</v>
@@ -52904,43 +52904,43 @@
         <v>52</v>
       </c>
       <c r="K589">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="L589">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="M589">
-        <v>2.9</v>
+        <v>4.333</v>
       </c>
       <c r="N589">
-        <v>2.15</v>
+        <v>1.833</v>
       </c>
       <c r="O589">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="P589">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="Q589">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R589">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="S589">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T589">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U589">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="V589">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W589">
-        <v>1.15</v>
+        <v>0.833</v>
       </c>
       <c r="X589">
         <v>-1</v>
@@ -52949,16 +52949,16 @@
         <v>-1</v>
       </c>
       <c r="Z589">
-        <v>0.825</v>
+        <v>0.8</v>
       </c>
       <c r="AA589">
         <v>-1</v>
       </c>
       <c r="AB589">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="AC589">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="590" spans="1:29">
@@ -53055,7 +53055,7 @@
         <v>589</v>
       </c>
       <c r="B591">
-        <v>4617739</v>
+        <v>4614403</v>
       </c>
       <c r="C591" t="s">
         <v>28</v>
@@ -53067,76 +53067,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F591" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G591" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H591">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I591">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J591" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K591">
-        <v>2.3</v>
+        <v>3</v>
       </c>
       <c r="L591">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="M591">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="N591">
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="O591">
         <v>3.5</v>
       </c>
       <c r="P591">
-        <v>3.4</v>
+        <v>2.15</v>
       </c>
       <c r="Q591">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R591">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="S591">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="T591">
         <v>2.25</v>
       </c>
       <c r="U591">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="V591">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="W591">
         <v>-1</v>
       </c>
       <c r="X591">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y591">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="Z591">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AA591">
-        <v>0.5</v>
+        <v>0.825</v>
       </c>
       <c r="AB591">
         <v>-0.5</v>
       </c>
       <c r="AC591">
-        <v>0.5</v>
+        <v>0.5125</v>
       </c>
     </row>
     <row r="592" spans="1:29">
@@ -53144,7 +53144,7 @@
         <v>590</v>
       </c>
       <c r="B592">
-        <v>4617490</v>
+        <v>4617739</v>
       </c>
       <c r="C592" t="s">
         <v>28</v>
@@ -53156,76 +53156,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F592" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G592" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H592">
+        <v>1</v>
+      </c>
+      <c r="I592">
+        <v>1</v>
+      </c>
+      <c r="J592" t="s">
+        <v>51</v>
+      </c>
+      <c r="K592">
+        <v>2.3</v>
+      </c>
+      <c r="L592">
+        <v>3.2</v>
+      </c>
+      <c r="M592">
         <v>3</v>
       </c>
-      <c r="I592">
-        <v>0</v>
-      </c>
-      <c r="J592" t="s">
-        <v>52</v>
-      </c>
-      <c r="K592">
-        <v>1.55</v>
-      </c>
-      <c r="L592">
-        <v>4</v>
-      </c>
-      <c r="M592">
-        <v>5.5</v>
-      </c>
       <c r="N592">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="O592">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P592">
-        <v>7.5</v>
+        <v>3.4</v>
       </c>
       <c r="Q592">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R592">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S592">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="T592">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="U592">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="V592">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="W592">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X592">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y592">
         <v>-1</v>
       </c>
       <c r="Z592">
-        <v>0.8500000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AA592">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="AB592">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AC592">
-        <v>-0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="593" spans="1:29">
@@ -53233,7 +53233,7 @@
         <v>591</v>
       </c>
       <c r="B593">
-        <v>4614403</v>
+        <v>4617490</v>
       </c>
       <c r="C593" t="s">
         <v>28</v>
@@ -53245,76 +53245,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F593" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G593" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H593">
+        <v>3</v>
+      </c>
+      <c r="I593">
         <v>0</v>
       </c>
-      <c r="I593">
-        <v>2</v>
-      </c>
       <c r="J593" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K593">
+        <v>1.55</v>
+      </c>
+      <c r="L593">
+        <v>4</v>
+      </c>
+      <c r="M593">
+        <v>5.5</v>
+      </c>
+      <c r="N593">
+        <v>1.4</v>
+      </c>
+      <c r="O593">
+        <v>4.75</v>
+      </c>
+      <c r="P593">
+        <v>7.5</v>
+      </c>
+      <c r="Q593">
+        <v>-1.25</v>
+      </c>
+      <c r="R593">
+        <v>1.85</v>
+      </c>
+      <c r="S593">
+        <v>1.95</v>
+      </c>
+      <c r="T593">
         <v>3</v>
       </c>
-      <c r="L593">
-        <v>3.4</v>
-      </c>
-      <c r="M593">
-        <v>2.2</v>
-      </c>
-      <c r="N593">
-        <v>3.4</v>
-      </c>
-      <c r="O593">
-        <v>3.5</v>
-      </c>
-      <c r="P593">
-        <v>2.15</v>
-      </c>
-      <c r="Q593">
-        <v>0.25</v>
-      </c>
-      <c r="R593">
-        <v>1.975</v>
-      </c>
-      <c r="S593">
-        <v>1.825</v>
-      </c>
-      <c r="T593">
-        <v>2.25</v>
-      </c>
       <c r="U593">
-        <v>1.775</v>
+        <v>2</v>
       </c>
       <c r="V593">
-        <v>2.025</v>
+        <v>1.8</v>
       </c>
       <c r="W593">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="X593">
         <v>-1</v>
       </c>
       <c r="Y593">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="Z593">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA593">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB593">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AC593">
-        <v>0.5125</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="594" spans="1:29">
@@ -72101,7 +72101,7 @@
         <v>803</v>
       </c>
       <c r="B805">
-        <v>7323186</v>
+        <v>7323253</v>
       </c>
       <c r="C805" t="s">
         <v>28</v>
@@ -72113,19 +72113,19 @@
         <v>45242.83333333334</v>
       </c>
       <c r="F805" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G805" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="H805">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I805">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J805" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K805">
         <v>2</v>
@@ -72137,52 +72137,52 @@
         <v>3.5</v>
       </c>
       <c r="N805">
-        <v>1.727</v>
+        <v>2.1</v>
       </c>
       <c r="O805">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="P805">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
       <c r="Q805">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R805">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S805">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T805">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U805">
+        <v>1.95</v>
+      </c>
+      <c r="V805">
         <v>1.85</v>
       </c>
-      <c r="V805">
-        <v>1.95</v>
-      </c>
       <c r="W805">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X805">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y805">
         <v>-1</v>
       </c>
       <c r="Z805">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AA805">
-        <v>-0.5</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB805">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC805">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="806" spans="1:29">
@@ -72190,7 +72190,7 @@
         <v>804</v>
       </c>
       <c r="B806">
-        <v>7323253</v>
+        <v>7323186</v>
       </c>
       <c r="C806" t="s">
         <v>28</v>
@@ -72202,19 +72202,19 @@
         <v>45242.83333333334</v>
       </c>
       <c r="F806" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G806" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="H806">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I806">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J806" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K806">
         <v>2</v>
@@ -72226,52 +72226,52 @@
         <v>3.5</v>
       </c>
       <c r="N806">
-        <v>2.1</v>
+        <v>1.727</v>
       </c>
       <c r="O806">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="P806">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="Q806">
+        <v>-0.75</v>
+      </c>
+      <c r="R806">
+        <v>1.9</v>
+      </c>
+      <c r="S806">
+        <v>1.9</v>
+      </c>
+      <c r="T806">
+        <v>2.75</v>
+      </c>
+      <c r="U806">
+        <v>1.85</v>
+      </c>
+      <c r="V806">
+        <v>1.95</v>
+      </c>
+      <c r="W806">
+        <v>0.7270000000000001</v>
+      </c>
+      <c r="X806">
+        <v>-1</v>
+      </c>
+      <c r="Y806">
+        <v>-1</v>
+      </c>
+      <c r="Z806">
+        <v>0.45</v>
+      </c>
+      <c r="AA806">
         <v>-0.5</v>
       </c>
-      <c r="R806">
-        <v>2.025</v>
-      </c>
-      <c r="S806">
-        <v>1.775</v>
-      </c>
-      <c r="T806">
-        <v>2.5</v>
-      </c>
-      <c r="U806">
-        <v>1.95</v>
-      </c>
-      <c r="V806">
-        <v>1.85</v>
-      </c>
-      <c r="W806">
-        <v>-1</v>
-      </c>
-      <c r="X806">
-        <v>2.5</v>
-      </c>
-      <c r="Y806">
-        <v>-1</v>
-      </c>
-      <c r="Z806">
-        <v>-1</v>
-      </c>
-      <c r="AA806">
-        <v>0.7749999999999999</v>
-      </c>
       <c r="AB806">
+        <v>-1</v>
+      </c>
+      <c r="AC806">
         <v>0.95</v>
-      </c>
-      <c r="AC806">
-        <v>-1</v>
       </c>
     </row>
     <row r="807" spans="1:29">
@@ -73080,7 +73080,7 @@
         <v>814</v>
       </c>
       <c r="B816">
-        <v>6078265</v>
+        <v>6078266</v>
       </c>
       <c r="C816" t="s">
         <v>28</v>
@@ -73092,76 +73092,76 @@
         <v>45262.75</v>
       </c>
       <c r="F816" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G816" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H816">
+        <v>4</v>
+      </c>
+      <c r="I816">
         <v>0</v>
       </c>
-      <c r="I816">
-        <v>2</v>
-      </c>
       <c r="J816" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K816">
-        <v>1.666</v>
+        <v>1.533</v>
       </c>
       <c r="L816">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="M816">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N816">
-        <v>2.25</v>
+        <v>1.363</v>
       </c>
       <c r="O816">
-        <v>3.3</v>
+        <v>4.75</v>
       </c>
       <c r="P816">
-        <v>3.3</v>
+        <v>7.5</v>
       </c>
       <c r="Q816">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R816">
+        <v>2.025</v>
+      </c>
+      <c r="S816">
+        <v>1.825</v>
+      </c>
+      <c r="T816">
+        <v>3</v>
+      </c>
+      <c r="U816">
+        <v>1.9</v>
+      </c>
+      <c r="V816">
         <v>1.95</v>
       </c>
-      <c r="S816">
-        <v>1.85</v>
-      </c>
-      <c r="T816">
-        <v>2.5</v>
-      </c>
-      <c r="U816">
-        <v>1.8</v>
-      </c>
-      <c r="V816">
-        <v>2</v>
-      </c>
       <c r="W816">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="X816">
         <v>-1</v>
       </c>
       <c r="Y816">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z816">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA816">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB816">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC816">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="817" spans="1:29">
@@ -73169,7 +73169,7 @@
         <v>815</v>
       </c>
       <c r="B817">
-        <v>6078266</v>
+        <v>6077498</v>
       </c>
       <c r="C817" t="s">
         <v>28</v>
@@ -73181,73 +73181,73 @@
         <v>45262.75</v>
       </c>
       <c r="F817" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G817" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H817">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I817">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J817" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K817">
-        <v>1.533</v>
+        <v>1.65</v>
       </c>
       <c r="L817">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="M817">
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="N817">
-        <v>1.363</v>
+        <v>1.909</v>
       </c>
       <c r="O817">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="P817">
-        <v>7.5</v>
+        <v>4.2</v>
       </c>
       <c r="Q817">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R817">
+        <v>1.85</v>
+      </c>
+      <c r="S817">
+        <v>2</v>
+      </c>
+      <c r="T817">
+        <v>2.75</v>
+      </c>
+      <c r="U817">
         <v>2.025</v>
       </c>
-      <c r="S817">
+      <c r="V817">
         <v>1.825</v>
       </c>
-      <c r="T817">
-        <v>3</v>
-      </c>
-      <c r="U817">
-        <v>1.9</v>
-      </c>
-      <c r="V817">
-        <v>1.95</v>
-      </c>
       <c r="W817">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="X817">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y817">
         <v>-1</v>
       </c>
       <c r="Z817">
+        <v>-1</v>
+      </c>
+      <c r="AA817">
+        <v>1</v>
+      </c>
+      <c r="AB817">
         <v>1.025</v>
-      </c>
-      <c r="AA817">
-        <v>-1</v>
-      </c>
-      <c r="AB817">
-        <v>0.8999999999999999</v>
       </c>
       <c r="AC817">
         <v>-1</v>
@@ -73258,7 +73258,7 @@
         <v>816</v>
       </c>
       <c r="B818">
-        <v>6077498</v>
+        <v>6078265</v>
       </c>
       <c r="C818" t="s">
         <v>28</v>
@@ -73270,76 +73270,76 @@
         <v>45262.75</v>
       </c>
       <c r="F818" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G818" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H818">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I818">
         <v>2</v>
       </c>
       <c r="J818" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K818">
-        <v>1.65</v>
+        <v>1.666</v>
       </c>
       <c r="L818">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M818">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="N818">
-        <v>1.909</v>
+        <v>2.25</v>
       </c>
       <c r="O818">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="P818">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="Q818">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R818">
+        <v>1.95</v>
+      </c>
+      <c r="S818">
         <v>1.85</v>
       </c>
-      <c r="S818">
-        <v>2</v>
-      </c>
       <c r="T818">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U818">
-        <v>2.025</v>
+        <v>1.8</v>
       </c>
       <c r="V818">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W818">
         <v>-1</v>
       </c>
       <c r="X818">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y818">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z818">
         <v>-1</v>
       </c>
       <c r="AA818">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB818">
+        <v>-1</v>
+      </c>
+      <c r="AC818">
         <v>1</v>
-      </c>
-      <c r="AB818">
-        <v>1.025</v>
-      </c>
-      <c r="AC818">
-        <v>-1</v>
       </c>
     </row>
     <row r="819" spans="1:29">
@@ -73970,7 +73970,7 @@
         <v>824</v>
       </c>
       <c r="B826">
-        <v>6078998</v>
+        <v>6078269</v>
       </c>
       <c r="C826" t="s">
         <v>28</v>
@@ -73982,73 +73982,73 @@
         <v>45269.75</v>
       </c>
       <c r="F826" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G826" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H826">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I826">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J826" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K826">
-        <v>1.909</v>
+        <v>1.85</v>
       </c>
       <c r="L826">
+        <v>3.4</v>
+      </c>
+      <c r="M826">
+        <v>4.333</v>
+      </c>
+      <c r="N826">
+        <v>1.8</v>
+      </c>
+      <c r="O826">
         <v>3.6</v>
       </c>
-      <c r="M826">
-        <v>3.8</v>
-      </c>
-      <c r="N826">
-        <v>2.15</v>
-      </c>
-      <c r="O826">
-        <v>3.75</v>
-      </c>
       <c r="P826">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="Q826">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R826">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S826">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="T826">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U826">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="V826">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W826">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X826">
         <v>-1</v>
       </c>
       <c r="Y826">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z826">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA826">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB826">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AC826">
         <v>-1</v>
@@ -74059,7 +74059,7 @@
         <v>825</v>
       </c>
       <c r="B827">
-        <v>6077499</v>
+        <v>6078998</v>
       </c>
       <c r="C827" t="s">
         <v>28</v>
@@ -74071,76 +74071,76 @@
         <v>45269.75</v>
       </c>
       <c r="F827" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G827" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H827">
         <v>2</v>
       </c>
       <c r="I827">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J827" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K827">
-        <v>2.1</v>
+        <v>1.909</v>
       </c>
       <c r="L827">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M827">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N827">
-        <v>2.9</v>
+        <v>2.15</v>
       </c>
       <c r="O827">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="P827">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="Q827">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R827">
-        <v>1.775</v>
+        <v>1.85</v>
       </c>
       <c r="S827">
-        <v>2.1</v>
+        <v>1.95</v>
       </c>
       <c r="T827">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U827">
         <v>1.85</v>
       </c>
       <c r="V827">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W827">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="X827">
         <v>-1</v>
       </c>
       <c r="Y827">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="Z827">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA827">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB827">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC827">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="828" spans="1:29">
@@ -74148,7 +74148,7 @@
         <v>826</v>
       </c>
       <c r="B828">
-        <v>6077768</v>
+        <v>6077499</v>
       </c>
       <c r="C828" t="s">
         <v>28</v>
@@ -74160,76 +74160,76 @@
         <v>45269.75</v>
       </c>
       <c r="F828" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G828" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H828">
+        <v>2</v>
+      </c>
+      <c r="I828">
         <v>0</v>
       </c>
-      <c r="I828">
-        <v>3</v>
-      </c>
       <c r="J828" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K828">
-        <v>2.05</v>
+        <v>2.1</v>
       </c>
       <c r="L828">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M828">
         <v>3.4</v>
       </c>
       <c r="N828">
-        <v>2.05</v>
+        <v>2.9</v>
       </c>
       <c r="O828">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="P828">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q828">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R828">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="S828">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="T828">
         <v>2.75</v>
       </c>
       <c r="U828">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V828">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W828">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="X828">
         <v>-1</v>
       </c>
       <c r="Y828">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z828">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA828">
+        <v>-1</v>
+      </c>
+      <c r="AB828">
+        <v>-1</v>
+      </c>
+      <c r="AC828">
         <v>1</v>
-      </c>
-      <c r="AB828">
-        <v>0.4875</v>
-      </c>
-      <c r="AC828">
-        <v>-0.5</v>
       </c>
     </row>
     <row r="829" spans="1:29">
@@ -74237,7 +74237,7 @@
         <v>827</v>
       </c>
       <c r="B829">
-        <v>6078269</v>
+        <v>6078268</v>
       </c>
       <c r="C829" t="s">
         <v>28</v>
@@ -74249,76 +74249,76 @@
         <v>45269.75</v>
       </c>
       <c r="F829" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G829" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="H829">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I829">
         <v>1</v>
       </c>
       <c r="J829" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K829">
-        <v>1.85</v>
+        <v>3.1</v>
       </c>
       <c r="L829">
+        <v>3.3</v>
+      </c>
+      <c r="M829">
+        <v>2.3</v>
+      </c>
+      <c r="N829">
+        <v>2.9</v>
+      </c>
+      <c r="O829">
         <v>3.4</v>
       </c>
-      <c r="M829">
-        <v>4.333</v>
-      </c>
-      <c r="N829">
+      <c r="P829">
+        <v>2.375</v>
+      </c>
+      <c r="Q829">
+        <v>0.25</v>
+      </c>
+      <c r="R829">
         <v>1.8</v>
       </c>
-      <c r="O829">
-        <v>3.6</v>
-      </c>
-      <c r="P829">
-        <v>4.5</v>
-      </c>
-      <c r="Q829">
-        <v>-0.75</v>
-      </c>
-      <c r="R829">
-        <v>1.925</v>
-      </c>
       <c r="S829">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="T829">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U829">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V829">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="W829">
+        <v>-1</v>
+      </c>
+      <c r="X829">
+        <v>-1</v>
+      </c>
+      <c r="Y829">
+        <v>1.375</v>
+      </c>
+      <c r="Z829">
+        <v>-1</v>
+      </c>
+      <c r="AA829">
+        <v>1</v>
+      </c>
+      <c r="AB829">
+        <v>-1</v>
+      </c>
+      <c r="AC829">
         <v>0.8</v>
-      </c>
-      <c r="X829">
-        <v>-1</v>
-      </c>
-      <c r="Y829">
-        <v>-1</v>
-      </c>
-      <c r="Z829">
-        <v>0.925</v>
-      </c>
-      <c r="AA829">
-        <v>-1</v>
-      </c>
-      <c r="AB829">
-        <v>1.025</v>
-      </c>
-      <c r="AC829">
-        <v>-1</v>
       </c>
     </row>
     <row r="830" spans="1:29">
@@ -74326,7 +74326,7 @@
         <v>828</v>
       </c>
       <c r="B830">
-        <v>6078268</v>
+        <v>6077768</v>
       </c>
       <c r="C830" t="s">
         <v>28</v>
@@ -74338,40 +74338,40 @@
         <v>45269.75</v>
       </c>
       <c r="F830" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G830" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H830">
         <v>0</v>
       </c>
       <c r="I830">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J830" t="s">
         <v>53</v>
       </c>
       <c r="K830">
-        <v>3.1</v>
+        <v>2.05</v>
       </c>
       <c r="L830">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M830">
-        <v>2.3</v>
+        <v>3.4</v>
       </c>
       <c r="N830">
-        <v>2.9</v>
+        <v>2.05</v>
       </c>
       <c r="O830">
+        <v>3.6</v>
+      </c>
+      <c r="P830">
         <v>3.4</v>
       </c>
-      <c r="P830">
-        <v>2.375</v>
-      </c>
       <c r="Q830">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R830">
         <v>1.8</v>
@@ -74383,10 +74383,10 @@
         <v>2.75</v>
       </c>
       <c r="U830">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V830">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="W830">
         <v>-1</v>
@@ -74395,7 +74395,7 @@
         <v>-1</v>
       </c>
       <c r="Y830">
-        <v>1.375</v>
+        <v>2.4</v>
       </c>
       <c r="Z830">
         <v>-1</v>
@@ -74404,10 +74404,10 @@
         <v>1</v>
       </c>
       <c r="AB830">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AC830">
-        <v>0.8</v>
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-28 às 18-17
</commit_message>
<xml_diff>
--- a/Chile Primera Division/Chile Primera Division.xlsx
+++ b/Chile Primera Division/Chile Primera Division.xlsx
@@ -6597,7 +6597,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>3201281</v>
+        <v>3200931</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6609,76 +6609,76 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F69" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G69" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K69">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="L69">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="M69">
-        <v>2.375</v>
+        <v>3.3</v>
       </c>
       <c r="N69">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="O69">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="P69">
-        <v>2.15</v>
+        <v>3.6</v>
       </c>
       <c r="Q69">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R69">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S69">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="T69">
         <v>2.25</v>
       </c>
       <c r="U69">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="V69">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W69">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="X69">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y69">
         <v>-1</v>
       </c>
       <c r="Z69">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AA69">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="AB69">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC69">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -6686,7 +6686,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>3201280</v>
+        <v>3201269</v>
       </c>
       <c r="C70" t="s">
         <v>28</v>
@@ -6698,10 +6698,10 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G70" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -6713,31 +6713,31 @@
         <v>51</v>
       </c>
       <c r="K70">
-        <v>1.833</v>
+        <v>2</v>
       </c>
       <c r="L70">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="M70">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N70">
-        <v>2</v>
+        <v>2.3</v>
       </c>
       <c r="O70">
         <v>3.5</v>
       </c>
       <c r="P70">
-        <v>3.5</v>
+        <v>2.875</v>
       </c>
       <c r="Q70">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R70">
-        <v>1.85</v>
+        <v>1.75</v>
       </c>
       <c r="S70">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T70">
         <v>2.5</v>
@@ -6758,10 +6758,10 @@
         <v>-1</v>
       </c>
       <c r="Z70">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AA70">
-        <v>0.475</v>
+        <v>-0</v>
       </c>
       <c r="AB70">
         <v>-1</v>
@@ -6775,7 +6775,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>3200931</v>
+        <v>3201280</v>
       </c>
       <c r="C71" t="s">
         <v>28</v>
@@ -6787,61 +6787,61 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F71" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G71" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J71" t="s">
         <v>51</v>
       </c>
       <c r="K71">
-        <v>2.2</v>
+        <v>1.833</v>
       </c>
       <c r="L71">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="M71">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="N71">
         <v>2</v>
       </c>
       <c r="O71">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P71">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="Q71">
         <v>-0.25</v>
       </c>
       <c r="R71">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S71">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="T71">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U71">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="V71">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="W71">
         <v>-1</v>
       </c>
       <c r="X71">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="Y71">
         <v>-1</v>
@@ -6850,13 +6850,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA71">
-        <v>0.5</v>
+        <v>0.475</v>
       </c>
       <c r="AB71">
         <v>-1</v>
       </c>
       <c r="AC71">
-        <v>0.95</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="72" spans="1:29">
@@ -6864,7 +6864,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>3201269</v>
+        <v>3201281</v>
       </c>
       <c r="C72" t="s">
         <v>28</v>
@@ -6876,76 +6876,76 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F72" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G72" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L72">
+        <v>3.2</v>
+      </c>
+      <c r="M72">
+        <v>2.375</v>
+      </c>
+      <c r="N72">
         <v>3.5</v>
       </c>
-      <c r="M72">
-        <v>3.6</v>
-      </c>
-      <c r="N72">
-        <v>2.3</v>
-      </c>
       <c r="O72">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="P72">
-        <v>2.875</v>
+        <v>2.15</v>
       </c>
       <c r="Q72">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R72">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="S72">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="T72">
+        <v>2.25</v>
+      </c>
+      <c r="U72">
+        <v>1.8</v>
+      </c>
+      <c r="V72">
+        <v>2</v>
+      </c>
+      <c r="W72">
         <v>2.5</v>
       </c>
-      <c r="U72">
-        <v>1.825</v>
-      </c>
-      <c r="V72">
-        <v>1.975</v>
-      </c>
-      <c r="W72">
-        <v>-1</v>
-      </c>
       <c r="X72">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y72">
         <v>-1</v>
       </c>
       <c r="Z72">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="AA72">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB72">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC72">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="73" spans="1:29">
@@ -7042,7 +7042,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>3234177</v>
+        <v>3234974</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7054,73 +7054,73 @@
         <v>44240.77083333334</v>
       </c>
       <c r="F74" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K74">
-        <v>1.85</v>
+        <v>1.75</v>
       </c>
       <c r="L74">
+        <v>3.4</v>
+      </c>
+      <c r="M74">
+        <v>5</v>
+      </c>
+      <c r="N74">
+        <v>1.6</v>
+      </c>
+      <c r="O74">
         <v>3.6</v>
       </c>
-      <c r="M74">
-        <v>4</v>
-      </c>
-      <c r="N74">
-        <v>1.95</v>
-      </c>
-      <c r="O74">
-        <v>3.5</v>
-      </c>
       <c r="P74">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q74">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R74">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S74">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U74">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="V74">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA74">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -7131,7 +7131,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>3234974</v>
+        <v>3234177</v>
       </c>
       <c r="C75" t="s">
         <v>28</v>
@@ -7143,73 +7143,73 @@
         <v>44240.77083333334</v>
       </c>
       <c r="F75" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G75" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H75">
+        <v>2</v>
+      </c>
+      <c r="I75">
         <v>3</v>
       </c>
-      <c r="I75">
+      <c r="J75" t="s">
+        <v>53</v>
+      </c>
+      <c r="K75">
+        <v>1.85</v>
+      </c>
+      <c r="L75">
+        <v>3.6</v>
+      </c>
+      <c r="M75">
+        <v>4</v>
+      </c>
+      <c r="N75">
+        <v>1.95</v>
+      </c>
+      <c r="O75">
+        <v>3.5</v>
+      </c>
+      <c r="P75">
+        <v>4</v>
+      </c>
+      <c r="Q75">
+        <v>-0.5</v>
+      </c>
+      <c r="R75">
+        <v>1.925</v>
+      </c>
+      <c r="S75">
+        <v>1.875</v>
+      </c>
+      <c r="T75">
+        <v>3</v>
+      </c>
+      <c r="U75">
+        <v>2</v>
+      </c>
+      <c r="V75">
+        <v>1.8</v>
+      </c>
+      <c r="W75">
+        <v>-1</v>
+      </c>
+      <c r="X75">
+        <v>-1</v>
+      </c>
+      <c r="Y75">
+        <v>3</v>
+      </c>
+      <c r="Z75">
+        <v>-1</v>
+      </c>
+      <c r="AA75">
+        <v>0.875</v>
+      </c>
+      <c r="AB75">
         <v>1</v>
-      </c>
-      <c r="J75" t="s">
-        <v>52</v>
-      </c>
-      <c r="K75">
-        <v>1.75</v>
-      </c>
-      <c r="L75">
-        <v>3.4</v>
-      </c>
-      <c r="M75">
-        <v>5</v>
-      </c>
-      <c r="N75">
-        <v>1.6</v>
-      </c>
-      <c r="O75">
-        <v>3.6</v>
-      </c>
-      <c r="P75">
-        <v>6</v>
-      </c>
-      <c r="Q75">
-        <v>-0.75</v>
-      </c>
-      <c r="R75">
-        <v>1.8</v>
-      </c>
-      <c r="S75">
-        <v>2</v>
-      </c>
-      <c r="T75">
-        <v>2.75</v>
-      </c>
-      <c r="U75">
-        <v>1.8</v>
-      </c>
-      <c r="V75">
-        <v>2</v>
-      </c>
-      <c r="W75">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="X75">
-        <v>-1</v>
-      </c>
-      <c r="Y75">
-        <v>-1</v>
-      </c>
-      <c r="Z75">
-        <v>0.8</v>
-      </c>
-      <c r="AA75">
-        <v>-1</v>
-      </c>
-      <c r="AB75">
-        <v>0.8</v>
       </c>
       <c r="AC75">
         <v>-1</v>
@@ -31250,7 +31250,7 @@
         <v>344</v>
       </c>
       <c r="B346">
-        <v>3898955</v>
+        <v>4365259</v>
       </c>
       <c r="C346" t="s">
         <v>28</v>
@@ -31262,76 +31262,76 @@
         <v>44528.75</v>
       </c>
       <c r="F346" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G346" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H346">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I346">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J346" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K346">
-        <v>1.5</v>
+        <v>2.45</v>
       </c>
       <c r="L346">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="M346">
-        <v>5.5</v>
+        <v>2.625</v>
       </c>
       <c r="N346">
-        <v>1.65</v>
+        <v>2.25</v>
       </c>
       <c r="O346">
-        <v>3.6</v>
+        <v>3.25</v>
       </c>
       <c r="P346">
-        <v>4.5</v>
+        <v>2.9</v>
       </c>
       <c r="Q346">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R346">
+        <v>1.95</v>
+      </c>
+      <c r="S346">
+        <v>1.85</v>
+      </c>
+      <c r="T346">
+        <v>2.5</v>
+      </c>
+      <c r="U346">
         <v>1.925</v>
       </c>
-      <c r="S346">
+      <c r="V346">
         <v>1.875</v>
       </c>
-      <c r="T346">
-        <v>2.75</v>
-      </c>
-      <c r="U346">
-        <v>2</v>
-      </c>
-      <c r="V346">
-        <v>1.8</v>
-      </c>
       <c r="W346">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X346">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="Y346">
         <v>-1</v>
       </c>
       <c r="Z346">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AA346">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AB346">
         <v>-1</v>
       </c>
       <c r="AC346">
-        <v>0.8</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="347" spans="1:29">
@@ -31339,7 +31339,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>4365259</v>
+        <v>3898955</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31351,76 +31351,76 @@
         <v>44528.75</v>
       </c>
       <c r="F347" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G347" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H347">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I347">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J347" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K347">
-        <v>2.45</v>
+        <v>1.5</v>
       </c>
       <c r="L347">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="M347">
-        <v>2.625</v>
+        <v>5.5</v>
       </c>
       <c r="N347">
-        <v>2.25</v>
+        <v>1.65</v>
       </c>
       <c r="O347">
-        <v>3.25</v>
+        <v>3.6</v>
       </c>
       <c r="P347">
-        <v>2.9</v>
+        <v>4.5</v>
       </c>
       <c r="Q347">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R347">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="S347">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="T347">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U347">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V347">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="W347">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="X347">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="Y347">
         <v>-1</v>
       </c>
       <c r="Z347">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AA347">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AB347">
         <v>-1</v>
       </c>
       <c r="AC347">
-        <v>0.875</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="348" spans="1:29">
@@ -31428,7 +31428,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>3899776</v>
+        <v>3899778</v>
       </c>
       <c r="C348" t="s">
         <v>28</v>
@@ -31440,49 +31440,49 @@
         <v>44534.75</v>
       </c>
       <c r="F348" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G348" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H348">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I348">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J348" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K348">
-        <v>1.666</v>
+        <v>2.05</v>
       </c>
       <c r="L348">
+        <v>3.4</v>
+      </c>
+      <c r="M348">
+        <v>3.1</v>
+      </c>
+      <c r="N348">
+        <v>2</v>
+      </c>
+      <c r="O348">
         <v>3.6</v>
       </c>
-      <c r="M348">
-        <v>4.5</v>
-      </c>
-      <c r="N348">
-        <v>1.333</v>
-      </c>
-      <c r="O348">
-        <v>4.75</v>
-      </c>
       <c r="P348">
-        <v>9.5</v>
+        <v>3.6</v>
       </c>
       <c r="Q348">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R348">
+        <v>2</v>
+      </c>
+      <c r="S348">
         <v>1.8</v>
       </c>
-      <c r="S348">
-        <v>2</v>
-      </c>
       <c r="T348">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U348">
         <v>1.85</v>
@@ -31494,22 +31494,22 @@
         <v>-1</v>
       </c>
       <c r="X348">
-        <v>3.75</v>
+        <v>-1</v>
       </c>
       <c r="Y348">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Z348">
         <v>-1</v>
       </c>
       <c r="AA348">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AB348">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC348">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="349" spans="1:29">
@@ -31517,7 +31517,7 @@
         <v>347</v>
       </c>
       <c r="B349">
-        <v>3898957</v>
+        <v>3899774</v>
       </c>
       <c r="C349" t="s">
         <v>28</v>
@@ -31529,76 +31529,76 @@
         <v>44534.75</v>
       </c>
       <c r="F349" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G349" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H349">
+        <v>1</v>
+      </c>
+      <c r="I349">
         <v>0</v>
       </c>
-      <c r="I349">
-        <v>3</v>
-      </c>
       <c r="J349" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K349">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="L349">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="M349">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="N349">
-        <v>3.5</v>
+        <v>9</v>
       </c>
       <c r="O349">
-        <v>3.4</v>
+        <v>4.75</v>
       </c>
       <c r="P349">
-        <v>2.1</v>
+        <v>1.363</v>
       </c>
       <c r="Q349">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="R349">
-        <v>2.05</v>
+        <v>1.775</v>
       </c>
       <c r="S349">
+        <v>2.025</v>
+      </c>
+      <c r="T349">
+        <v>2.5</v>
+      </c>
+      <c r="U349">
         <v>1.8</v>
       </c>
-      <c r="T349">
-        <v>2.25</v>
-      </c>
-      <c r="U349">
-        <v>1.825</v>
-      </c>
       <c r="V349">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W349">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="X349">
         <v>-1</v>
       </c>
       <c r="Y349">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="Z349">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA349">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB349">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC349">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350" spans="1:29">
@@ -31606,7 +31606,7 @@
         <v>348</v>
       </c>
       <c r="B350">
-        <v>3899774</v>
+        <v>3898957</v>
       </c>
       <c r="C350" t="s">
         <v>28</v>
@@ -31618,76 +31618,76 @@
         <v>44534.75</v>
       </c>
       <c r="F350" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G350" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H350">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I350">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J350" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K350">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="L350">
+        <v>3.25</v>
+      </c>
+      <c r="M350">
+        <v>2.05</v>
+      </c>
+      <c r="N350">
+        <v>3.5</v>
+      </c>
+      <c r="O350">
         <v>3.4</v>
       </c>
-      <c r="M350">
+      <c r="P350">
+        <v>2.1</v>
+      </c>
+      <c r="Q350">
+        <v>0.25</v>
+      </c>
+      <c r="R350">
+        <v>2.05</v>
+      </c>
+      <c r="S350">
         <v>1.8</v>
       </c>
-      <c r="N350">
-        <v>9</v>
-      </c>
-      <c r="O350">
-        <v>4.75</v>
-      </c>
-      <c r="P350">
-        <v>1.363</v>
-      </c>
-      <c r="Q350">
-        <v>1.5</v>
-      </c>
-      <c r="R350">
-        <v>1.775</v>
-      </c>
-      <c r="S350">
+      <c r="T350">
+        <v>2.25</v>
+      </c>
+      <c r="U350">
+        <v>1.825</v>
+      </c>
+      <c r="V350">
         <v>2.025</v>
       </c>
-      <c r="T350">
-        <v>2.5</v>
-      </c>
-      <c r="U350">
-        <v>1.8</v>
-      </c>
-      <c r="V350">
-        <v>2</v>
-      </c>
       <c r="W350">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="X350">
         <v>-1</v>
       </c>
       <c r="Y350">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="Z350">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA350">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB350">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC350">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="351" spans="1:29">
@@ -31695,7 +31695,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>3899778</v>
+        <v>3899776</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31707,49 +31707,49 @@
         <v>44534.75</v>
       </c>
       <c r="F351" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G351" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H351">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I351">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J351" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K351">
-        <v>2.05</v>
+        <v>1.666</v>
       </c>
       <c r="L351">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M351">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="N351">
-        <v>2</v>
+        <v>1.333</v>
       </c>
       <c r="O351">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P351">
-        <v>3.6</v>
+        <v>9.5</v>
       </c>
       <c r="Q351">
-        <v>-0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R351">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="S351">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="T351">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U351">
         <v>1.85</v>
@@ -31761,22 +31761,22 @@
         <v>-1</v>
       </c>
       <c r="X351">
-        <v>-1</v>
+        <v>3.75</v>
       </c>
       <c r="Y351">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z351">
         <v>-1</v>
       </c>
       <c r="AA351">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AB351">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC351">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="352" spans="1:29">
@@ -52699,7 +52699,7 @@
         <v>585</v>
       </c>
       <c r="B587">
-        <v>4617491</v>
+        <v>4614405</v>
       </c>
       <c r="C587" t="s">
         <v>28</v>
@@ -52711,73 +52711,73 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F587" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G587" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H587">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I587">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J587" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K587">
-        <v>2.7</v>
+        <v>1.75</v>
       </c>
       <c r="L587">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M587">
-        <v>2.45</v>
+        <v>4.333</v>
       </c>
       <c r="N587">
-        <v>2.7</v>
+        <v>1.833</v>
       </c>
       <c r="O587">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P587">
-        <v>2.6</v>
+        <v>4.5</v>
       </c>
       <c r="Q587">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R587">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="S587">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="T587">
         <v>2.5</v>
       </c>
       <c r="U587">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="V587">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W587">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="X587">
         <v>-1</v>
       </c>
       <c r="Y587">
-        <v>1.6</v>
+        <v>-1</v>
       </c>
       <c r="Z587">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA587">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB587">
-        <v>0.8999999999999999</v>
+        <v>0.875</v>
       </c>
       <c r="AC587">
         <v>-1</v>
@@ -52788,7 +52788,7 @@
         <v>586</v>
       </c>
       <c r="B588">
-        <v>4617747</v>
+        <v>4617491</v>
       </c>
       <c r="C588" t="s">
         <v>28</v>
@@ -52800,76 +52800,76 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F588" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G588" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H588">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I588">
+        <v>4</v>
+      </c>
+      <c r="J588" t="s">
+        <v>53</v>
+      </c>
+      <c r="K588">
+        <v>2.7</v>
+      </c>
+      <c r="L588">
+        <v>3.3</v>
+      </c>
+      <c r="M588">
+        <v>2.45</v>
+      </c>
+      <c r="N588">
+        <v>2.7</v>
+      </c>
+      <c r="O588">
+        <v>3.4</v>
+      </c>
+      <c r="P588">
+        <v>2.6</v>
+      </c>
+      <c r="Q588">
         <v>0</v>
       </c>
-      <c r="J588" t="s">
-        <v>52</v>
-      </c>
-      <c r="K588">
-        <v>2.4</v>
-      </c>
-      <c r="L588">
-        <v>3.1</v>
-      </c>
-      <c r="M588">
-        <v>2.9</v>
-      </c>
-      <c r="N588">
-        <v>2.15</v>
-      </c>
-      <c r="O588">
-        <v>3.25</v>
-      </c>
-      <c r="P588">
-        <v>3.5</v>
-      </c>
-      <c r="Q588">
-        <v>-0.25</v>
-      </c>
       <c r="R588">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="S588">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T588">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U588">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="V588">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="W588">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X588">
         <v>-1</v>
       </c>
       <c r="Y588">
-        <v>-1</v>
+        <v>1.6</v>
       </c>
       <c r="Z588">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA588">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB588">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC588">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="589" spans="1:29">
@@ -52877,7 +52877,7 @@
         <v>587</v>
       </c>
       <c r="B589">
-        <v>4614405</v>
+        <v>4617747</v>
       </c>
       <c r="C589" t="s">
         <v>28</v>
@@ -52889,13 +52889,13 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F589" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G589" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H589">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I589">
         <v>0</v>
@@ -52904,43 +52904,43 @@
         <v>52</v>
       </c>
       <c r="K589">
-        <v>1.75</v>
+        <v>2.4</v>
       </c>
       <c r="L589">
+        <v>3.1</v>
+      </c>
+      <c r="M589">
+        <v>2.9</v>
+      </c>
+      <c r="N589">
+        <v>2.15</v>
+      </c>
+      <c r="O589">
+        <v>3.25</v>
+      </c>
+      <c r="P589">
         <v>3.5</v>
       </c>
-      <c r="M589">
-        <v>4.333</v>
-      </c>
-      <c r="N589">
-        <v>1.833</v>
-      </c>
-      <c r="O589">
-        <v>3.5</v>
-      </c>
-      <c r="P589">
-        <v>4.5</v>
-      </c>
       <c r="Q589">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R589">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="S589">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T589">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U589">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V589">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W589">
-        <v>0.833</v>
+        <v>1.15</v>
       </c>
       <c r="X589">
         <v>-1</v>
@@ -52949,16 +52949,16 @@
         <v>-1</v>
       </c>
       <c r="Z589">
-        <v>0.8</v>
+        <v>0.825</v>
       </c>
       <c r="AA589">
         <v>-1</v>
       </c>
       <c r="AB589">
-        <v>0.875</v>
+        <v>0</v>
       </c>
       <c r="AC589">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="590" spans="1:29">
@@ -53055,7 +53055,7 @@
         <v>589</v>
       </c>
       <c r="B591">
-        <v>4614403</v>
+        <v>4617739</v>
       </c>
       <c r="C591" t="s">
         <v>28</v>
@@ -53067,76 +53067,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F591" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G591" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H591">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I591">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J591" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K591">
+        <v>2.3</v>
+      </c>
+      <c r="L591">
+        <v>3.2</v>
+      </c>
+      <c r="M591">
         <v>3</v>
       </c>
-      <c r="L591">
-        <v>3.4</v>
-      </c>
-      <c r="M591">
-        <v>2.2</v>
-      </c>
       <c r="N591">
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="O591">
         <v>3.5</v>
       </c>
       <c r="P591">
-        <v>2.15</v>
+        <v>3.4</v>
       </c>
       <c r="Q591">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R591">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="S591">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="T591">
         <v>2.25</v>
       </c>
       <c r="U591">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="V591">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W591">
         <v>-1</v>
       </c>
       <c r="X591">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y591">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="Z591">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AA591">
-        <v>0.825</v>
+        <v>0.5</v>
       </c>
       <c r="AB591">
         <v>-0.5</v>
       </c>
       <c r="AC591">
-        <v>0.5125</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="592" spans="1:29">
@@ -53144,7 +53144,7 @@
         <v>590</v>
       </c>
       <c r="B592">
-        <v>4617739</v>
+        <v>4617490</v>
       </c>
       <c r="C592" t="s">
         <v>28</v>
@@ -53156,76 +53156,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F592" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G592" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H592">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I592">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J592" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K592">
-        <v>2.3</v>
+        <v>1.55</v>
       </c>
       <c r="L592">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="M592">
+        <v>5.5</v>
+      </c>
+      <c r="N592">
+        <v>1.4</v>
+      </c>
+      <c r="O592">
+        <v>4.75</v>
+      </c>
+      <c r="P592">
+        <v>7.5</v>
+      </c>
+      <c r="Q592">
+        <v>-1.25</v>
+      </c>
+      <c r="R592">
+        <v>1.85</v>
+      </c>
+      <c r="S592">
+        <v>1.95</v>
+      </c>
+      <c r="T592">
         <v>3</v>
       </c>
-      <c r="N592">
-        <v>2.1</v>
-      </c>
-      <c r="O592">
-        <v>3.5</v>
-      </c>
-      <c r="P592">
-        <v>3.4</v>
-      </c>
-      <c r="Q592">
-        <v>-0.25</v>
-      </c>
-      <c r="R592">
+      <c r="U592">
+        <v>2</v>
+      </c>
+      <c r="V592">
         <v>1.8</v>
       </c>
-      <c r="S592">
-        <v>2</v>
-      </c>
-      <c r="T592">
-        <v>2.25</v>
-      </c>
-      <c r="U592">
-        <v>1.8</v>
-      </c>
-      <c r="V592">
-        <v>2</v>
-      </c>
       <c r="W592">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="X592">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y592">
         <v>-1</v>
       </c>
       <c r="Z592">
-        <v>-0.5</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA592">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB592">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AC592">
-        <v>0.5</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="593" spans="1:29">
@@ -53233,7 +53233,7 @@
         <v>591</v>
       </c>
       <c r="B593">
-        <v>4617490</v>
+        <v>4614403</v>
       </c>
       <c r="C593" t="s">
         <v>28</v>
@@ -53245,76 +53245,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F593" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G593" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H593">
+        <v>0</v>
+      </c>
+      <c r="I593">
+        <v>2</v>
+      </c>
+      <c r="J593" t="s">
+        <v>53</v>
+      </c>
+      <c r="K593">
         <v>3</v>
       </c>
-      <c r="I593">
-        <v>0</v>
-      </c>
-      <c r="J593" t="s">
-        <v>52</v>
-      </c>
-      <c r="K593">
-        <v>1.55</v>
-      </c>
       <c r="L593">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="M593">
-        <v>5.5</v>
+        <v>2.2</v>
       </c>
       <c r="N593">
-        <v>1.4</v>
+        <v>3.4</v>
       </c>
       <c r="O593">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P593">
-        <v>7.5</v>
+        <v>2.15</v>
       </c>
       <c r="Q593">
-        <v>-1.25</v>
+        <v>0.25</v>
       </c>
       <c r="R593">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S593">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T593">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="U593">
-        <v>2</v>
+        <v>1.775</v>
       </c>
       <c r="V593">
-        <v>1.8</v>
+        <v>2.025</v>
       </c>
       <c r="W593">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X593">
         <v>-1</v>
       </c>
       <c r="Y593">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="Z593">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA593">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB593">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AC593">
-        <v>-0</v>
+        <v>0.5125</v>
       </c>
     </row>
     <row r="594" spans="1:29">
@@ -72101,7 +72101,7 @@
         <v>803</v>
       </c>
       <c r="B805">
-        <v>7323253</v>
+        <v>7323186</v>
       </c>
       <c r="C805" t="s">
         <v>28</v>
@@ -72113,19 +72113,19 @@
         <v>45242.83333333334</v>
       </c>
       <c r="F805" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G805" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="H805">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I805">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J805" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K805">
         <v>2</v>
@@ -72137,52 +72137,52 @@
         <v>3.5</v>
       </c>
       <c r="N805">
-        <v>2.1</v>
+        <v>1.727</v>
       </c>
       <c r="O805">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="P805">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="Q805">
+        <v>-0.75</v>
+      </c>
+      <c r="R805">
+        <v>1.9</v>
+      </c>
+      <c r="S805">
+        <v>1.9</v>
+      </c>
+      <c r="T805">
+        <v>2.75</v>
+      </c>
+      <c r="U805">
+        <v>1.85</v>
+      </c>
+      <c r="V805">
+        <v>1.95</v>
+      </c>
+      <c r="W805">
+        <v>0.7270000000000001</v>
+      </c>
+      <c r="X805">
+        <v>-1</v>
+      </c>
+      <c r="Y805">
+        <v>-1</v>
+      </c>
+      <c r="Z805">
+        <v>0.45</v>
+      </c>
+      <c r="AA805">
         <v>-0.5</v>
       </c>
-      <c r="R805">
-        <v>2.025</v>
-      </c>
-      <c r="S805">
-        <v>1.775</v>
-      </c>
-      <c r="T805">
-        <v>2.5</v>
-      </c>
-      <c r="U805">
-        <v>1.95</v>
-      </c>
-      <c r="V805">
-        <v>1.85</v>
-      </c>
-      <c r="W805">
-        <v>-1</v>
-      </c>
-      <c r="X805">
-        <v>2.5</v>
-      </c>
-      <c r="Y805">
-        <v>-1</v>
-      </c>
-      <c r="Z805">
-        <v>-1</v>
-      </c>
-      <c r="AA805">
-        <v>0.7749999999999999</v>
-      </c>
       <c r="AB805">
+        <v>-1</v>
+      </c>
+      <c r="AC805">
         <v>0.95</v>
-      </c>
-      <c r="AC805">
-        <v>-1</v>
       </c>
     </row>
     <row r="806" spans="1:29">
@@ -72190,7 +72190,7 @@
         <v>804</v>
       </c>
       <c r="B806">
-        <v>7323186</v>
+        <v>7323253</v>
       </c>
       <c r="C806" t="s">
         <v>28</v>
@@ -72202,19 +72202,19 @@
         <v>45242.83333333334</v>
       </c>
       <c r="F806" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G806" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="H806">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I806">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J806" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K806">
         <v>2</v>
@@ -72226,52 +72226,52 @@
         <v>3.5</v>
       </c>
       <c r="N806">
-        <v>1.727</v>
+        <v>2.1</v>
       </c>
       <c r="O806">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="P806">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
       <c r="Q806">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R806">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S806">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T806">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U806">
+        <v>1.95</v>
+      </c>
+      <c r="V806">
         <v>1.85</v>
       </c>
-      <c r="V806">
-        <v>1.95</v>
-      </c>
       <c r="W806">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X806">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y806">
         <v>-1</v>
       </c>
       <c r="Z806">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AA806">
-        <v>-0.5</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB806">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC806">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="807" spans="1:29">
@@ -73080,7 +73080,7 @@
         <v>814</v>
       </c>
       <c r="B816">
-        <v>6078266</v>
+        <v>6078265</v>
       </c>
       <c r="C816" t="s">
         <v>28</v>
@@ -73092,76 +73092,76 @@
         <v>45262.75</v>
       </c>
       <c r="F816" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G816" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H816">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I816">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J816" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K816">
-        <v>1.533</v>
+        <v>1.666</v>
       </c>
       <c r="L816">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M816">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N816">
-        <v>1.363</v>
+        <v>2.25</v>
       </c>
       <c r="O816">
-        <v>4.75</v>
+        <v>3.3</v>
       </c>
       <c r="P816">
-        <v>7.5</v>
+        <v>3.3</v>
       </c>
       <c r="Q816">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R816">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="S816">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="T816">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U816">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V816">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W816">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="X816">
         <v>-1</v>
       </c>
       <c r="Y816">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z816">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA816">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB816">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC816">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="817" spans="1:29">
@@ -73169,7 +73169,7 @@
         <v>815</v>
       </c>
       <c r="B817">
-        <v>6077498</v>
+        <v>6078266</v>
       </c>
       <c r="C817" t="s">
         <v>28</v>
@@ -73181,73 +73181,73 @@
         <v>45262.75</v>
       </c>
       <c r="F817" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G817" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H817">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I817">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J817" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K817">
-        <v>1.65</v>
+        <v>1.533</v>
       </c>
       <c r="L817">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="M817">
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="N817">
-        <v>1.909</v>
+        <v>1.363</v>
       </c>
       <c r="O817">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P817">
-        <v>4.2</v>
+        <v>7.5</v>
       </c>
       <c r="Q817">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="R817">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="S817">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="T817">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U817">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V817">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W817">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="X817">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y817">
         <v>-1</v>
       </c>
       <c r="Z817">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA817">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB817">
-        <v>1.025</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC817">
         <v>-1</v>
@@ -73258,7 +73258,7 @@
         <v>816</v>
       </c>
       <c r="B818">
-        <v>6078265</v>
+        <v>6077498</v>
       </c>
       <c r="C818" t="s">
         <v>28</v>
@@ -73270,76 +73270,76 @@
         <v>45262.75</v>
       </c>
       <c r="F818" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G818" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H818">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I818">
         <v>2</v>
       </c>
       <c r="J818" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K818">
-        <v>1.666</v>
+        <v>1.65</v>
       </c>
       <c r="L818">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="M818">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="N818">
-        <v>2.25</v>
+        <v>1.909</v>
       </c>
       <c r="O818">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="P818">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="Q818">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R818">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="S818">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="T818">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U818">
-        <v>1.8</v>
+        <v>2.025</v>
       </c>
       <c r="V818">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W818">
         <v>-1</v>
       </c>
       <c r="X818">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y818">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z818">
         <v>-1</v>
       </c>
       <c r="AA818">
-        <v>0.8500000000000001</v>
+        <v>1</v>
       </c>
       <c r="AB818">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC818">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="819" spans="1:29">
@@ -73703,7 +73703,7 @@
         <v>821</v>
       </c>
       <c r="B823">
-        <v>6143704</v>
+        <v>6078997</v>
       </c>
       <c r="C823" t="s">
         <v>28</v>
@@ -73715,67 +73715,67 @@
         <v>45268.75</v>
       </c>
       <c r="F823" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G823" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H823">
+        <v>1</v>
+      </c>
+      <c r="I823">
         <v>0</v>
       </c>
-      <c r="I823">
-        <v>1</v>
-      </c>
       <c r="J823" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K823">
-        <v>6.5</v>
+        <v>3.8</v>
       </c>
       <c r="L823">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="M823">
-        <v>1.4</v>
+        <v>1.909</v>
       </c>
       <c r="N823">
-        <v>12</v>
+        <v>2.7</v>
       </c>
       <c r="O823">
-        <v>8.5</v>
+        <v>3.6</v>
       </c>
       <c r="P823">
-        <v>1.166</v>
+        <v>2.45</v>
       </c>
       <c r="Q823">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R823">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S823">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T823">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U823">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V823">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W823">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="X823">
         <v>-1</v>
       </c>
       <c r="Y823">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z823">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA823">
         <v>-1</v>
@@ -73784,7 +73784,7 @@
         <v>-1</v>
       </c>
       <c r="AC823">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="824" spans="1:29">
@@ -73792,7 +73792,7 @@
         <v>822</v>
       </c>
       <c r="B824">
-        <v>6078997</v>
+        <v>6078267</v>
       </c>
       <c r="C824" t="s">
         <v>28</v>
@@ -73804,13 +73804,13 @@
         <v>45268.75</v>
       </c>
       <c r="F824" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G824" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H824">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I824">
         <v>0</v>
@@ -73819,28 +73819,28 @@
         <v>52</v>
       </c>
       <c r="K824">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="L824">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="M824">
-        <v>1.909</v>
+        <v>6</v>
       </c>
       <c r="N824">
-        <v>2.7</v>
+        <v>1.444</v>
       </c>
       <c r="O824">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P824">
-        <v>2.45</v>
+        <v>7</v>
       </c>
       <c r="Q824">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="R824">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="S824">
         <v>1.825</v>
@@ -73849,13 +73849,13 @@
         <v>2.75</v>
       </c>
       <c r="U824">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="V824">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="W824">
-        <v>1.7</v>
+        <v>0.444</v>
       </c>
       <c r="X824">
         <v>-1</v>
@@ -73864,7 +73864,7 @@
         <v>-1</v>
       </c>
       <c r="Z824">
-        <v>0.9750000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AA824">
         <v>-1</v>
@@ -73873,7 +73873,7 @@
         <v>-1</v>
       </c>
       <c r="AC824">
-        <v>1.025</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="825" spans="1:29">
@@ -73881,7 +73881,7 @@
         <v>823</v>
       </c>
       <c r="B825">
-        <v>6078267</v>
+        <v>6143704</v>
       </c>
       <c r="C825" t="s">
         <v>28</v>
@@ -73893,67 +73893,67 @@
         <v>45268.75</v>
       </c>
       <c r="F825" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G825" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H825">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I825">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J825" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K825">
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="L825">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="M825">
-        <v>6</v>
+        <v>1.4</v>
       </c>
       <c r="N825">
-        <v>1.444</v>
+        <v>12</v>
       </c>
       <c r="O825">
-        <v>4.75</v>
+        <v>8.5</v>
       </c>
       <c r="P825">
-        <v>7</v>
+        <v>1.166</v>
       </c>
       <c r="Q825">
-        <v>-1.25</v>
+        <v>2</v>
       </c>
       <c r="R825">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="S825">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T825">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U825">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="V825">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W825">
-        <v>0.444</v>
+        <v>-1</v>
       </c>
       <c r="X825">
         <v>-1</v>
       </c>
       <c r="Y825">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="Z825">
-        <v>1.025</v>
+        <v>1</v>
       </c>
       <c r="AA825">
         <v>-1</v>
@@ -73962,7 +73962,7 @@
         <v>-1</v>
       </c>
       <c r="AC825">
-        <v>1.05</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="826" spans="1:29">
@@ -73970,7 +73970,7 @@
         <v>824</v>
       </c>
       <c r="B826">
-        <v>6078269</v>
+        <v>6078998</v>
       </c>
       <c r="C826" t="s">
         <v>28</v>
@@ -73982,73 +73982,73 @@
         <v>45269.75</v>
       </c>
       <c r="F826" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G826" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H826">
+        <v>2</v>
+      </c>
+      <c r="I826">
         <v>3</v>
       </c>
-      <c r="I826">
-        <v>1</v>
-      </c>
       <c r="J826" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K826">
+        <v>1.909</v>
+      </c>
+      <c r="L826">
+        <v>3.6</v>
+      </c>
+      <c r="M826">
+        <v>3.8</v>
+      </c>
+      <c r="N826">
+        <v>2.15</v>
+      </c>
+      <c r="O826">
+        <v>3.75</v>
+      </c>
+      <c r="P826">
+        <v>3.1</v>
+      </c>
+      <c r="Q826">
+        <v>-0.25</v>
+      </c>
+      <c r="R826">
         <v>1.85</v>
       </c>
-      <c r="L826">
-        <v>3.4</v>
-      </c>
-      <c r="M826">
-        <v>4.333</v>
-      </c>
-      <c r="N826">
-        <v>1.8</v>
-      </c>
-      <c r="O826">
-        <v>3.6</v>
-      </c>
-      <c r="P826">
-        <v>4.5</v>
-      </c>
-      <c r="Q826">
-        <v>-0.75</v>
-      </c>
-      <c r="R826">
-        <v>1.925</v>
-      </c>
       <c r="S826">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T826">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U826">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V826">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W826">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="X826">
         <v>-1</v>
       </c>
       <c r="Y826">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="Z826">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA826">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB826">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC826">
         <v>-1</v>
@@ -74059,7 +74059,7 @@
         <v>825</v>
       </c>
       <c r="B827">
-        <v>6078998</v>
+        <v>6077499</v>
       </c>
       <c r="C827" t="s">
         <v>28</v>
@@ -74071,76 +74071,76 @@
         <v>45269.75</v>
       </c>
       <c r="F827" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G827" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="H827">
         <v>2</v>
       </c>
       <c r="I827">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J827" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K827">
-        <v>1.909</v>
+        <v>2.1</v>
       </c>
       <c r="L827">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M827">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N827">
-        <v>2.15</v>
+        <v>2.9</v>
       </c>
       <c r="O827">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P827">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="Q827">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R827">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="S827">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="T827">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U827">
         <v>1.85</v>
       </c>
       <c r="V827">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W827">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="X827">
         <v>-1</v>
       </c>
       <c r="Y827">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z827">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA827">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB827">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC827">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="828" spans="1:29">
@@ -74148,7 +74148,7 @@
         <v>826</v>
       </c>
       <c r="B828">
-        <v>6077499</v>
+        <v>6077768</v>
       </c>
       <c r="C828" t="s">
         <v>28</v>
@@ -74160,76 +74160,76 @@
         <v>45269.75</v>
       </c>
       <c r="F828" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G828" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H828">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I828">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J828" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K828">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="L828">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M828">
         <v>3.4</v>
       </c>
       <c r="N828">
-        <v>2.9</v>
+        <v>2.05</v>
       </c>
       <c r="O828">
+        <v>3.6</v>
+      </c>
+      <c r="P828">
         <v>3.4</v>
       </c>
-      <c r="P828">
-        <v>2.4</v>
-      </c>
       <c r="Q828">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R828">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="S828">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="T828">
         <v>2.75</v>
       </c>
       <c r="U828">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V828">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W828">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="X828">
         <v>-1</v>
       </c>
       <c r="Y828">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z828">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA828">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB828">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AC828">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="829" spans="1:29">
@@ -74237,7 +74237,7 @@
         <v>827</v>
       </c>
       <c r="B829">
-        <v>6078268</v>
+        <v>6078269</v>
       </c>
       <c r="C829" t="s">
         <v>28</v>
@@ -74249,76 +74249,76 @@
         <v>45269.75</v>
       </c>
       <c r="F829" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G829" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="H829">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I829">
         <v>1</v>
       </c>
       <c r="J829" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K829">
-        <v>3.1</v>
+        <v>1.85</v>
       </c>
       <c r="L829">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="M829">
-        <v>2.3</v>
+        <v>4.333</v>
       </c>
       <c r="N829">
-        <v>2.9</v>
+        <v>1.8</v>
       </c>
       <c r="O829">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="P829">
-        <v>2.375</v>
+        <v>4.5</v>
       </c>
       <c r="Q829">
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R829">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S829">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="T829">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U829">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V829">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="W829">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X829">
         <v>-1</v>
       </c>
       <c r="Y829">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Z829">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA829">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB829">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC829">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="830" spans="1:29">
@@ -74326,7 +74326,7 @@
         <v>828</v>
       </c>
       <c r="B830">
-        <v>6077768</v>
+        <v>6078268</v>
       </c>
       <c r="C830" t="s">
         <v>28</v>
@@ -74338,40 +74338,40 @@
         <v>45269.75</v>
       </c>
       <c r="F830" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G830" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H830">
         <v>0</v>
       </c>
       <c r="I830">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J830" t="s">
         <v>53</v>
       </c>
       <c r="K830">
-        <v>2.05</v>
+        <v>3.1</v>
       </c>
       <c r="L830">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M830">
+        <v>2.3</v>
+      </c>
+      <c r="N830">
+        <v>2.9</v>
+      </c>
+      <c r="O830">
         <v>3.4</v>
       </c>
-      <c r="N830">
-        <v>2.05</v>
-      </c>
-      <c r="O830">
-        <v>3.6</v>
-      </c>
       <c r="P830">
-        <v>3.4</v>
+        <v>2.375</v>
       </c>
       <c r="Q830">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R830">
         <v>1.8</v>
@@ -74383,10 +74383,10 @@
         <v>2.75</v>
       </c>
       <c r="U830">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="V830">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="W830">
         <v>-1</v>
@@ -74395,7 +74395,7 @@
         <v>-1</v>
       </c>
       <c r="Y830">
-        <v>2.4</v>
+        <v>1.375</v>
       </c>
       <c r="Z830">
         <v>-1</v>
@@ -74404,10 +74404,10 @@
         <v>1</v>
       </c>
       <c r="AB830">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AC830">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-28 às 23-11
</commit_message>
<xml_diff>
--- a/Chile Primera Division/Chile Primera Division.xlsx
+++ b/Chile Primera Division/Chile Primera Division.xlsx
@@ -6597,7 +6597,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>3200931</v>
+        <v>3201280</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6609,61 +6609,61 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F69" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G69" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" t="s">
         <v>51</v>
       </c>
       <c r="K69">
-        <v>2.2</v>
+        <v>1.833</v>
       </c>
       <c r="L69">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="M69">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="N69">
         <v>2</v>
       </c>
       <c r="O69">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P69">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="Q69">
         <v>-0.25</v>
       </c>
       <c r="R69">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S69">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="T69">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U69">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="V69">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="W69">
         <v>-1</v>
       </c>
       <c r="X69">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="Y69">
         <v>-1</v>
@@ -6672,13 +6672,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA69">
-        <v>0.5</v>
+        <v>0.475</v>
       </c>
       <c r="AB69">
         <v>-1</v>
       </c>
       <c r="AC69">
-        <v>0.95</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -6775,7 +6775,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>3201280</v>
+        <v>3201281</v>
       </c>
       <c r="C71" t="s">
         <v>28</v>
@@ -6787,76 +6787,76 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F71" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G71" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J71" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K71">
-        <v>1.833</v>
+        <v>3</v>
       </c>
       <c r="L71">
-        <v>3.75</v>
+        <v>3.2</v>
       </c>
       <c r="M71">
-        <v>4</v>
+        <v>2.375</v>
       </c>
       <c r="N71">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="O71">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="P71">
-        <v>3.5</v>
+        <v>2.15</v>
       </c>
       <c r="Q71">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R71">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S71">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T71">
+        <v>2.25</v>
+      </c>
+      <c r="U71">
+        <v>1.8</v>
+      </c>
+      <c r="V71">
+        <v>2</v>
+      </c>
+      <c r="W71">
         <v>2.5</v>
       </c>
-      <c r="U71">
-        <v>1.825</v>
-      </c>
-      <c r="V71">
-        <v>1.975</v>
-      </c>
-      <c r="W71">
-        <v>-1</v>
-      </c>
       <c r="X71">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y71">
         <v>-1</v>
       </c>
       <c r="Z71">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AA71">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB71">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC71">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="72" spans="1:29">
@@ -6864,7 +6864,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>3201281</v>
+        <v>3200931</v>
       </c>
       <c r="C72" t="s">
         <v>28</v>
@@ -6876,76 +6876,76 @@
         <v>44238.77083333334</v>
       </c>
       <c r="F72" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G72" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H72">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I72">
         <v>0</v>
       </c>
       <c r="J72" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K72">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="L72">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="M72">
-        <v>2.375</v>
+        <v>3.3</v>
       </c>
       <c r="N72">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="O72">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="P72">
-        <v>2.15</v>
+        <v>3.6</v>
       </c>
       <c r="Q72">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R72">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S72">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="T72">
         <v>2.25</v>
       </c>
       <c r="U72">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="V72">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W72">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="X72">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y72">
         <v>-1</v>
       </c>
       <c r="Z72">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AA72">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="AB72">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC72">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="73" spans="1:29">
@@ -7398,7 +7398,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>3234976</v>
+        <v>3234178</v>
       </c>
       <c r="C78" t="s">
         <v>28</v>
@@ -7410,76 +7410,76 @@
         <v>44241.75</v>
       </c>
       <c r="F78" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G78" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I78">
         <v>2</v>
       </c>
       <c r="J78" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K78">
-        <v>1.363</v>
+        <v>2.2</v>
       </c>
       <c r="L78">
-        <v>4.75</v>
+        <v>3.25</v>
       </c>
       <c r="M78">
-        <v>8</v>
+        <v>3.25</v>
       </c>
       <c r="N78">
-        <v>1.4</v>
+        <v>2.05</v>
       </c>
       <c r="O78">
-        <v>4.333</v>
+        <v>3.3</v>
       </c>
       <c r="P78">
-        <v>6.5</v>
+        <v>3.6</v>
       </c>
       <c r="Q78">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R78">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="S78">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="T78">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U78">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="V78">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W78">
         <v>-1</v>
       </c>
       <c r="X78">
-        <v>3.333</v>
+        <v>-1</v>
       </c>
       <c r="Y78">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Z78">
         <v>-1</v>
       </c>
       <c r="AA78">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AB78">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC78">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="79" spans="1:29">
@@ -7487,7 +7487,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>3234175</v>
+        <v>3234976</v>
       </c>
       <c r="C79" t="s">
         <v>28</v>
@@ -7499,76 +7499,76 @@
         <v>44241.75</v>
       </c>
       <c r="F79" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G79" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H79">
         <v>2</v>
       </c>
       <c r="I79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J79" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K79">
-        <v>2.8</v>
+        <v>1.363</v>
       </c>
       <c r="L79">
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
       <c r="M79">
-        <v>2.5</v>
+        <v>8</v>
       </c>
       <c r="N79">
-        <v>3.2</v>
+        <v>1.4</v>
       </c>
       <c r="O79">
-        <v>3.5</v>
+        <v>4.333</v>
       </c>
       <c r="P79">
-        <v>2.15</v>
+        <v>6.5</v>
       </c>
       <c r="Q79">
-        <v>0.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R79">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="S79">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="T79">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U79">
-        <v>1.775</v>
+        <v>1.825</v>
       </c>
       <c r="V79">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="W79">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="X79">
-        <v>-1</v>
+        <v>3.333</v>
       </c>
       <c r="Y79">
         <v>-1</v>
       </c>
       <c r="Z79">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA79">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB79">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC79">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="80" spans="1:29">
@@ -7665,7 +7665,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>3234178</v>
+        <v>3234175</v>
       </c>
       <c r="C81" t="s">
         <v>28</v>
@@ -7677,76 +7677,76 @@
         <v>44241.75</v>
       </c>
       <c r="F81" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G81" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H81">
+        <v>2</v>
+      </c>
+      <c r="I81">
         <v>0</v>
       </c>
-      <c r="I81">
-        <v>2</v>
-      </c>
       <c r="J81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K81">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="L81">
         <v>3.25</v>
       </c>
       <c r="M81">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="N81">
-        <v>2.05</v>
+        <v>3.2</v>
       </c>
       <c r="O81">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="P81">
-        <v>3.6</v>
+        <v>2.15</v>
       </c>
       <c r="Q81">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R81">
+        <v>1.95</v>
+      </c>
+      <c r="S81">
         <v>1.85</v>
       </c>
-      <c r="S81">
-        <v>1.95</v>
-      </c>
       <c r="T81">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U81">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V81">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W81">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="X81">
         <v>-1</v>
       </c>
       <c r="Y81">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z81">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA81">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB81">
         <v>-1</v>
       </c>
       <c r="AC81">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="82" spans="1:29">
@@ -30716,7 +30716,7 @@
         <v>338</v>
       </c>
       <c r="B340">
-        <v>3899770</v>
+        <v>3899769</v>
       </c>
       <c r="C340" t="s">
         <v>28</v>
@@ -30728,76 +30728,76 @@
         <v>44527.75</v>
       </c>
       <c r="F340" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="G340" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H340">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I340">
         <v>0</v>
       </c>
       <c r="J340" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K340">
-        <v>2.2</v>
+        <v>2.15</v>
       </c>
       <c r="L340">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="M340">
         <v>3.1</v>
       </c>
       <c r="N340">
-        <v>2.55</v>
+        <v>1.95</v>
       </c>
       <c r="O340">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="P340">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="Q340">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R340">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="S340">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="T340">
         <v>2.25</v>
       </c>
       <c r="U340">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V340">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W340">
-        <v>1.55</v>
+        <v>-1</v>
       </c>
       <c r="X340">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y340">
         <v>-1</v>
       </c>
       <c r="Z340">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
       <c r="AA340">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AB340">
         <v>-1</v>
       </c>
       <c r="AC340">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="341" spans="1:29">
@@ -30805,7 +30805,7 @@
         <v>339</v>
       </c>
       <c r="B341">
-        <v>3899769</v>
+        <v>3899770</v>
       </c>
       <c r="C341" t="s">
         <v>28</v>
@@ -30817,76 +30817,76 @@
         <v>44527.75</v>
       </c>
       <c r="F341" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G341" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H341">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I341">
         <v>0</v>
       </c>
       <c r="J341" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K341">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="L341">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="M341">
         <v>3.1</v>
       </c>
       <c r="N341">
-        <v>1.95</v>
+        <v>2.55</v>
       </c>
       <c r="O341">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="P341">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="Q341">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R341">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="S341">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="T341">
         <v>2.25</v>
       </c>
       <c r="U341">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V341">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W341">
-        <v>-1</v>
+        <v>1.55</v>
       </c>
       <c r="X341">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y341">
         <v>-1</v>
       </c>
       <c r="Z341">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
       <c r="AA341">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AB341">
         <v>-1</v>
       </c>
       <c r="AC341">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="342" spans="1:29">
@@ -31161,7 +31161,7 @@
         <v>343</v>
       </c>
       <c r="B345">
-        <v>3899772</v>
+        <v>3898955</v>
       </c>
       <c r="C345" t="s">
         <v>28</v>
@@ -31173,76 +31173,76 @@
         <v>44528.75</v>
       </c>
       <c r="F345" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G345" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H345">
+        <v>2</v>
+      </c>
+      <c r="I345">
         <v>0</v>
       </c>
-      <c r="I345">
-        <v>1</v>
-      </c>
       <c r="J345" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K345">
-        <v>1.363</v>
+        <v>1.5</v>
       </c>
       <c r="L345">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="M345">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="N345">
-        <v>1.3</v>
+        <v>1.65</v>
       </c>
       <c r="O345">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="P345">
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="Q345">
-        <v>-1.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R345">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="S345">
-        <v>1.975</v>
+        <v>1.875</v>
       </c>
       <c r="T345">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U345">
+        <v>2</v>
+      </c>
+      <c r="V345">
         <v>1.8</v>
       </c>
-      <c r="V345">
-        <v>2</v>
-      </c>
       <c r="W345">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="X345">
         <v>-1</v>
       </c>
       <c r="Y345">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="Z345">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA345">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB345">
         <v>-1</v>
       </c>
       <c r="AC345">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="346" spans="1:29">
@@ -31339,7 +31339,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>3898955</v>
+        <v>3899772</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31351,76 +31351,76 @@
         <v>44528.75</v>
       </c>
       <c r="F347" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G347" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H347">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I347">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J347" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K347">
-        <v>1.5</v>
+        <v>1.363</v>
       </c>
       <c r="L347">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="M347">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="N347">
-        <v>1.65</v>
+        <v>1.3</v>
       </c>
       <c r="O347">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="P347">
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="Q347">
-        <v>-0.75</v>
+        <v>-1.5</v>
       </c>
       <c r="R347">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="S347">
-        <v>1.875</v>
+        <v>1.975</v>
       </c>
       <c r="T347">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U347">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="V347">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="W347">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X347">
         <v>-1</v>
       </c>
       <c r="Y347">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="Z347">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA347">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB347">
         <v>-1</v>
       </c>
       <c r="AC347">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="348" spans="1:29">
@@ -31428,7 +31428,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>3899778</v>
+        <v>3899776</v>
       </c>
       <c r="C348" t="s">
         <v>28</v>
@@ -31440,49 +31440,49 @@
         <v>44534.75</v>
       </c>
       <c r="F348" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G348" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H348">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I348">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J348" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K348">
-        <v>2.05</v>
+        <v>1.666</v>
       </c>
       <c r="L348">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M348">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="N348">
-        <v>2</v>
+        <v>1.333</v>
       </c>
       <c r="O348">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P348">
-        <v>3.6</v>
+        <v>9.5</v>
       </c>
       <c r="Q348">
-        <v>-0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R348">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="S348">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="T348">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U348">
         <v>1.85</v>
@@ -31494,22 +31494,22 @@
         <v>-1</v>
       </c>
       <c r="X348">
-        <v>-1</v>
+        <v>3.75</v>
       </c>
       <c r="Y348">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z348">
         <v>-1</v>
       </c>
       <c r="AA348">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AB348">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC348">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="349" spans="1:29">
@@ -31695,7 +31695,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>3899776</v>
+        <v>3899778</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31707,49 +31707,49 @@
         <v>44534.75</v>
       </c>
       <c r="F351" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G351" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H351">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I351">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J351" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K351">
-        <v>1.666</v>
+        <v>2.05</v>
       </c>
       <c r="L351">
+        <v>3.4</v>
+      </c>
+      <c r="M351">
+        <v>3.1</v>
+      </c>
+      <c r="N351">
+        <v>2</v>
+      </c>
+      <c r="O351">
         <v>3.6</v>
       </c>
-      <c r="M351">
-        <v>4.5</v>
-      </c>
-      <c r="N351">
-        <v>1.333</v>
-      </c>
-      <c r="O351">
-        <v>4.75</v>
-      </c>
       <c r="P351">
-        <v>9.5</v>
+        <v>3.6</v>
       </c>
       <c r="Q351">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R351">
+        <v>2</v>
+      </c>
+      <c r="S351">
         <v>1.8</v>
       </c>
-      <c r="S351">
-        <v>2</v>
-      </c>
       <c r="T351">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U351">
         <v>1.85</v>
@@ -31761,22 +31761,22 @@
         <v>-1</v>
       </c>
       <c r="X351">
-        <v>3.75</v>
+        <v>-1</v>
       </c>
       <c r="Y351">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Z351">
         <v>-1</v>
       </c>
       <c r="AA351">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AB351">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC351">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="352" spans="1:29">
@@ -31784,7 +31784,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>3899777</v>
+        <v>3898958</v>
       </c>
       <c r="C352" t="s">
         <v>28</v>
@@ -31796,76 +31796,76 @@
         <v>44535.75</v>
       </c>
       <c r="F352" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G352" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H352">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I352">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J352" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K352">
+        <v>2.1</v>
+      </c>
+      <c r="L352">
+        <v>3.3</v>
+      </c>
+      <c r="M352">
+        <v>3.1</v>
+      </c>
+      <c r="N352">
+        <v>2.1</v>
+      </c>
+      <c r="O352">
+        <v>3.6</v>
+      </c>
+      <c r="P352">
+        <v>3.4</v>
+      </c>
+      <c r="Q352">
+        <v>-0.25</v>
+      </c>
+      <c r="R352">
+        <v>1.775</v>
+      </c>
+      <c r="S352">
+        <v>2.025</v>
+      </c>
+      <c r="T352">
         <v>2.25</v>
       </c>
-      <c r="L352">
-        <v>3.1</v>
-      </c>
-      <c r="M352">
-        <v>3</v>
-      </c>
-      <c r="N352">
-        <v>2.75</v>
-      </c>
-      <c r="O352">
-        <v>2.75</v>
-      </c>
-      <c r="P352">
-        <v>2.7</v>
-      </c>
-      <c r="Q352">
-        <v>0</v>
-      </c>
-      <c r="R352">
-        <v>1.9</v>
-      </c>
-      <c r="S352">
-        <v>1.9</v>
-      </c>
-      <c r="T352">
-        <v>2</v>
-      </c>
       <c r="U352">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V352">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W352">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="X352">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y352">
         <v>-1</v>
       </c>
       <c r="Z352">
-        <v>0</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA352">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB352">
-        <v>0</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AC352">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="353" spans="1:29">
@@ -31962,7 +31962,7 @@
         <v>352</v>
       </c>
       <c r="B354">
-        <v>3898958</v>
+        <v>3899777</v>
       </c>
       <c r="C354" t="s">
         <v>28</v>
@@ -31974,76 +31974,76 @@
         <v>44535.75</v>
       </c>
       <c r="F354" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G354" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H354">
+        <v>1</v>
+      </c>
+      <c r="I354">
+        <v>1</v>
+      </c>
+      <c r="J354" t="s">
+        <v>51</v>
+      </c>
+      <c r="K354">
+        <v>2.25</v>
+      </c>
+      <c r="L354">
+        <v>3.1</v>
+      </c>
+      <c r="M354">
         <v>3</v>
       </c>
-      <c r="I354">
-        <v>2</v>
-      </c>
-      <c r="J354" t="s">
-        <v>52</v>
-      </c>
-      <c r="K354">
-        <v>2.1</v>
-      </c>
-      <c r="L354">
-        <v>3.3</v>
-      </c>
-      <c r="M354">
-        <v>3.1</v>
-      </c>
       <c r="N354">
-        <v>2.1</v>
+        <v>2.75</v>
       </c>
       <c r="O354">
-        <v>3.6</v>
+        <v>2.75</v>
       </c>
       <c r="P354">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="Q354">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R354">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="S354">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="T354">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="U354">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="V354">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W354">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="X354">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y354">
         <v>-1</v>
       </c>
       <c r="Z354">
-        <v>0.7749999999999999</v>
+        <v>0</v>
       </c>
       <c r="AA354">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB354">
-        <v>0.7749999999999999</v>
+        <v>0</v>
       </c>
       <c r="AC354">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="355" spans="1:29">
@@ -41485,7 +41485,7 @@
         <v>459</v>
       </c>
       <c r="B461">
-        <v>5034214</v>
+        <v>4614316</v>
       </c>
       <c r="C461" t="s">
         <v>28</v>
@@ -41497,73 +41497,73 @@
         <v>44702.66666666666</v>
       </c>
       <c r="F461" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G461" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H461">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I461">
         <v>2</v>
       </c>
       <c r="J461" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K461">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="L461">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="M461">
         <v>2.45</v>
       </c>
       <c r="N461">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="O461">
         <v>3.1</v>
       </c>
       <c r="P461">
-        <v>2.9</v>
+        <v>2.45</v>
       </c>
       <c r="Q461">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R461">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="S461">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T461">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="U461">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="V461">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="W461">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="X461">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Y461">
         <v>-1</v>
       </c>
       <c r="Z461">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AA461">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB461">
-        <v>0.825</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC461">
         <v>-1</v>
@@ -41574,7 +41574,7 @@
         <v>460</v>
       </c>
       <c r="B462">
-        <v>4614316</v>
+        <v>5034214</v>
       </c>
       <c r="C462" t="s">
         <v>28</v>
@@ -41586,73 +41586,73 @@
         <v>44702.66666666666</v>
       </c>
       <c r="F462" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G462" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H462">
+        <v>2</v>
+      </c>
+      <c r="I462">
+        <v>2</v>
+      </c>
+      <c r="J462" t="s">
+        <v>51</v>
+      </c>
+      <c r="K462">
         <v>3</v>
       </c>
-      <c r="I462">
-        <v>2</v>
-      </c>
-      <c r="J462" t="s">
-        <v>52</v>
-      </c>
-      <c r="K462">
-        <v>3.1</v>
-      </c>
       <c r="L462">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="M462">
         <v>2.45</v>
       </c>
       <c r="N462">
-        <v>3.1</v>
+        <v>2.6</v>
       </c>
       <c r="O462">
         <v>3.1</v>
       </c>
       <c r="P462">
-        <v>2.45</v>
+        <v>2.9</v>
       </c>
       <c r="Q462">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R462">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="S462">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T462">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="U462">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="V462">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="W462">
+        <v>-1</v>
+      </c>
+      <c r="X462">
         <v>2.1</v>
       </c>
-      <c r="X462">
-        <v>-1</v>
-      </c>
       <c r="Y462">
         <v>-1</v>
       </c>
       <c r="Z462">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AA462">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB462">
-        <v>0.8500000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AC462">
         <v>-1</v>
@@ -51542,7 +51542,7 @@
         <v>572</v>
       </c>
       <c r="B574">
-        <v>4614399</v>
+        <v>4617486</v>
       </c>
       <c r="C574" t="s">
         <v>28</v>
@@ -51554,40 +51554,40 @@
         <v>44857.625</v>
       </c>
       <c r="F574" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G574" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H574">
+        <v>2</v>
+      </c>
+      <c r="I574">
         <v>0</v>
       </c>
-      <c r="I574">
-        <v>2</v>
-      </c>
       <c r="J574" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K574">
-        <v>5.25</v>
+        <v>2.1</v>
       </c>
       <c r="L574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M574">
-        <v>1.615</v>
+        <v>3.25</v>
       </c>
       <c r="N574">
-        <v>5</v>
+        <v>1.909</v>
       </c>
       <c r="O574">
         <v>3.8</v>
       </c>
       <c r="P574">
-        <v>1.7</v>
+        <v>3.75</v>
       </c>
       <c r="Q574">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R574">
         <v>1.925</v>
@@ -51596,34 +51596,34 @@
         <v>1.925</v>
       </c>
       <c r="T574">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U574">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V574">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W574">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X574">
         <v>-1</v>
       </c>
       <c r="Y574">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Z574">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA574">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AB574">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC574">
-        <v>0.4125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="575" spans="1:29">
@@ -51631,7 +51631,7 @@
         <v>573</v>
       </c>
       <c r="B575">
-        <v>4617486</v>
+        <v>4614399</v>
       </c>
       <c r="C575" t="s">
         <v>28</v>
@@ -51643,40 +51643,40 @@
         <v>44857.625</v>
       </c>
       <c r="F575" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G575" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H575">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I575">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J575" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K575">
-        <v>2.1</v>
+        <v>5.25</v>
       </c>
       <c r="L575">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M575">
-        <v>3.25</v>
+        <v>1.615</v>
       </c>
       <c r="N575">
-        <v>1.909</v>
+        <v>5</v>
       </c>
       <c r="O575">
         <v>3.8</v>
       </c>
       <c r="P575">
-        <v>3.75</v>
+        <v>1.7</v>
       </c>
       <c r="Q575">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R575">
         <v>1.925</v>
@@ -51685,34 +51685,34 @@
         <v>1.925</v>
       </c>
       <c r="T575">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U575">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="V575">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W575">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X575">
         <v>-1</v>
       </c>
       <c r="Y575">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="Z575">
+        <v>-1</v>
+      </c>
+      <c r="AA575">
         <v>0.925</v>
       </c>
-      <c r="AA575">
-        <v>-1</v>
-      </c>
       <c r="AB575">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AC575">
-        <v>1</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="576" spans="1:29">
@@ -52165,7 +52165,7 @@
         <v>579</v>
       </c>
       <c r="B581">
-        <v>4653847</v>
+        <v>4617488</v>
       </c>
       <c r="C581" t="s">
         <v>28</v>
@@ -52177,58 +52177,58 @@
         <v>44864.625</v>
       </c>
       <c r="F581" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G581" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H581">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I581">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J581" t="s">
         <v>52</v>
       </c>
       <c r="K581">
-        <v>1.666</v>
+        <v>3.4</v>
       </c>
       <c r="L581">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M581">
+        <v>2</v>
+      </c>
+      <c r="N581">
         <v>4.75</v>
       </c>
-      <c r="N581">
-        <v>1.615</v>
-      </c>
       <c r="O581">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P581">
-        <v>5.5</v>
+        <v>1.727</v>
       </c>
       <c r="Q581">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="R581">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="S581">
-        <v>1.775</v>
+        <v>1.95</v>
       </c>
       <c r="T581">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U581">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V581">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="W581">
-        <v>0.615</v>
+        <v>3.75</v>
       </c>
       <c r="X581">
         <v>-1</v>
@@ -52237,16 +52237,16 @@
         <v>-1</v>
       </c>
       <c r="Z581">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA581">
         <v>-1</v>
       </c>
       <c r="AB581">
-        <v>0.95</v>
+        <v>0.4625</v>
       </c>
       <c r="AC581">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="582" spans="1:29">
@@ -52343,7 +52343,7 @@
         <v>581</v>
       </c>
       <c r="B583">
-        <v>4617488</v>
+        <v>4653847</v>
       </c>
       <c r="C583" t="s">
         <v>28</v>
@@ -52355,58 +52355,58 @@
         <v>44864.625</v>
       </c>
       <c r="F583" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G583" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H583">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I583">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J583" t="s">
         <v>52</v>
       </c>
       <c r="K583">
-        <v>3.4</v>
+        <v>1.666</v>
       </c>
       <c r="L583">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M583">
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="N583">
-        <v>4.75</v>
+        <v>1.615</v>
       </c>
       <c r="O583">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P583">
-        <v>1.727</v>
+        <v>5.5</v>
       </c>
       <c r="Q583">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="R583">
+        <v>2.025</v>
+      </c>
+      <c r="S583">
+        <v>1.775</v>
+      </c>
+      <c r="T583">
+        <v>2.5</v>
+      </c>
+      <c r="U583">
+        <v>1.95</v>
+      </c>
+      <c r="V583">
         <v>1.85</v>
       </c>
-      <c r="S583">
-        <v>1.95</v>
-      </c>
-      <c r="T583">
-        <v>2.75</v>
-      </c>
-      <c r="U583">
-        <v>1.925</v>
-      </c>
-      <c r="V583">
-        <v>1.875</v>
-      </c>
       <c r="W583">
-        <v>3.75</v>
+        <v>0.615</v>
       </c>
       <c r="X583">
         <v>-1</v>
@@ -52415,16 +52415,16 @@
         <v>-1</v>
       </c>
       <c r="Z583">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AA583">
         <v>-1</v>
       </c>
       <c r="AB583">
-        <v>0.4625</v>
+        <v>0.95</v>
       </c>
       <c r="AC583">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="584" spans="1:29">
@@ -52699,7 +52699,7 @@
         <v>585</v>
       </c>
       <c r="B587">
-        <v>4614405</v>
+        <v>4617491</v>
       </c>
       <c r="C587" t="s">
         <v>28</v>
@@ -52711,73 +52711,73 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F587" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G587" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H587">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I587">
+        <v>4</v>
+      </c>
+      <c r="J587" t="s">
+        <v>53</v>
+      </c>
+      <c r="K587">
+        <v>2.7</v>
+      </c>
+      <c r="L587">
+        <v>3.3</v>
+      </c>
+      <c r="M587">
+        <v>2.45</v>
+      </c>
+      <c r="N587">
+        <v>2.7</v>
+      </c>
+      <c r="O587">
+        <v>3.4</v>
+      </c>
+      <c r="P587">
+        <v>2.6</v>
+      </c>
+      <c r="Q587">
         <v>0</v>
       </c>
-      <c r="J587" t="s">
-        <v>52</v>
-      </c>
-      <c r="K587">
-        <v>1.75</v>
-      </c>
-      <c r="L587">
-        <v>3.5</v>
-      </c>
-      <c r="M587">
-        <v>4.333</v>
-      </c>
-      <c r="N587">
-        <v>1.833</v>
-      </c>
-      <c r="O587">
-        <v>3.5</v>
-      </c>
-      <c r="P587">
-        <v>4.5</v>
-      </c>
-      <c r="Q587">
-        <v>-0.5</v>
-      </c>
       <c r="R587">
+        <v>2</v>
+      </c>
+      <c r="S587">
         <v>1.8</v>
-      </c>
-      <c r="S587">
-        <v>2</v>
       </c>
       <c r="T587">
         <v>2.5</v>
       </c>
       <c r="U587">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="V587">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W587">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="X587">
         <v>-1</v>
       </c>
       <c r="Y587">
-        <v>-1</v>
+        <v>1.6</v>
       </c>
       <c r="Z587">
+        <v>-1</v>
+      </c>
+      <c r="AA587">
         <v>0.8</v>
       </c>
-      <c r="AA587">
-        <v>-1</v>
-      </c>
       <c r="AB587">
-        <v>0.875</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC587">
         <v>-1</v>
@@ -52788,7 +52788,7 @@
         <v>586</v>
       </c>
       <c r="B588">
-        <v>4617491</v>
+        <v>4617747</v>
       </c>
       <c r="C588" t="s">
         <v>28</v>
@@ -52800,76 +52800,76 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F588" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G588" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H588">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I588">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J588" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K588">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
       <c r="L588">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="M588">
-        <v>2.45</v>
+        <v>2.9</v>
       </c>
       <c r="N588">
-        <v>2.7</v>
+        <v>2.15</v>
       </c>
       <c r="O588">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="P588">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
       <c r="Q588">
+        <v>-0.25</v>
+      </c>
+      <c r="R588">
+        <v>1.825</v>
+      </c>
+      <c r="S588">
+        <v>1.975</v>
+      </c>
+      <c r="T588">
+        <v>2</v>
+      </c>
+      <c r="U588">
+        <v>1.775</v>
+      </c>
+      <c r="V588">
+        <v>2.025</v>
+      </c>
+      <c r="W588">
+        <v>1.15</v>
+      </c>
+      <c r="X588">
+        <v>-1</v>
+      </c>
+      <c r="Y588">
+        <v>-1</v>
+      </c>
+      <c r="Z588">
+        <v>0.825</v>
+      </c>
+      <c r="AA588">
+        <v>-1</v>
+      </c>
+      <c r="AB588">
         <v>0</v>
       </c>
-      <c r="R588">
-        <v>2</v>
-      </c>
-      <c r="S588">
-        <v>1.8</v>
-      </c>
-      <c r="T588">
-        <v>2.5</v>
-      </c>
-      <c r="U588">
-        <v>1.9</v>
-      </c>
-      <c r="V588">
-        <v>1.9</v>
-      </c>
-      <c r="W588">
-        <v>-1</v>
-      </c>
-      <c r="X588">
-        <v>-1</v>
-      </c>
-      <c r="Y588">
-        <v>1.6</v>
-      </c>
-      <c r="Z588">
-        <v>-1</v>
-      </c>
-      <c r="AA588">
-        <v>0.8</v>
-      </c>
-      <c r="AB588">
-        <v>0.8999999999999999</v>
-      </c>
       <c r="AC588">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="589" spans="1:29">
@@ -52877,7 +52877,7 @@
         <v>587</v>
       </c>
       <c r="B589">
-        <v>4617747</v>
+        <v>4614405</v>
       </c>
       <c r="C589" t="s">
         <v>28</v>
@@ -52889,13 +52889,13 @@
         <v>44870.52083333334</v>
       </c>
       <c r="F589" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G589" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H589">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I589">
         <v>0</v>
@@ -52904,43 +52904,43 @@
         <v>52</v>
       </c>
       <c r="K589">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="L589">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="M589">
-        <v>2.9</v>
+        <v>4.333</v>
       </c>
       <c r="N589">
-        <v>2.15</v>
+        <v>1.833</v>
       </c>
       <c r="O589">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="P589">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="Q589">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R589">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="S589">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T589">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U589">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="V589">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W589">
-        <v>1.15</v>
+        <v>0.833</v>
       </c>
       <c r="X589">
         <v>-1</v>
@@ -52949,16 +52949,16 @@
         <v>-1</v>
       </c>
       <c r="Z589">
-        <v>0.825</v>
+        <v>0.8</v>
       </c>
       <c r="AA589">
         <v>-1</v>
       </c>
       <c r="AB589">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="AC589">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="590" spans="1:29">
@@ -52966,7 +52966,7 @@
         <v>588</v>
       </c>
       <c r="B590">
-        <v>4614404</v>
+        <v>4617739</v>
       </c>
       <c r="C590" t="s">
         <v>28</v>
@@ -52978,10 +52978,10 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F590" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G590" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H590">
         <v>1</v>
@@ -52993,46 +52993,46 @@
         <v>51</v>
       </c>
       <c r="K590">
-        <v>2.75</v>
+        <v>2.3</v>
       </c>
       <c r="L590">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="M590">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="N590">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="O590">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="P590">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="Q590">
         <v>-0.25</v>
       </c>
       <c r="R590">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="S590">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T590">
         <v>2.25</v>
       </c>
       <c r="U590">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="V590">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W590">
         <v>-1</v>
       </c>
       <c r="X590">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="Y590">
         <v>-1</v>
@@ -53041,13 +53041,13 @@
         <v>-0.5</v>
       </c>
       <c r="AA590">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="AB590">
         <v>-0.5</v>
       </c>
       <c r="AC590">
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="591" spans="1:29">
@@ -53055,7 +53055,7 @@
         <v>589</v>
       </c>
       <c r="B591">
-        <v>4617739</v>
+        <v>4617490</v>
       </c>
       <c r="C591" t="s">
         <v>28</v>
@@ -53067,76 +53067,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F591" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G591" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H591">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I591">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J591" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K591">
-        <v>2.3</v>
+        <v>1.55</v>
       </c>
       <c r="L591">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="M591">
+        <v>5.5</v>
+      </c>
+      <c r="N591">
+        <v>1.4</v>
+      </c>
+      <c r="O591">
+        <v>4.75</v>
+      </c>
+      <c r="P591">
+        <v>7.5</v>
+      </c>
+      <c r="Q591">
+        <v>-1.25</v>
+      </c>
+      <c r="R591">
+        <v>1.85</v>
+      </c>
+      <c r="S591">
+        <v>1.95</v>
+      </c>
+      <c r="T591">
         <v>3</v>
       </c>
-      <c r="N591">
-        <v>2.1</v>
-      </c>
-      <c r="O591">
-        <v>3.5</v>
-      </c>
-      <c r="P591">
-        <v>3.4</v>
-      </c>
-      <c r="Q591">
-        <v>-0.25</v>
-      </c>
-      <c r="R591">
+      <c r="U591">
+        <v>2</v>
+      </c>
+      <c r="V591">
         <v>1.8</v>
       </c>
-      <c r="S591">
-        <v>2</v>
-      </c>
-      <c r="T591">
-        <v>2.25</v>
-      </c>
-      <c r="U591">
-        <v>1.8</v>
-      </c>
-      <c r="V591">
-        <v>2</v>
-      </c>
       <c r="W591">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="X591">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y591">
         <v>-1</v>
       </c>
       <c r="Z591">
-        <v>-0.5</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA591">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB591">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AC591">
-        <v>0.5</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="592" spans="1:29">
@@ -53144,7 +53144,7 @@
         <v>590</v>
       </c>
       <c r="B592">
-        <v>4617490</v>
+        <v>4614403</v>
       </c>
       <c r="C592" t="s">
         <v>28</v>
@@ -53156,76 +53156,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F592" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G592" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H592">
+        <v>0</v>
+      </c>
+      <c r="I592">
+        <v>2</v>
+      </c>
+      <c r="J592" t="s">
+        <v>53</v>
+      </c>
+      <c r="K592">
         <v>3</v>
       </c>
-      <c r="I592">
-        <v>0</v>
-      </c>
-      <c r="J592" t="s">
-        <v>52</v>
-      </c>
-      <c r="K592">
-        <v>1.55</v>
-      </c>
       <c r="L592">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="M592">
-        <v>5.5</v>
+        <v>2.2</v>
       </c>
       <c r="N592">
-        <v>1.4</v>
+        <v>3.4</v>
       </c>
       <c r="O592">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P592">
-        <v>7.5</v>
+        <v>2.15</v>
       </c>
       <c r="Q592">
-        <v>-1.25</v>
+        <v>0.25</v>
       </c>
       <c r="R592">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S592">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T592">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="U592">
-        <v>2</v>
+        <v>1.775</v>
       </c>
       <c r="V592">
-        <v>1.8</v>
+        <v>2.025</v>
       </c>
       <c r="W592">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X592">
         <v>-1</v>
       </c>
       <c r="Y592">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="Z592">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA592">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB592">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AC592">
-        <v>-0</v>
+        <v>0.5125</v>
       </c>
     </row>
     <row r="593" spans="1:29">
@@ -53233,7 +53233,7 @@
         <v>591</v>
       </c>
       <c r="B593">
-        <v>4614403</v>
+        <v>4614404</v>
       </c>
       <c r="C593" t="s">
         <v>28</v>
@@ -53245,76 +53245,76 @@
         <v>44871.66666666666</v>
       </c>
       <c r="F593" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="G593" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H593">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I593">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J593" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K593">
+        <v>2.75</v>
+      </c>
+      <c r="L593">
+        <v>3.1</v>
+      </c>
+      <c r="M593">
+        <v>2.5</v>
+      </c>
+      <c r="N593">
+        <v>2.4</v>
+      </c>
+      <c r="O593">
+        <v>3.25</v>
+      </c>
+      <c r="P593">
         <v>3</v>
       </c>
-      <c r="L593">
-        <v>3.4</v>
-      </c>
-      <c r="M593">
-        <v>2.2</v>
-      </c>
-      <c r="N593">
-        <v>3.4</v>
-      </c>
-      <c r="O593">
-        <v>3.5</v>
-      </c>
-      <c r="P593">
-        <v>2.15</v>
-      </c>
       <c r="Q593">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R593">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="S593">
-        <v>1.825</v>
+        <v>1.75</v>
       </c>
       <c r="T593">
         <v>2.25</v>
       </c>
       <c r="U593">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="V593">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W593">
         <v>-1</v>
       </c>
       <c r="X593">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="Y593">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="Z593">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AA593">
-        <v>0.825</v>
+        <v>0.375</v>
       </c>
       <c r="AB593">
         <v>-0.5</v>
       </c>
       <c r="AC593">
-        <v>0.5125</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="594" spans="1:29">
@@ -55547,7 +55547,7 @@
         <v>617</v>
       </c>
       <c r="B619">
-        <v>6078853</v>
+        <v>6073146</v>
       </c>
       <c r="C619" t="s">
         <v>28</v>
@@ -55559,73 +55559,73 @@
         <v>44967.875</v>
       </c>
       <c r="F619" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G619" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H619">
+        <v>1</v>
+      </c>
+      <c r="I619">
         <v>3</v>
       </c>
-      <c r="I619">
-        <v>2</v>
-      </c>
       <c r="J619" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K619">
-        <v>2.625</v>
+        <v>2.7</v>
       </c>
       <c r="L619">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="M619">
-        <v>2.4</v>
+        <v>2.45</v>
       </c>
       <c r="N619">
-        <v>1.909</v>
+        <v>3.3</v>
       </c>
       <c r="O619">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="P619">
-        <v>4.2</v>
+        <v>2.25</v>
       </c>
       <c r="Q619">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R619">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="S619">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="T619">
         <v>2.5</v>
       </c>
       <c r="U619">
+        <v>1.875</v>
+      </c>
+      <c r="V619">
         <v>1.925</v>
       </c>
-      <c r="V619">
-        <v>1.875</v>
-      </c>
       <c r="W619">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X619">
         <v>-1</v>
       </c>
       <c r="Y619">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="Z619">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA619">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB619">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AC619">
         <v>-1</v>
@@ -55636,7 +55636,7 @@
         <v>618</v>
       </c>
       <c r="B620">
-        <v>6073146</v>
+        <v>6078853</v>
       </c>
       <c r="C620" t="s">
         <v>28</v>
@@ -55648,73 +55648,73 @@
         <v>44967.875</v>
       </c>
       <c r="F620" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G620" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H620">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I620">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J620" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K620">
-        <v>2.7</v>
+        <v>2.625</v>
       </c>
       <c r="L620">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="M620">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="N620">
-        <v>3.3</v>
+        <v>1.909</v>
       </c>
       <c r="O620">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="P620">
-        <v>2.25</v>
+        <v>4.2</v>
       </c>
       <c r="Q620">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R620">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="S620">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="T620">
         <v>2.5</v>
       </c>
       <c r="U620">
+        <v>1.925</v>
+      </c>
+      <c r="V620">
         <v>1.875</v>
       </c>
-      <c r="V620">
-        <v>1.925</v>
-      </c>
       <c r="W620">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X620">
         <v>-1</v>
       </c>
       <c r="Y620">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Z620">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA620">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB620">
-        <v>0.875</v>
+        <v>0.925</v>
       </c>
       <c r="AC620">
         <v>-1</v>
@@ -57505,7 +57505,7 @@
         <v>639</v>
       </c>
       <c r="B641">
-        <v>6078862</v>
+        <v>6078937</v>
       </c>
       <c r="C641" t="s">
         <v>28</v>
@@ -57517,13 +57517,13 @@
         <v>44988.75</v>
       </c>
       <c r="F641" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G641" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H641">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I641">
         <v>1</v>
@@ -57532,43 +57532,43 @@
         <v>52</v>
       </c>
       <c r="K641">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="L641">
         <v>3.3</v>
       </c>
       <c r="M641">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="N641">
-        <v>1.8</v>
+        <v>2.45</v>
       </c>
       <c r="O641">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="P641">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="Q641">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R641">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S641">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="T641">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U641">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V641">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W641">
-        <v>0.8</v>
+        <v>1.45</v>
       </c>
       <c r="X641">
         <v>-1</v>
@@ -57577,16 +57577,16 @@
         <v>-1</v>
       </c>
       <c r="Z641">
-        <v>0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA641">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB641">
-        <v>0.475</v>
+        <v>1.025</v>
       </c>
       <c r="AC641">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="642" spans="1:29">
@@ -57594,7 +57594,7 @@
         <v>640</v>
       </c>
       <c r="B642">
-        <v>6078937</v>
+        <v>6078862</v>
       </c>
       <c r="C642" t="s">
         <v>28</v>
@@ -57606,13 +57606,13 @@
         <v>44988.75</v>
       </c>
       <c r="F642" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G642" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H642">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I642">
         <v>1</v>
@@ -57621,43 +57621,43 @@
         <v>52</v>
       </c>
       <c r="K642">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="L642">
         <v>3.3</v>
       </c>
       <c r="M642">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="N642">
-        <v>2.45</v>
+        <v>1.8</v>
       </c>
       <c r="O642">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="P642">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="Q642">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R642">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S642">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="T642">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U642">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V642">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W642">
-        <v>1.45</v>
+        <v>0.8</v>
       </c>
       <c r="X642">
         <v>-1</v>
@@ -57666,16 +57666,16 @@
         <v>-1</v>
       </c>
       <c r="Z642">
-        <v>0.9750000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="AA642">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB642">
-        <v>1.025</v>
+        <v>0.475</v>
       </c>
       <c r="AC642">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="643" spans="1:29">
@@ -58751,7 +58751,7 @@
         <v>653</v>
       </c>
       <c r="B655">
-        <v>6078944</v>
+        <v>6078868</v>
       </c>
       <c r="C655" t="s">
         <v>28</v>
@@ -58763,76 +58763,76 @@
         <v>45003.75</v>
       </c>
       <c r="F655" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G655" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H655">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I655">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J655" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K655">
-        <v>2</v>
+        <v>2.875</v>
       </c>
       <c r="L655">
         <v>3.25</v>
       </c>
       <c r="M655">
-        <v>3.4</v>
+        <v>2.25</v>
       </c>
       <c r="N655">
-        <v>2.15</v>
+        <v>3.3</v>
       </c>
       <c r="O655">
-        <v>3.25</v>
+        <v>3.3</v>
       </c>
       <c r="P655">
-        <v>3.6</v>
+        <v>2.25</v>
       </c>
       <c r="Q655">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R655">
+        <v>1.875</v>
+      </c>
+      <c r="S655">
+        <v>1.925</v>
+      </c>
+      <c r="T655">
+        <v>2.5</v>
+      </c>
+      <c r="U655">
+        <v>2</v>
+      </c>
+      <c r="V655">
         <v>1.8</v>
       </c>
-      <c r="S655">
-        <v>2</v>
-      </c>
-      <c r="T655">
-        <v>2.25</v>
-      </c>
-      <c r="U655">
-        <v>1.85</v>
-      </c>
-      <c r="V655">
-        <v>1.95</v>
-      </c>
       <c r="W655">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="X655">
         <v>-1</v>
       </c>
       <c r="Y655">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z655">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA655">
+        <v>-1</v>
+      </c>
+      <c r="AB655">
         <v>1</v>
       </c>
-      <c r="AB655">
-        <v>-0.5</v>
-      </c>
       <c r="AC655">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="656" spans="1:29">
@@ -58840,7 +58840,7 @@
         <v>654</v>
       </c>
       <c r="B656">
-        <v>6078868</v>
+        <v>6078944</v>
       </c>
       <c r="C656" t="s">
         <v>28</v>
@@ -58852,76 +58852,76 @@
         <v>45003.75</v>
       </c>
       <c r="F656" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G656" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H656">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I656">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J656" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K656">
-        <v>2.875</v>
+        <v>2</v>
       </c>
       <c r="L656">
         <v>3.25</v>
       </c>
       <c r="M656">
+        <v>3.4</v>
+      </c>
+      <c r="N656">
+        <v>2.15</v>
+      </c>
+      <c r="O656">
+        <v>3.25</v>
+      </c>
+      <c r="P656">
+        <v>3.6</v>
+      </c>
+      <c r="Q656">
+        <v>-0.25</v>
+      </c>
+      <c r="R656">
+        <v>1.8</v>
+      </c>
+      <c r="S656">
+        <v>2</v>
+      </c>
+      <c r="T656">
         <v>2.25</v>
       </c>
-      <c r="N656">
-        <v>3.3</v>
-      </c>
-      <c r="O656">
-        <v>3.3</v>
-      </c>
-      <c r="P656">
-        <v>2.25</v>
-      </c>
-      <c r="Q656">
-        <v>0.25</v>
-      </c>
-      <c r="R656">
-        <v>1.875</v>
-      </c>
-      <c r="S656">
-        <v>1.925</v>
-      </c>
-      <c r="T656">
-        <v>2.5</v>
-      </c>
       <c r="U656">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V656">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="W656">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="X656">
         <v>-1</v>
       </c>
       <c r="Y656">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Z656">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA656">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB656">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AC656">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
     </row>
     <row r="657" spans="1:29">
@@ -59107,7 +59107,7 @@
         <v>657</v>
       </c>
       <c r="B659">
-        <v>6075784</v>
+        <v>6078866</v>
       </c>
       <c r="C659" t="s">
         <v>28</v>
@@ -59119,70 +59119,70 @@
         <v>45004.85416666666</v>
       </c>
       <c r="F659" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G659" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H659">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I659">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J659" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K659">
-        <v>3</v>
+        <v>2.625</v>
       </c>
       <c r="L659">
         <v>3.3</v>
       </c>
       <c r="M659">
+        <v>2.375</v>
+      </c>
+      <c r="N659">
+        <v>3.3</v>
+      </c>
+      <c r="O659">
+        <v>3.5</v>
+      </c>
+      <c r="P659">
         <v>2.15</v>
-      </c>
-      <c r="N659">
-        <v>3.4</v>
-      </c>
-      <c r="O659">
-        <v>3.6</v>
-      </c>
-      <c r="P659">
-        <v>2.05</v>
       </c>
       <c r="Q659">
         <v>0.25</v>
       </c>
       <c r="R659">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="S659">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="T659">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U659">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V659">
         <v>1.925</v>
       </c>
       <c r="W659">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="X659">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y659">
         <v>-1</v>
       </c>
       <c r="Z659">
-        <v>0.5125</v>
+        <v>0.95</v>
       </c>
       <c r="AA659">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB659">
         <v>-1</v>
@@ -59196,7 +59196,7 @@
         <v>658</v>
       </c>
       <c r="B660">
-        <v>6078866</v>
+        <v>6075784</v>
       </c>
       <c r="C660" t="s">
         <v>28</v>
@@ -59208,70 +59208,70 @@
         <v>45004.85416666666</v>
       </c>
       <c r="F660" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G660" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H660">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I660">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J660" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K660">
-        <v>2.625</v>
+        <v>3</v>
       </c>
       <c r="L660">
         <v>3.3</v>
       </c>
       <c r="M660">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N660">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="O660">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="P660">
-        <v>2.15</v>
+        <v>2.05</v>
       </c>
       <c r="Q660">
         <v>0.25</v>
       </c>
       <c r="R660">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S660">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="T660">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U660">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V660">
         <v>1.925</v>
       </c>
       <c r="W660">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="X660">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y660">
         <v>-1</v>
       </c>
       <c r="Z660">
-        <v>0.95</v>
+        <v>0.5125</v>
       </c>
       <c r="AA660">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB660">
         <v>-1</v>
@@ -61599,7 +61599,7 @@
         <v>685</v>
       </c>
       <c r="B687">
-        <v>6075792</v>
+        <v>6078878</v>
       </c>
       <c r="C687" t="s">
         <v>28</v>
@@ -61611,58 +61611,58 @@
         <v>45055.79166666666</v>
       </c>
       <c r="F687" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G687" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="H687">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I687">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J687" t="s">
         <v>52</v>
       </c>
       <c r="K687">
-        <v>1.85</v>
+        <v>2.2</v>
       </c>
       <c r="L687">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="M687">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="N687">
-        <v>1.95</v>
+        <v>2.55</v>
       </c>
       <c r="O687">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="P687">
-        <v>4</v>
+        <v>2.875</v>
       </c>
       <c r="Q687">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R687">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S687">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T687">
         <v>2.5</v>
       </c>
       <c r="U687">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V687">
         <v>1.875</v>
       </c>
       <c r="W687">
-        <v>0.95</v>
+        <v>1.55</v>
       </c>
       <c r="X687">
         <v>-1</v>
@@ -61671,16 +61671,16 @@
         <v>-1</v>
       </c>
       <c r="Z687">
-        <v>0.8999999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="AA687">
         <v>-1</v>
       </c>
       <c r="AB687">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC687">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="688" spans="1:29">
@@ -61688,7 +61688,7 @@
         <v>686</v>
       </c>
       <c r="B688">
-        <v>6078878</v>
+        <v>6075792</v>
       </c>
       <c r="C688" t="s">
         <v>28</v>
@@ -61700,58 +61700,58 @@
         <v>45055.79166666666</v>
       </c>
       <c r="F688" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G688" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="H688">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I688">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J688" t="s">
         <v>52</v>
       </c>
       <c r="K688">
-        <v>2.2</v>
+        <v>1.85</v>
       </c>
       <c r="L688">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="M688">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="N688">
-        <v>2.55</v>
+        <v>1.95</v>
       </c>
       <c r="O688">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="P688">
-        <v>2.875</v>
+        <v>4</v>
       </c>
       <c r="Q688">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R688">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="S688">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="T688">
         <v>2.5</v>
       </c>
       <c r="U688">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V688">
         <v>1.875</v>
       </c>
       <c r="W688">
-        <v>1.55</v>
+        <v>0.95</v>
       </c>
       <c r="X688">
         <v>-1</v>
@@ -61760,16 +61760,16 @@
         <v>-1</v>
       </c>
       <c r="Z688">
-        <v>0.8</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA688">
         <v>-1</v>
       </c>
       <c r="AB688">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC688">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="689" spans="1:29">
@@ -61866,7 +61866,7 @@
         <v>688</v>
       </c>
       <c r="B690">
-        <v>6532619</v>
+        <v>6078876</v>
       </c>
       <c r="C690" t="s">
         <v>28</v>
@@ -61878,58 +61878,58 @@
         <v>45056.79166666666</v>
       </c>
       <c r="F690" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G690" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H690">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I690">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J690" t="s">
         <v>52</v>
       </c>
       <c r="K690">
-        <v>2.55</v>
+        <v>1.85</v>
       </c>
       <c r="L690">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M690">
+        <v>3.75</v>
+      </c>
+      <c r="N690">
+        <v>1.909</v>
+      </c>
+      <c r="O690">
+        <v>3.6</v>
+      </c>
+      <c r="P690">
+        <v>4.2</v>
+      </c>
+      <c r="Q690">
+        <v>-0.5</v>
+      </c>
+      <c r="R690">
+        <v>1.85</v>
+      </c>
+      <c r="S690">
+        <v>1.95</v>
+      </c>
+      <c r="T690">
         <v>2.5</v>
       </c>
-      <c r="N690">
-        <v>2.45</v>
-      </c>
-      <c r="O690">
-        <v>3.3</v>
-      </c>
-      <c r="P690">
-        <v>3</v>
-      </c>
-      <c r="Q690">
-        <v>-0.25</v>
-      </c>
-      <c r="R690">
-        <v>2.05</v>
-      </c>
-      <c r="S690">
-        <v>1.75</v>
-      </c>
-      <c r="T690">
-        <v>2.25</v>
-      </c>
       <c r="U690">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="V690">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W690">
-        <v>1.45</v>
+        <v>0.909</v>
       </c>
       <c r="X690">
         <v>-1</v>
@@ -61938,16 +61938,16 @@
         <v>-1</v>
       </c>
       <c r="Z690">
-        <v>1.05</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA690">
         <v>-1</v>
       </c>
       <c r="AB690">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC690">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="691" spans="1:29">
@@ -61955,7 +61955,7 @@
         <v>689</v>
       </c>
       <c r="B691">
-        <v>6078876</v>
+        <v>6532619</v>
       </c>
       <c r="C691" t="s">
         <v>28</v>
@@ -61967,58 +61967,58 @@
         <v>45056.79166666666</v>
       </c>
       <c r="F691" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G691" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H691">
+        <v>2</v>
+      </c>
+      <c r="I691">
         <v>1</v>
-      </c>
-      <c r="I691">
-        <v>0</v>
       </c>
       <c r="J691" t="s">
         <v>52</v>
       </c>
       <c r="K691">
-        <v>1.85</v>
+        <v>2.55</v>
       </c>
       <c r="L691">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M691">
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
       <c r="N691">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="O691">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="P691">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="Q691">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R691">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="S691">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="T691">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U691">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V691">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="W691">
-        <v>0.909</v>
+        <v>1.45</v>
       </c>
       <c r="X691">
         <v>-1</v>
@@ -62027,16 +62027,16 @@
         <v>-1</v>
       </c>
       <c r="Z691">
-        <v>0.8500000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="AA691">
         <v>-1</v>
       </c>
       <c r="AB691">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC691">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="692" spans="1:29">
@@ -73703,7 +73703,7 @@
         <v>821</v>
       </c>
       <c r="B823">
-        <v>6078997</v>
+        <v>6078267</v>
       </c>
       <c r="C823" t="s">
         <v>28</v>
@@ -73715,13 +73715,13 @@
         <v>45268.75</v>
       </c>
       <c r="F823" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G823" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H823">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I823">
         <v>0</v>
@@ -73730,28 +73730,28 @@
         <v>52</v>
       </c>
       <c r="K823">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="L823">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="M823">
-        <v>1.909</v>
+        <v>6</v>
       </c>
       <c r="N823">
-        <v>2.7</v>
+        <v>1.444</v>
       </c>
       <c r="O823">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P823">
-        <v>2.45</v>
+        <v>7</v>
       </c>
       <c r="Q823">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="R823">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="S823">
         <v>1.825</v>
@@ -73760,13 +73760,13 @@
         <v>2.75</v>
       </c>
       <c r="U823">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="V823">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="W823">
-        <v>1.7</v>
+        <v>0.444</v>
       </c>
       <c r="X823">
         <v>-1</v>
@@ -73775,7 +73775,7 @@
         <v>-1</v>
       </c>
       <c r="Z823">
-        <v>0.9750000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AA823">
         <v>-1</v>
@@ -73784,7 +73784,7 @@
         <v>-1</v>
       </c>
       <c r="AC823">
-        <v>1.025</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="824" spans="1:29">
@@ -73792,7 +73792,7 @@
         <v>822</v>
       </c>
       <c r="B824">
-        <v>6078267</v>
+        <v>6143704</v>
       </c>
       <c r="C824" t="s">
         <v>28</v>
@@ -73804,67 +73804,67 @@
         <v>45268.75</v>
       </c>
       <c r="F824" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G824" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H824">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I824">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J824" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K824">
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="L824">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="M824">
-        <v>6</v>
+        <v>1.4</v>
       </c>
       <c r="N824">
-        <v>1.444</v>
+        <v>12</v>
       </c>
       <c r="O824">
-        <v>4.75</v>
+        <v>8.5</v>
       </c>
       <c r="P824">
-        <v>7</v>
+        <v>1.166</v>
       </c>
       <c r="Q824">
-        <v>-1.25</v>
+        <v>2</v>
       </c>
       <c r="R824">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="S824">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T824">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U824">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="V824">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W824">
-        <v>0.444</v>
+        <v>-1</v>
       </c>
       <c r="X824">
         <v>-1</v>
       </c>
       <c r="Y824">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="Z824">
-        <v>1.025</v>
+        <v>1</v>
       </c>
       <c r="AA824">
         <v>-1</v>
@@ -73873,7 +73873,7 @@
         <v>-1</v>
       </c>
       <c r="AC824">
-        <v>1.05</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="825" spans="1:29">
@@ -73881,7 +73881,7 @@
         <v>823</v>
       </c>
       <c r="B825">
-        <v>6143704</v>
+        <v>6078997</v>
       </c>
       <c r="C825" t="s">
         <v>28</v>
@@ -73893,67 +73893,67 @@
         <v>45268.75</v>
       </c>
       <c r="F825" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G825" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H825">
+        <v>1</v>
+      </c>
+      <c r="I825">
         <v>0</v>
       </c>
-      <c r="I825">
-        <v>1</v>
-      </c>
       <c r="J825" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K825">
-        <v>6.5</v>
+        <v>3.8</v>
       </c>
       <c r="L825">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="M825">
-        <v>1.4</v>
+        <v>1.909</v>
       </c>
       <c r="N825">
-        <v>12</v>
+        <v>2.7</v>
       </c>
       <c r="O825">
-        <v>8.5</v>
+        <v>3.6</v>
       </c>
       <c r="P825">
-        <v>1.166</v>
+        <v>2.45</v>
       </c>
       <c r="Q825">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R825">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S825">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T825">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U825">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V825">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W825">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="X825">
         <v>-1</v>
       </c>
       <c r="Y825">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z825">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA825">
         <v>-1</v>
@@ -73962,7 +73962,7 @@
         <v>-1</v>
       </c>
       <c r="AC825">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="826" spans="1:29">
@@ -73970,7 +73970,7 @@
         <v>824</v>
       </c>
       <c r="B826">
-        <v>6078998</v>
+        <v>6078268</v>
       </c>
       <c r="C826" t="s">
         <v>28</v>
@@ -73982,55 +73982,55 @@
         <v>45269.75</v>
       </c>
       <c r="F826" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="G826" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H826">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I826">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J826" t="s">
         <v>53</v>
       </c>
       <c r="K826">
-        <v>1.909</v>
+        <v>3.1</v>
       </c>
       <c r="L826">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="M826">
-        <v>3.8</v>
+        <v>2.3</v>
       </c>
       <c r="N826">
-        <v>2.15</v>
+        <v>2.9</v>
       </c>
       <c r="O826">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P826">
-        <v>3.1</v>
+        <v>2.375</v>
       </c>
       <c r="Q826">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R826">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S826">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="T826">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U826">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="V826">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="W826">
         <v>-1</v>
@@ -74039,19 +74039,19 @@
         <v>-1</v>
       </c>
       <c r="Y826">
-        <v>2.1</v>
+        <v>1.375</v>
       </c>
       <c r="Z826">
         <v>-1</v>
       </c>
       <c r="AA826">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="AB826">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC826">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="827" spans="1:29">
@@ -74148,7 +74148,7 @@
         <v>826</v>
       </c>
       <c r="B828">
-        <v>6077768</v>
+        <v>6078269</v>
       </c>
       <c r="C828" t="s">
         <v>28</v>
@@ -74160,76 +74160,76 @@
         <v>45269.75</v>
       </c>
       <c r="F828" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G828" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H828">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I828">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J828" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K828">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="L828">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M828">
-        <v>3.4</v>
+        <v>4.333</v>
       </c>
       <c r="N828">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="O828">
         <v>3.6</v>
       </c>
       <c r="P828">
-        <v>3.4</v>
+        <v>4.5</v>
       </c>
       <c r="Q828">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R828">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S828">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="T828">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U828">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V828">
         <v>1.825</v>
       </c>
       <c r="W828">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X828">
         <v>-1</v>
       </c>
       <c r="Y828">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z828">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA828">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB828">
-        <v>0.4875</v>
+        <v>1.025</v>
       </c>
       <c r="AC828">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="829" spans="1:29">
@@ -74237,7 +74237,7 @@
         <v>827</v>
       </c>
       <c r="B829">
-        <v>6078269</v>
+        <v>6078998</v>
       </c>
       <c r="C829" t="s">
         <v>28</v>
@@ -74249,73 +74249,73 @@
         <v>45269.75</v>
       </c>
       <c r="F829" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G829" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H829">
+        <v>2</v>
+      </c>
+      <c r="I829">
         <v>3</v>
       </c>
-      <c r="I829">
-        <v>1</v>
-      </c>
       <c r="J829" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K829">
+        <v>1.909</v>
+      </c>
+      <c r="L829">
+        <v>3.6</v>
+      </c>
+      <c r="M829">
+        <v>3.8</v>
+      </c>
+      <c r="N829">
+        <v>2.15</v>
+      </c>
+      <c r="O829">
+        <v>3.75</v>
+      </c>
+      <c r="P829">
+        <v>3.1</v>
+      </c>
+      <c r="Q829">
+        <v>-0.25</v>
+      </c>
+      <c r="R829">
         <v>1.85</v>
       </c>
-      <c r="L829">
-        <v>3.4</v>
-      </c>
-      <c r="M829">
-        <v>4.333</v>
-      </c>
-      <c r="N829">
-        <v>1.8</v>
-      </c>
-      <c r="O829">
-        <v>3.6</v>
-      </c>
-      <c r="P829">
-        <v>4.5</v>
-      </c>
-      <c r="Q829">
-        <v>-0.75</v>
-      </c>
-      <c r="R829">
-        <v>1.925</v>
-      </c>
       <c r="S829">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T829">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U829">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V829">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W829">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="X829">
         <v>-1</v>
       </c>
       <c r="Y829">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="Z829">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA829">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB829">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC829">
         <v>-1</v>
@@ -74326,7 +74326,7 @@
         <v>828</v>
       </c>
       <c r="B830">
-        <v>6078268</v>
+        <v>6077768</v>
       </c>
       <c r="C830" t="s">
         <v>28</v>
@@ -74338,40 +74338,40 @@
         <v>45269.75</v>
       </c>
       <c r="F830" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G830" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H830">
         <v>0</v>
       </c>
       <c r="I830">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J830" t="s">
         <v>53</v>
       </c>
       <c r="K830">
-        <v>3.1</v>
+        <v>2.05</v>
       </c>
       <c r="L830">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M830">
-        <v>2.3</v>
+        <v>3.4</v>
       </c>
       <c r="N830">
-        <v>2.9</v>
+        <v>2.05</v>
       </c>
       <c r="O830">
+        <v>3.6</v>
+      </c>
+      <c r="P830">
         <v>3.4</v>
       </c>
-      <c r="P830">
-        <v>2.375</v>
-      </c>
       <c r="Q830">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R830">
         <v>1.8</v>
@@ -74383,10 +74383,10 @@
         <v>2.75</v>
       </c>
       <c r="U830">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V830">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="W830">
         <v>-1</v>
@@ -74395,7 +74395,7 @@
         <v>-1</v>
       </c>
       <c r="Y830">
-        <v>1.375</v>
+        <v>2.4</v>
       </c>
       <c r="Z830">
         <v>-1</v>
@@ -74404,10 +74404,10 @@
         <v>1</v>
       </c>
       <c r="AB830">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AC830">
-        <v>0.8</v>
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-30 às 23-14
</commit_message>
<xml_diff>
--- a/Chile Primera Division/Chile Primera Division.xlsx
+++ b/Chile Primera Division/Chile Primera Division.xlsx
@@ -31873,7 +31873,7 @@
         <v>351</v>
       </c>
       <c r="B353">
-        <v>3899436</v>
+        <v>3899777</v>
       </c>
       <c r="C353" t="s">
         <v>28</v>
@@ -31885,76 +31885,76 @@
         <v>44535.75</v>
       </c>
       <c r="F353" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G353" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H353">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I353">
         <v>1</v>
       </c>
       <c r="J353" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K353">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="L353">
-        <v>4.5</v>
+        <v>3.1</v>
       </c>
       <c r="M353">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N353">
-        <v>1.444</v>
+        <v>2.75</v>
       </c>
       <c r="O353">
-        <v>4.75</v>
+        <v>2.75</v>
       </c>
       <c r="P353">
-        <v>6.5</v>
+        <v>2.7</v>
       </c>
       <c r="Q353">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="R353">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S353">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="T353">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="U353">
-        <v>1.975</v>
+        <v>1.875</v>
       </c>
       <c r="V353">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="W353">
-        <v>0.444</v>
+        <v>-1</v>
       </c>
       <c r="X353">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y353">
         <v>-1</v>
       </c>
       <c r="Z353">
-        <v>1.025</v>
+        <v>0</v>
       </c>
       <c r="AA353">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB353">
-        <v>0.9750000000000001</v>
+        <v>0</v>
       </c>
       <c r="AC353">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="354" spans="1:29">
@@ -31962,7 +31962,7 @@
         <v>352</v>
       </c>
       <c r="B354">
-        <v>3899777</v>
+        <v>4396881</v>
       </c>
       <c r="C354" t="s">
         <v>28</v>
@@ -31974,76 +31974,76 @@
         <v>44535.75</v>
       </c>
       <c r="F354" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G354" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H354">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I354">
         <v>1</v>
       </c>
       <c r="J354" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K354">
-        <v>2.25</v>
+        <v>2.45</v>
       </c>
       <c r="L354">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="M354">
-        <v>3</v>
+        <v>2.625</v>
       </c>
       <c r="N354">
-        <v>2.75</v>
+        <v>2.7</v>
       </c>
       <c r="O354">
-        <v>2.75</v>
+        <v>3.6</v>
       </c>
       <c r="P354">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="Q354">
         <v>0</v>
       </c>
       <c r="R354">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="S354">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="T354">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U354">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V354">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="W354">
         <v>-1</v>
       </c>
       <c r="X354">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y354">
-        <v>-1</v>
+        <v>1.5</v>
       </c>
       <c r="Z354">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA354">
-        <v>-0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB354">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC354">
-        <v>-0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="355" spans="1:29">
@@ -32051,7 +32051,7 @@
         <v>353</v>
       </c>
       <c r="B355">
-        <v>4396881</v>
+        <v>3899436</v>
       </c>
       <c r="C355" t="s">
         <v>28</v>
@@ -32063,76 +32063,76 @@
         <v>44535.75</v>
       </c>
       <c r="F355" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G355" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H355">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I355">
         <v>1</v>
       </c>
       <c r="J355" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K355">
-        <v>2.45</v>
+        <v>1.4</v>
       </c>
       <c r="L355">
-        <v>3.2</v>
+        <v>4.5</v>
       </c>
       <c r="M355">
-        <v>2.625</v>
+        <v>6</v>
       </c>
       <c r="N355">
-        <v>2.7</v>
+        <v>1.444</v>
       </c>
       <c r="O355">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P355">
-        <v>2.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q355">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="R355">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S355">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="T355">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U355">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V355">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="W355">
-        <v>-1</v>
+        <v>0.444</v>
       </c>
       <c r="X355">
         <v>-1</v>
       </c>
       <c r="Y355">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="Z355">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA355">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB355">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC355">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="356" spans="1:29">
@@ -55547,7 +55547,7 @@
         <v>617</v>
       </c>
       <c r="B619">
-        <v>6078853</v>
+        <v>6073146</v>
       </c>
       <c r="C619" t="s">
         <v>28</v>
@@ -55559,73 +55559,73 @@
         <v>44967.875</v>
       </c>
       <c r="F619" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G619" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H619">
+        <v>1</v>
+      </c>
+      <c r="I619">
         <v>3</v>
       </c>
-      <c r="I619">
-        <v>2</v>
-      </c>
       <c r="J619" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K619">
-        <v>2.625</v>
+        <v>2.7</v>
       </c>
       <c r="L619">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="M619">
-        <v>2.4</v>
+        <v>2.45</v>
       </c>
       <c r="N619">
-        <v>1.909</v>
+        <v>3.3</v>
       </c>
       <c r="O619">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="P619">
-        <v>4.2</v>
+        <v>2.25</v>
       </c>
       <c r="Q619">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R619">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="S619">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="T619">
         <v>2.5</v>
       </c>
       <c r="U619">
+        <v>1.875</v>
+      </c>
+      <c r="V619">
         <v>1.925</v>
       </c>
-      <c r="V619">
-        <v>1.875</v>
-      </c>
       <c r="W619">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X619">
         <v>-1</v>
       </c>
       <c r="Y619">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="Z619">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA619">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB619">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AC619">
         <v>-1</v>
@@ -55636,7 +55636,7 @@
         <v>618</v>
       </c>
       <c r="B620">
-        <v>6073146</v>
+        <v>6078853</v>
       </c>
       <c r="C620" t="s">
         <v>28</v>
@@ -55648,73 +55648,73 @@
         <v>44967.875</v>
       </c>
       <c r="F620" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G620" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H620">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I620">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J620" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K620">
-        <v>2.7</v>
+        <v>2.625</v>
       </c>
       <c r="L620">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="M620">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="N620">
-        <v>3.3</v>
+        <v>1.909</v>
       </c>
       <c r="O620">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="P620">
-        <v>2.25</v>
+        <v>4.2</v>
       </c>
       <c r="Q620">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R620">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="S620">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="T620">
         <v>2.5</v>
       </c>
       <c r="U620">
+        <v>1.925</v>
+      </c>
+      <c r="V620">
         <v>1.875</v>
       </c>
-      <c r="V620">
-        <v>1.925</v>
-      </c>
       <c r="W620">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X620">
         <v>-1</v>
       </c>
       <c r="Y620">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Z620">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA620">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB620">
-        <v>0.875</v>
+        <v>0.925</v>
       </c>
       <c r="AC620">
         <v>-1</v>
@@ -57505,7 +57505,7 @@
         <v>639</v>
       </c>
       <c r="B641">
-        <v>6078862</v>
+        <v>6078937</v>
       </c>
       <c r="C641" t="s">
         <v>28</v>
@@ -57517,13 +57517,13 @@
         <v>44988.75</v>
       </c>
       <c r="F641" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G641" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H641">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I641">
         <v>1</v>
@@ -57532,43 +57532,43 @@
         <v>52</v>
       </c>
       <c r="K641">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="L641">
         <v>3.3</v>
       </c>
       <c r="M641">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="N641">
-        <v>1.8</v>
+        <v>2.45</v>
       </c>
       <c r="O641">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="P641">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="Q641">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R641">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S641">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="T641">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U641">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V641">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W641">
-        <v>0.8</v>
+        <v>1.45</v>
       </c>
       <c r="X641">
         <v>-1</v>
@@ -57577,16 +57577,16 @@
         <v>-1</v>
       </c>
       <c r="Z641">
-        <v>0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA641">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB641">
-        <v>0.475</v>
+        <v>1.025</v>
       </c>
       <c r="AC641">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="642" spans="1:29">
@@ -57594,7 +57594,7 @@
         <v>640</v>
       </c>
       <c r="B642">
-        <v>6078937</v>
+        <v>6078862</v>
       </c>
       <c r="C642" t="s">
         <v>28</v>
@@ -57606,13 +57606,13 @@
         <v>44988.75</v>
       </c>
       <c r="F642" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G642" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H642">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I642">
         <v>1</v>
@@ -57621,43 +57621,43 @@
         <v>52</v>
       </c>
       <c r="K642">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="L642">
         <v>3.3</v>
       </c>
       <c r="M642">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="N642">
-        <v>2.45</v>
+        <v>1.8</v>
       </c>
       <c r="O642">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="P642">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="Q642">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R642">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S642">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="T642">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U642">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V642">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W642">
-        <v>1.45</v>
+        <v>0.8</v>
       </c>
       <c r="X642">
         <v>-1</v>
@@ -57666,16 +57666,16 @@
         <v>-1</v>
       </c>
       <c r="Z642">
-        <v>0.9750000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="AA642">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB642">
-        <v>1.025</v>
+        <v>0.475</v>
       </c>
       <c r="AC642">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="643" spans="1:29">
@@ -61599,7 +61599,7 @@
         <v>685</v>
       </c>
       <c r="B687">
-        <v>6078878</v>
+        <v>6075792</v>
       </c>
       <c r="C687" t="s">
         <v>28</v>
@@ -61611,58 +61611,58 @@
         <v>45055.79166666666</v>
       </c>
       <c r="F687" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G687" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="H687">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I687">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J687" t="s">
         <v>52</v>
       </c>
       <c r="K687">
-        <v>2.2</v>
+        <v>1.85</v>
       </c>
       <c r="L687">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="M687">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="N687">
-        <v>2.55</v>
+        <v>1.95</v>
       </c>
       <c r="O687">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="P687">
-        <v>2.875</v>
+        <v>4</v>
       </c>
       <c r="Q687">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R687">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="S687">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="T687">
         <v>2.5</v>
       </c>
       <c r="U687">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V687">
         <v>1.875</v>
       </c>
       <c r="W687">
-        <v>1.55</v>
+        <v>0.95</v>
       </c>
       <c r="X687">
         <v>-1</v>
@@ -61671,16 +61671,16 @@
         <v>-1</v>
       </c>
       <c r="Z687">
-        <v>0.8</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA687">
         <v>-1</v>
       </c>
       <c r="AB687">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC687">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="688" spans="1:29">
@@ -61688,7 +61688,7 @@
         <v>686</v>
       </c>
       <c r="B688">
-        <v>6075792</v>
+        <v>6078878</v>
       </c>
       <c r="C688" t="s">
         <v>28</v>
@@ -61700,58 +61700,58 @@
         <v>45055.79166666666</v>
       </c>
       <c r="F688" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G688" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="H688">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I688">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J688" t="s">
         <v>52</v>
       </c>
       <c r="K688">
-        <v>1.85</v>
+        <v>2.2</v>
       </c>
       <c r="L688">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="M688">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="N688">
-        <v>1.95</v>
+        <v>2.55</v>
       </c>
       <c r="O688">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="P688">
-        <v>4</v>
+        <v>2.875</v>
       </c>
       <c r="Q688">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R688">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S688">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T688">
         <v>2.5</v>
       </c>
       <c r="U688">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V688">
         <v>1.875</v>
       </c>
       <c r="W688">
-        <v>0.95</v>
+        <v>1.55</v>
       </c>
       <c r="X688">
         <v>-1</v>
@@ -61760,16 +61760,16 @@
         <v>-1</v>
       </c>
       <c r="Z688">
-        <v>0.8999999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="AA688">
         <v>-1</v>
       </c>
       <c r="AB688">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC688">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="689" spans="1:29">
@@ -72813,7 +72813,7 @@
         <v>811</v>
       </c>
       <c r="B813">
-        <v>6077763</v>
+        <v>6077497</v>
       </c>
       <c r="C813" t="s">
         <v>28</v>
@@ -72825,37 +72825,37 @@
         <v>45256.85416666666</v>
       </c>
       <c r="F813" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G813" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H813">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I813">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J813" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K813">
-        <v>2.15</v>
+        <v>2.6</v>
       </c>
       <c r="L813">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M813">
+        <v>2.6</v>
+      </c>
+      <c r="N813">
+        <v>2.8</v>
+      </c>
+      <c r="O813">
         <v>3.2</v>
       </c>
-      <c r="N813">
-        <v>2.625</v>
-      </c>
-      <c r="O813">
-        <v>3.5</v>
-      </c>
       <c r="P813">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="Q813">
         <v>0</v>
@@ -72867,34 +72867,34 @@
         <v>1.9</v>
       </c>
       <c r="T813">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U813">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="V813">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="W813">
         <v>-1</v>
       </c>
       <c r="X813">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y813">
-        <v>1.6</v>
+        <v>-1</v>
       </c>
       <c r="Z813">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA813">
-        <v>0.8999999999999999</v>
+        <v>-0</v>
       </c>
       <c r="AB813">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AC813">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="814" spans="1:29">
@@ -72902,7 +72902,7 @@
         <v>812</v>
       </c>
       <c r="B814">
-        <v>6077497</v>
+        <v>6077763</v>
       </c>
       <c r="C814" t="s">
         <v>28</v>
@@ -72914,37 +72914,37 @@
         <v>45256.85416666666</v>
       </c>
       <c r="F814" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G814" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H814">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I814">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J814" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K814">
+        <v>2.15</v>
+      </c>
+      <c r="L814">
+        <v>3.5</v>
+      </c>
+      <c r="M814">
+        <v>3.2</v>
+      </c>
+      <c r="N814">
+        <v>2.625</v>
+      </c>
+      <c r="O814">
+        <v>3.5</v>
+      </c>
+      <c r="P814">
         <v>2.6</v>
-      </c>
-      <c r="L814">
-        <v>3.4</v>
-      </c>
-      <c r="M814">
-        <v>2.6</v>
-      </c>
-      <c r="N814">
-        <v>2.8</v>
-      </c>
-      <c r="O814">
-        <v>3.2</v>
-      </c>
-      <c r="P814">
-        <v>2.7</v>
       </c>
       <c r="Q814">
         <v>0</v>
@@ -72956,34 +72956,34 @@
         <v>1.9</v>
       </c>
       <c r="T814">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U814">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V814">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="W814">
         <v>-1</v>
       </c>
       <c r="X814">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y814">
-        <v>-1</v>
+        <v>1.6</v>
       </c>
       <c r="Z814">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA814">
-        <v>-0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB814">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC814">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="815" spans="1:29">
@@ -73080,7 +73080,7 @@
         <v>814</v>
       </c>
       <c r="B816">
-        <v>6078266</v>
+        <v>6077498</v>
       </c>
       <c r="C816" t="s">
         <v>28</v>
@@ -73092,73 +73092,73 @@
         <v>45262.75</v>
       </c>
       <c r="F816" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G816" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H816">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I816">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J816" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K816">
-        <v>1.533</v>
+        <v>1.65</v>
       </c>
       <c r="L816">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="M816">
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="N816">
-        <v>1.363</v>
+        <v>1.909</v>
       </c>
       <c r="O816">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="P816">
-        <v>7.5</v>
+        <v>4.2</v>
       </c>
       <c r="Q816">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R816">
+        <v>1.85</v>
+      </c>
+      <c r="S816">
+        <v>2</v>
+      </c>
+      <c r="T816">
+        <v>2.75</v>
+      </c>
+      <c r="U816">
         <v>2.025</v>
       </c>
-      <c r="S816">
+      <c r="V816">
         <v>1.825</v>
       </c>
-      <c r="T816">
-        <v>3</v>
-      </c>
-      <c r="U816">
-        <v>1.9</v>
-      </c>
-      <c r="V816">
-        <v>1.95</v>
-      </c>
       <c r="W816">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="X816">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y816">
         <v>-1</v>
       </c>
       <c r="Z816">
+        <v>-1</v>
+      </c>
+      <c r="AA816">
+        <v>1</v>
+      </c>
+      <c r="AB816">
         <v>1.025</v>
-      </c>
-      <c r="AA816">
-        <v>-1</v>
-      </c>
-      <c r="AB816">
-        <v>0.8999999999999999</v>
       </c>
       <c r="AC816">
         <v>-1</v>
@@ -73258,7 +73258,7 @@
         <v>816</v>
       </c>
       <c r="B818">
-        <v>6077498</v>
+        <v>6078266</v>
       </c>
       <c r="C818" t="s">
         <v>28</v>
@@ -73270,73 +73270,73 @@
         <v>45262.75</v>
       </c>
       <c r="F818" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G818" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H818">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I818">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J818" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K818">
-        <v>1.65</v>
+        <v>1.533</v>
       </c>
       <c r="L818">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="M818">
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="N818">
-        <v>1.909</v>
+        <v>1.363</v>
       </c>
       <c r="O818">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P818">
-        <v>4.2</v>
+        <v>7.5</v>
       </c>
       <c r="Q818">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="R818">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="S818">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="T818">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U818">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V818">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W818">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="X818">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y818">
         <v>-1</v>
       </c>
       <c r="Z818">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA818">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB818">
-        <v>1.025</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC818">
         <v>-1</v>
@@ -73436,7 +73436,7 @@
         <v>818</v>
       </c>
       <c r="B820">
-        <v>6078996</v>
+        <v>6077767</v>
       </c>
       <c r="C820" t="s">
         <v>28</v>
@@ -73448,55 +73448,55 @@
         <v>45263.75</v>
       </c>
       <c r="F820" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G820" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H820">
         <v>0</v>
       </c>
       <c r="I820">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J820" t="s">
         <v>53</v>
       </c>
       <c r="K820">
-        <v>1.4</v>
+        <v>2.75</v>
       </c>
       <c r="L820">
-        <v>4.333</v>
+        <v>3.4</v>
       </c>
       <c r="M820">
-        <v>7</v>
+        <v>2.45</v>
       </c>
       <c r="N820">
-        <v>1.285</v>
+        <v>2.875</v>
       </c>
       <c r="O820">
-        <v>5.5</v>
+        <v>3.3</v>
       </c>
       <c r="P820">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="Q820">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="R820">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="S820">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="T820">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="U820">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="V820">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="W820">
         <v>-1</v>
@@ -73505,19 +73505,19 @@
         <v>-1</v>
       </c>
       <c r="Y820">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="Z820">
         <v>-1</v>
       </c>
       <c r="AA820">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="AB820">
         <v>-1</v>
       </c>
       <c r="AC820">
-        <v>0.8500000000000001</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="821" spans="1:29">
@@ -73525,7 +73525,7 @@
         <v>819</v>
       </c>
       <c r="B821">
-        <v>6077767</v>
+        <v>6078263</v>
       </c>
       <c r="C821" t="s">
         <v>28</v>
@@ -73537,76 +73537,76 @@
         <v>45263.75</v>
       </c>
       <c r="F821" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G821" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H821">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I821">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J821" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K821">
-        <v>2.75</v>
+        <v>2.05</v>
       </c>
       <c r="L821">
         <v>3.4</v>
       </c>
       <c r="M821">
-        <v>2.45</v>
+        <v>3.5</v>
       </c>
       <c r="N821">
-        <v>2.875</v>
+        <v>2.05</v>
       </c>
       <c r="O821">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="P821">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="Q821">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R821">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="S821">
         <v>1.8</v>
       </c>
       <c r="T821">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U821">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V821">
-        <v>2.05</v>
+        <v>1.9</v>
       </c>
       <c r="W821">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="X821">
         <v>-1</v>
       </c>
       <c r="Y821">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="Z821">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA821">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB821">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC821">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="822" spans="1:29">
@@ -73614,7 +73614,7 @@
         <v>820</v>
       </c>
       <c r="B822">
-        <v>6078263</v>
+        <v>6078996</v>
       </c>
       <c r="C822" t="s">
         <v>28</v>
@@ -73626,76 +73626,76 @@
         <v>45263.75</v>
       </c>
       <c r="F822" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G822" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="H822">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I822">
+        <v>2</v>
+      </c>
+      <c r="J822" t="s">
+        <v>53</v>
+      </c>
+      <c r="K822">
+        <v>1.4</v>
+      </c>
+      <c r="L822">
+        <v>4.333</v>
+      </c>
+      <c r="M822">
+        <v>7</v>
+      </c>
+      <c r="N822">
+        <v>1.285</v>
+      </c>
+      <c r="O822">
+        <v>5.5</v>
+      </c>
+      <c r="P822">
+        <v>11</v>
+      </c>
+      <c r="Q822">
+        <v>-1.5</v>
+      </c>
+      <c r="R822">
+        <v>1.9</v>
+      </c>
+      <c r="S822">
+        <v>1.95</v>
+      </c>
+      <c r="T822">
         <v>3</v>
       </c>
-      <c r="J822" t="s">
-        <v>52</v>
-      </c>
-      <c r="K822">
-        <v>2.05</v>
-      </c>
-      <c r="L822">
-        <v>3.4</v>
-      </c>
-      <c r="M822">
-        <v>3.5</v>
-      </c>
-      <c r="N822">
-        <v>2.05</v>
-      </c>
-      <c r="O822">
-        <v>3.6</v>
-      </c>
-      <c r="P822">
-        <v>3.5</v>
-      </c>
-      <c r="Q822">
-        <v>-0.5</v>
-      </c>
-      <c r="R822">
-        <v>2</v>
-      </c>
-      <c r="S822">
-        <v>1.8</v>
-      </c>
-      <c r="T822">
-        <v>2.75</v>
-      </c>
       <c r="U822">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="V822">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="W822">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="X822">
         <v>-1</v>
       </c>
       <c r="Y822">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="Z822">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA822">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB822">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC822">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="823" spans="1:29">
@@ -73703,7 +73703,7 @@
         <v>821</v>
       </c>
       <c r="B823">
-        <v>6078997</v>
+        <v>6078267</v>
       </c>
       <c r="C823" t="s">
         <v>28</v>
@@ -73715,13 +73715,13 @@
         <v>45268.75</v>
       </c>
       <c r="F823" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G823" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H823">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I823">
         <v>0</v>
@@ -73730,28 +73730,28 @@
         <v>52</v>
       </c>
       <c r="K823">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="L823">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="M823">
-        <v>1.909</v>
+        <v>6</v>
       </c>
       <c r="N823">
-        <v>2.7</v>
+        <v>1.444</v>
       </c>
       <c r="O823">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P823">
-        <v>2.45</v>
+        <v>7</v>
       </c>
       <c r="Q823">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="R823">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="S823">
         <v>1.825</v>
@@ -73760,13 +73760,13 @@
         <v>2.75</v>
       </c>
       <c r="U823">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="V823">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="W823">
-        <v>1.7</v>
+        <v>0.444</v>
       </c>
       <c r="X823">
         <v>-1</v>
@@ -73775,7 +73775,7 @@
         <v>-1</v>
       </c>
       <c r="Z823">
-        <v>0.9750000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AA823">
         <v>-1</v>
@@ -73784,7 +73784,7 @@
         <v>-1</v>
       </c>
       <c r="AC823">
-        <v>1.025</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="824" spans="1:29">
@@ -73792,7 +73792,7 @@
         <v>822</v>
       </c>
       <c r="B824">
-        <v>6078267</v>
+        <v>6143704</v>
       </c>
       <c r="C824" t="s">
         <v>28</v>
@@ -73804,67 +73804,67 @@
         <v>45268.75</v>
       </c>
       <c r="F824" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G824" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H824">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I824">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J824" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K824">
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="L824">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="M824">
-        <v>6</v>
+        <v>1.4</v>
       </c>
       <c r="N824">
-        <v>1.444</v>
+        <v>12</v>
       </c>
       <c r="O824">
-        <v>4.75</v>
+        <v>8.5</v>
       </c>
       <c r="P824">
-        <v>7</v>
+        <v>1.166</v>
       </c>
       <c r="Q824">
-        <v>-1.25</v>
+        <v>2</v>
       </c>
       <c r="R824">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="S824">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T824">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U824">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="V824">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W824">
-        <v>0.444</v>
+        <v>-1</v>
       </c>
       <c r="X824">
         <v>-1</v>
       </c>
       <c r="Y824">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="Z824">
-        <v>1.025</v>
+        <v>1</v>
       </c>
       <c r="AA824">
         <v>-1</v>
@@ -73873,7 +73873,7 @@
         <v>-1</v>
       </c>
       <c r="AC824">
-        <v>1.05</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="825" spans="1:29">
@@ -73881,7 +73881,7 @@
         <v>823</v>
       </c>
       <c r="B825">
-        <v>6143704</v>
+        <v>6078997</v>
       </c>
       <c r="C825" t="s">
         <v>28</v>
@@ -73893,67 +73893,67 @@
         <v>45268.75</v>
       </c>
       <c r="F825" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G825" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H825">
+        <v>1</v>
+      </c>
+      <c r="I825">
         <v>0</v>
       </c>
-      <c r="I825">
-        <v>1</v>
-      </c>
       <c r="J825" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K825">
-        <v>6.5</v>
+        <v>3.8</v>
       </c>
       <c r="L825">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="M825">
-        <v>1.4</v>
+        <v>1.909</v>
       </c>
       <c r="N825">
-        <v>12</v>
+        <v>2.7</v>
       </c>
       <c r="O825">
-        <v>8.5</v>
+        <v>3.6</v>
       </c>
       <c r="P825">
-        <v>1.166</v>
+        <v>2.45</v>
       </c>
       <c r="Q825">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R825">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S825">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T825">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U825">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V825">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W825">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="X825">
         <v>-1</v>
       </c>
       <c r="Y825">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z825">
-        <v>1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA825">
         <v>-1</v>
@@ -73962,7 +73962,7 @@
         <v>-1</v>
       </c>
       <c r="AC825">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="826" spans="1:29">
@@ -73970,7 +73970,7 @@
         <v>824</v>
       </c>
       <c r="B826">
-        <v>6078998</v>
+        <v>6077499</v>
       </c>
       <c r="C826" t="s">
         <v>28</v>
@@ -73982,76 +73982,76 @@
         <v>45269.75</v>
       </c>
       <c r="F826" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G826" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="H826">
         <v>2</v>
       </c>
       <c r="I826">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J826" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K826">
-        <v>1.909</v>
+        <v>2.1</v>
       </c>
       <c r="L826">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M826">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N826">
-        <v>2.15</v>
+        <v>2.9</v>
       </c>
       <c r="O826">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P826">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="Q826">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R826">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="S826">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="T826">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U826">
         <v>1.85</v>
       </c>
       <c r="V826">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W826">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="X826">
         <v>-1</v>
       </c>
       <c r="Y826">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z826">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA826">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB826">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC826">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="827" spans="1:29">
@@ -74059,7 +74059,7 @@
         <v>825</v>
       </c>
       <c r="B827">
-        <v>6078269</v>
+        <v>6077768</v>
       </c>
       <c r="C827" t="s">
         <v>28</v>
@@ -74071,76 +74071,76 @@
         <v>45269.75</v>
       </c>
       <c r="F827" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G827" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H827">
+        <v>0</v>
+      </c>
+      <c r="I827">
         <v>3</v>
       </c>
-      <c r="I827">
-        <v>1</v>
-      </c>
       <c r="J827" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K827">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="L827">
+        <v>3.5</v>
+      </c>
+      <c r="M827">
         <v>3.4</v>
       </c>
-      <c r="M827">
-        <v>4.333</v>
-      </c>
       <c r="N827">
-        <v>1.8</v>
+        <v>2.05</v>
       </c>
       <c r="O827">
         <v>3.6</v>
       </c>
       <c r="P827">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="Q827">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R827">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S827">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="T827">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U827">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V827">
         <v>1.825</v>
       </c>
       <c r="W827">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="X827">
         <v>-1</v>
       </c>
       <c r="Y827">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z827">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA827">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB827">
-        <v>1.025</v>
+        <v>0.4875</v>
       </c>
       <c r="AC827">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="828" spans="1:29">
@@ -74148,7 +74148,7 @@
         <v>826</v>
       </c>
       <c r="B828">
-        <v>6077768</v>
+        <v>6078269</v>
       </c>
       <c r="C828" t="s">
         <v>28</v>
@@ -74160,76 +74160,76 @@
         <v>45269.75</v>
       </c>
       <c r="F828" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G828" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H828">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I828">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J828" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K828">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="L828">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M828">
-        <v>3.4</v>
+        <v>4.333</v>
       </c>
       <c r="N828">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="O828">
         <v>3.6</v>
       </c>
       <c r="P828">
-        <v>3.4</v>
+        <v>4.5</v>
       </c>
       <c r="Q828">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R828">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S828">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="T828">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U828">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V828">
         <v>1.825</v>
       </c>
       <c r="W828">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X828">
         <v>-1</v>
       </c>
       <c r="Y828">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z828">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA828">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB828">
-        <v>0.4875</v>
+        <v>1.025</v>
       </c>
       <c r="AC828">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="829" spans="1:29">
@@ -74237,7 +74237,7 @@
         <v>827</v>
       </c>
       <c r="B829">
-        <v>6078268</v>
+        <v>6078998</v>
       </c>
       <c r="C829" t="s">
         <v>28</v>
@@ -74249,55 +74249,55 @@
         <v>45269.75</v>
       </c>
       <c r="F829" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G829" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="H829">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I829">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J829" t="s">
         <v>53</v>
       </c>
       <c r="K829">
+        <v>1.909</v>
+      </c>
+      <c r="L829">
+        <v>3.6</v>
+      </c>
+      <c r="M829">
+        <v>3.8</v>
+      </c>
+      <c r="N829">
+        <v>2.15</v>
+      </c>
+      <c r="O829">
+        <v>3.75</v>
+      </c>
+      <c r="P829">
         <v>3.1</v>
       </c>
-      <c r="L829">
-        <v>3.3</v>
-      </c>
-      <c r="M829">
-        <v>2.3</v>
-      </c>
-      <c r="N829">
-        <v>2.9</v>
-      </c>
-      <c r="O829">
-        <v>3.4</v>
-      </c>
-      <c r="P829">
-        <v>2.375</v>
-      </c>
       <c r="Q829">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R829">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S829">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="T829">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U829">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V829">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="W829">
         <v>-1</v>
@@ -74306,19 +74306,19 @@
         <v>-1</v>
       </c>
       <c r="Y829">
-        <v>1.375</v>
+        <v>2.1</v>
       </c>
       <c r="Z829">
         <v>-1</v>
       </c>
       <c r="AA829">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="AB829">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC829">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="830" spans="1:29">
@@ -74326,7 +74326,7 @@
         <v>828</v>
       </c>
       <c r="B830">
-        <v>6077499</v>
+        <v>6078268</v>
       </c>
       <c r="C830" t="s">
         <v>28</v>
@@ -74338,28 +74338,28 @@
         <v>45269.75</v>
       </c>
       <c r="F830" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G830" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H830">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I830">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J830" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K830">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="L830">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="M830">
-        <v>3.4</v>
+        <v>2.3</v>
       </c>
       <c r="N830">
         <v>2.9</v>
@@ -74368,46 +74368,46 @@
         <v>3.4</v>
       </c>
       <c r="P830">
-        <v>2.4</v>
+        <v>2.375</v>
       </c>
       <c r="Q830">
         <v>0.25</v>
       </c>
       <c r="R830">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="S830">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="T830">
         <v>2.75</v>
       </c>
       <c r="U830">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="V830">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="W830">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="X830">
         <v>-1</v>
       </c>
       <c r="Y830">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Z830">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA830">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB830">
         <v>-1</v>
       </c>
       <c r="AC830">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-02-08 às 00:22
</commit_message>
<xml_diff>
--- a/Chile Primera Division/Chile Primera Division.xlsx
+++ b/Chile Primera Division/Chile Primera Division.xlsx
@@ -2752,7 +2752,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6073146</v>
+        <v>6078853</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -2764,73 +2764,73 @@
         <v>44967.875</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G26" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K26">
-        <v>2.7</v>
+        <v>2.625</v>
       </c>
       <c r="L26">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="M26">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="N26">
-        <v>3.3</v>
+        <v>1.909</v>
       </c>
       <c r="O26">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="P26">
-        <v>2.25</v>
+        <v>4.2</v>
       </c>
       <c r="Q26">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R26">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="S26">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="T26">
         <v>2.5</v>
       </c>
       <c r="U26">
+        <v>1.925</v>
+      </c>
+      <c r="V26">
         <v>1.875</v>
       </c>
-      <c r="V26">
-        <v>1.925</v>
-      </c>
       <c r="W26">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X26">
         <v>-1</v>
       </c>
       <c r="Y26">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Z26">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA26">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB26">
-        <v>0.875</v>
+        <v>0.925</v>
       </c>
       <c r="AC26">
         <v>-1</v>
@@ -2841,7 +2841,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>6078853</v>
+        <v>6073146</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -2853,73 +2853,73 @@
         <v>44967.875</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>3</v>
       </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
       <c r="J27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K27">
-        <v>2.625</v>
+        <v>2.7</v>
       </c>
       <c r="L27">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="M27">
-        <v>2.4</v>
+        <v>2.45</v>
       </c>
       <c r="N27">
-        <v>1.909</v>
+        <v>3.3</v>
       </c>
       <c r="O27">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="P27">
-        <v>4.2</v>
+        <v>2.25</v>
       </c>
       <c r="Q27">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R27">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="S27">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="T27">
         <v>2.5</v>
       </c>
       <c r="U27">
+        <v>1.875</v>
+      </c>
+      <c r="V27">
         <v>1.925</v>
       </c>
-      <c r="V27">
-        <v>1.875</v>
-      </c>
       <c r="W27">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X27">
         <v>-1</v>
       </c>
       <c r="Y27">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="Z27">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA27">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB27">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AC27">
         <v>-1</v>
@@ -4443,7 +4443,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>6078935</v>
+        <v>6073148</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
@@ -4455,73 +4455,73 @@
         <v>44984.85416666666</v>
       </c>
       <c r="F45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45" t="s">
+        <v>46</v>
+      </c>
+      <c r="K45">
+        <v>3.2</v>
+      </c>
+      <c r="L45">
+        <v>3.4</v>
+      </c>
+      <c r="M45">
+        <v>2.2</v>
+      </c>
+      <c r="N45">
+        <v>2.4</v>
+      </c>
+      <c r="O45">
+        <v>3.25</v>
+      </c>
+      <c r="P45">
         <v>3</v>
       </c>
-      <c r="I45">
-        <v>1</v>
-      </c>
-      <c r="J45" t="s">
-        <v>47</v>
-      </c>
-      <c r="K45">
-        <v>1.95</v>
-      </c>
-      <c r="L45">
-        <v>3.5</v>
-      </c>
-      <c r="M45">
-        <v>3.8</v>
-      </c>
-      <c r="N45">
+      <c r="Q45">
+        <v>-0.25</v>
+      </c>
+      <c r="R45">
+        <v>2.05</v>
+      </c>
+      <c r="S45">
         <v>1.75</v>
       </c>
-      <c r="O45">
-        <v>4</v>
-      </c>
-      <c r="P45">
-        <v>4.5</v>
-      </c>
-      <c r="Q45">
-        <v>-0.75</v>
-      </c>
-      <c r="R45">
-        <v>1.95</v>
-      </c>
-      <c r="S45">
-        <v>1.85</v>
-      </c>
       <c r="T45">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U45">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="V45">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W45">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="X45">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="Y45">
         <v>-1</v>
       </c>
       <c r="Z45">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="AA45">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AB45">
-        <v>0.925</v>
+        <v>0.8</v>
       </c>
       <c r="AC45">
         <v>-1</v>
@@ -4532,7 +4532,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>6073148</v>
+        <v>6078935</v>
       </c>
       <c r="C46" t="s">
         <v>28</v>
@@ -4544,73 +4544,73 @@
         <v>44984.85416666666</v>
       </c>
       <c r="F46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G46" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K46">
-        <v>3.2</v>
+        <v>1.95</v>
       </c>
       <c r="L46">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M46">
-        <v>2.2</v>
+        <v>3.8</v>
       </c>
       <c r="N46">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="O46">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="P46">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="Q46">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R46">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S46">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
       <c r="T46">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="U46">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V46">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W46">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="X46">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="Y46">
         <v>-1</v>
       </c>
       <c r="Z46">
-        <v>-0.5</v>
+        <v>0.95</v>
       </c>
       <c r="AA46">
-        <v>0.375</v>
+        <v>-1</v>
       </c>
       <c r="AB46">
-        <v>0.8</v>
+        <v>0.925</v>
       </c>
       <c r="AC46">
         <v>-1</v>
@@ -6312,7 +6312,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>6075784</v>
+        <v>6078866</v>
       </c>
       <c r="C66" t="s">
         <v>28</v>
@@ -6324,70 +6324,70 @@
         <v>45004.85416666666</v>
       </c>
       <c r="F66" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G66" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K66">
-        <v>3</v>
+        <v>2.625</v>
       </c>
       <c r="L66">
         <v>3.3</v>
       </c>
       <c r="M66">
+        <v>2.375</v>
+      </c>
+      <c r="N66">
+        <v>3.3</v>
+      </c>
+      <c r="O66">
+        <v>3.5</v>
+      </c>
+      <c r="P66">
         <v>2.15</v>
-      </c>
-      <c r="N66">
-        <v>3.4</v>
-      </c>
-      <c r="O66">
-        <v>3.6</v>
-      </c>
-      <c r="P66">
-        <v>2.05</v>
       </c>
       <c r="Q66">
         <v>0.25</v>
       </c>
       <c r="R66">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="S66">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="T66">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U66">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V66">
         <v>1.925</v>
       </c>
       <c r="W66">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="X66">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y66">
         <v>-1</v>
       </c>
       <c r="Z66">
-        <v>0.5125</v>
+        <v>0.95</v>
       </c>
       <c r="AA66">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB66">
         <v>-1</v>
@@ -6401,7 +6401,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>6078866</v>
+        <v>6075784</v>
       </c>
       <c r="C67" t="s">
         <v>28</v>
@@ -6413,70 +6413,70 @@
         <v>45004.85416666666</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G67" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K67">
-        <v>2.625</v>
+        <v>3</v>
       </c>
       <c r="L67">
         <v>3.3</v>
       </c>
       <c r="M67">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N67">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="O67">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="P67">
-        <v>2.15</v>
+        <v>2.05</v>
       </c>
       <c r="Q67">
         <v>0.25</v>
       </c>
       <c r="R67">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S67">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="T67">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U67">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V67">
         <v>1.925</v>
       </c>
       <c r="W67">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="X67">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y67">
         <v>-1</v>
       </c>
       <c r="Z67">
-        <v>0.95</v>
+        <v>0.5125</v>
       </c>
       <c r="AA67">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB67">
         <v>-1</v>
@@ -8804,7 +8804,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>6075792</v>
+        <v>6078878</v>
       </c>
       <c r="C94" t="s">
         <v>28</v>
@@ -8816,58 +8816,58 @@
         <v>45055.79166666666</v>
       </c>
       <c r="F94" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G94" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I94">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J94" t="s">
         <v>47</v>
       </c>
       <c r="K94">
-        <v>1.85</v>
+        <v>2.2</v>
       </c>
       <c r="L94">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="M94">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="N94">
-        <v>1.95</v>
+        <v>2.55</v>
       </c>
       <c r="O94">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="P94">
-        <v>4</v>
+        <v>2.875</v>
       </c>
       <c r="Q94">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R94">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S94">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T94">
         <v>2.5</v>
       </c>
       <c r="U94">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V94">
         <v>1.875</v>
       </c>
       <c r="W94">
-        <v>0.95</v>
+        <v>1.55</v>
       </c>
       <c r="X94">
         <v>-1</v>
@@ -8876,16 +8876,16 @@
         <v>-1</v>
       </c>
       <c r="Z94">
-        <v>0.8999999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="AA94">
         <v>-1</v>
       </c>
       <c r="AB94">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC94">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="95" spans="1:29">
@@ -8893,7 +8893,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>6078878</v>
+        <v>6075792</v>
       </c>
       <c r="C95" t="s">
         <v>28</v>
@@ -8905,58 +8905,58 @@
         <v>45055.79166666666</v>
       </c>
       <c r="F95" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G95" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H95">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I95">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J95" t="s">
         <v>47</v>
       </c>
       <c r="K95">
-        <v>2.2</v>
+        <v>1.85</v>
       </c>
       <c r="L95">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="M95">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="N95">
-        <v>2.55</v>
+        <v>1.95</v>
       </c>
       <c r="O95">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="P95">
-        <v>2.875</v>
+        <v>4</v>
       </c>
       <c r="Q95">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R95">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="S95">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="T95">
         <v>2.5</v>
       </c>
       <c r="U95">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V95">
         <v>1.875</v>
       </c>
       <c r="W95">
-        <v>1.55</v>
+        <v>0.95</v>
       </c>
       <c r="X95">
         <v>-1</v>
@@ -8965,16 +8965,16 @@
         <v>-1</v>
       </c>
       <c r="Z95">
-        <v>0.8</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA95">
         <v>-1</v>
       </c>
       <c r="AB95">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC95">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="96" spans="1:29">
@@ -9071,7 +9071,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>6532619</v>
+        <v>6078876</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9083,58 +9083,58 @@
         <v>45056.79166666666</v>
       </c>
       <c r="F97" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G97" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J97" t="s">
         <v>47</v>
       </c>
       <c r="K97">
-        <v>2.55</v>
+        <v>1.85</v>
       </c>
       <c r="L97">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M97">
+        <v>3.75</v>
+      </c>
+      <c r="N97">
+        <v>1.909</v>
+      </c>
+      <c r="O97">
+        <v>3.6</v>
+      </c>
+      <c r="P97">
+        <v>4.2</v>
+      </c>
+      <c r="Q97">
+        <v>-0.5</v>
+      </c>
+      <c r="R97">
+        <v>1.85</v>
+      </c>
+      <c r="S97">
+        <v>1.95</v>
+      </c>
+      <c r="T97">
         <v>2.5</v>
       </c>
-      <c r="N97">
-        <v>2.45</v>
-      </c>
-      <c r="O97">
-        <v>3.3</v>
-      </c>
-      <c r="P97">
-        <v>3</v>
-      </c>
-      <c r="Q97">
-        <v>-0.25</v>
-      </c>
-      <c r="R97">
-        <v>2.05</v>
-      </c>
-      <c r="S97">
-        <v>1.75</v>
-      </c>
-      <c r="T97">
-        <v>2.25</v>
-      </c>
       <c r="U97">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="V97">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W97">
-        <v>1.45</v>
+        <v>0.909</v>
       </c>
       <c r="X97">
         <v>-1</v>
@@ -9143,16 +9143,16 @@
         <v>-1</v>
       </c>
       <c r="Z97">
-        <v>1.05</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA97">
         <v>-1</v>
       </c>
       <c r="AB97">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC97">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="98" spans="1:29">
@@ -9160,7 +9160,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>6078876</v>
+        <v>6532619</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9172,58 +9172,58 @@
         <v>45056.79166666666</v>
       </c>
       <c r="F98" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G98" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J98" t="s">
         <v>47</v>
       </c>
       <c r="K98">
-        <v>1.85</v>
+        <v>2.55</v>
       </c>
       <c r="L98">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M98">
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
       <c r="N98">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="O98">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="P98">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="Q98">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R98">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="S98">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="T98">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="U98">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="V98">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="W98">
-        <v>0.909</v>
+        <v>1.45</v>
       </c>
       <c r="X98">
         <v>-1</v>
@@ -9232,16 +9232,16 @@
         <v>-1</v>
       </c>
       <c r="Z98">
-        <v>0.8500000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="AA98">
         <v>-1</v>
       </c>
       <c r="AB98">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC98">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="99" spans="1:29">
@@ -19306,7 +19306,7 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>7323186</v>
+        <v>7323253</v>
       </c>
       <c r="C212" t="s">
         <v>28</v>
@@ -19318,19 +19318,19 @@
         <v>45242.83333333334</v>
       </c>
       <c r="F212" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G212" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="H212">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I212">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J212" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K212">
         <v>2</v>
@@ -19342,52 +19342,52 @@
         <v>3.5</v>
       </c>
       <c r="N212">
-        <v>1.727</v>
+        <v>2.1</v>
       </c>
       <c r="O212">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="P212">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
       <c r="Q212">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R212">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S212">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T212">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U212">
+        <v>1.95</v>
+      </c>
+      <c r="V212">
         <v>1.85</v>
       </c>
-      <c r="V212">
-        <v>1.95</v>
-      </c>
       <c r="W212">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X212">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y212">
         <v>-1</v>
       </c>
       <c r="Z212">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AA212">
-        <v>-0.5</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB212">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC212">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="213" spans="1:29">
@@ -19395,7 +19395,7 @@
         <v>211</v>
       </c>
       <c r="B213">
-        <v>7323253</v>
+        <v>7323186</v>
       </c>
       <c r="C213" t="s">
         <v>28</v>
@@ -19407,19 +19407,19 @@
         <v>45242.83333333334</v>
       </c>
       <c r="F213" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G213" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H213">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I213">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J213" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K213">
         <v>2</v>
@@ -19431,52 +19431,52 @@
         <v>3.5</v>
       </c>
       <c r="N213">
-        <v>2.1</v>
+        <v>1.727</v>
       </c>
       <c r="O213">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="P213">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="Q213">
+        <v>-0.75</v>
+      </c>
+      <c r="R213">
+        <v>1.9</v>
+      </c>
+      <c r="S213">
+        <v>1.9</v>
+      </c>
+      <c r="T213">
+        <v>2.75</v>
+      </c>
+      <c r="U213">
+        <v>1.85</v>
+      </c>
+      <c r="V213">
+        <v>1.95</v>
+      </c>
+      <c r="W213">
+        <v>0.7270000000000001</v>
+      </c>
+      <c r="X213">
+        <v>-1</v>
+      </c>
+      <c r="Y213">
+        <v>-1</v>
+      </c>
+      <c r="Z213">
+        <v>0.45</v>
+      </c>
+      <c r="AA213">
         <v>-0.5</v>
       </c>
-      <c r="R213">
-        <v>2.025</v>
-      </c>
-      <c r="S213">
-        <v>1.775</v>
-      </c>
-      <c r="T213">
-        <v>2.5</v>
-      </c>
-      <c r="U213">
-        <v>1.95</v>
-      </c>
-      <c r="V213">
-        <v>1.85</v>
-      </c>
-      <c r="W213">
-        <v>-1</v>
-      </c>
-      <c r="X213">
-        <v>2.5</v>
-      </c>
-      <c r="Y213">
-        <v>-1</v>
-      </c>
-      <c r="Z213">
-        <v>-1</v>
-      </c>
-      <c r="AA213">
-        <v>0.7749999999999999</v>
-      </c>
       <c r="AB213">
+        <v>-1</v>
+      </c>
+      <c r="AC213">
         <v>0.95</v>
-      </c>
-      <c r="AC213">
-        <v>-1</v>
       </c>
     </row>
     <row r="214" spans="1:29">
@@ -20018,7 +20018,7 @@
         <v>218</v>
       </c>
       <c r="B220">
-        <v>6077497</v>
+        <v>6077763</v>
       </c>
       <c r="C220" t="s">
         <v>28</v>
@@ -20030,37 +20030,37 @@
         <v>45256.85416666666</v>
       </c>
       <c r="F220" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G220" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H220">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I220">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J220" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K220">
+        <v>2.15</v>
+      </c>
+      <c r="L220">
+        <v>3.5</v>
+      </c>
+      <c r="M220">
+        <v>3.2</v>
+      </c>
+      <c r="N220">
+        <v>2.625</v>
+      </c>
+      <c r="O220">
+        <v>3.5</v>
+      </c>
+      <c r="P220">
         <v>2.6</v>
-      </c>
-      <c r="L220">
-        <v>3.4</v>
-      </c>
-      <c r="M220">
-        <v>2.6</v>
-      </c>
-      <c r="N220">
-        <v>2.8</v>
-      </c>
-      <c r="O220">
-        <v>3.2</v>
-      </c>
-      <c r="P220">
-        <v>2.7</v>
       </c>
       <c r="Q220">
         <v>0</v>
@@ -20072,34 +20072,34 @@
         <v>1.9</v>
       </c>
       <c r="T220">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U220">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V220">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="W220">
         <v>-1</v>
       </c>
       <c r="X220">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y220">
-        <v>-1</v>
+        <v>1.6</v>
       </c>
       <c r="Z220">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA220">
-        <v>-0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB220">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC220">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="221" spans="1:29">
@@ -20107,7 +20107,7 @@
         <v>219</v>
       </c>
       <c r="B221">
-        <v>6077763</v>
+        <v>6077497</v>
       </c>
       <c r="C221" t="s">
         <v>28</v>
@@ -20119,37 +20119,37 @@
         <v>45256.85416666666</v>
       </c>
       <c r="F221" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G221" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H221">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I221">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J221" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K221">
-        <v>2.15</v>
+        <v>2.6</v>
       </c>
       <c r="L221">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M221">
+        <v>2.6</v>
+      </c>
+      <c r="N221">
+        <v>2.8</v>
+      </c>
+      <c r="O221">
         <v>3.2</v>
       </c>
-      <c r="N221">
-        <v>2.625</v>
-      </c>
-      <c r="O221">
-        <v>3.5</v>
-      </c>
       <c r="P221">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="Q221">
         <v>0</v>
@@ -20161,34 +20161,34 @@
         <v>1.9</v>
       </c>
       <c r="T221">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U221">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="V221">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="W221">
         <v>-1</v>
       </c>
       <c r="X221">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y221">
-        <v>1.6</v>
+        <v>-1</v>
       </c>
       <c r="Z221">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA221">
-        <v>0.8999999999999999</v>
+        <v>-0</v>
       </c>
       <c r="AB221">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AC221">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="222" spans="1:29">
@@ -20730,7 +20730,7 @@
         <v>226</v>
       </c>
       <c r="B228">
-        <v>6077767</v>
+        <v>6078263</v>
       </c>
       <c r="C228" t="s">
         <v>28</v>
@@ -20742,76 +20742,76 @@
         <v>45263.75</v>
       </c>
       <c r="F228" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G228" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H228">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I228">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J228" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K228">
-        <v>2.75</v>
+        <v>2.05</v>
       </c>
       <c r="L228">
         <v>3.4</v>
       </c>
       <c r="M228">
-        <v>2.45</v>
+        <v>3.5</v>
       </c>
       <c r="N228">
-        <v>2.875</v>
+        <v>2.05</v>
       </c>
       <c r="O228">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="P228">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="Q228">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R228">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="S228">
         <v>1.8</v>
       </c>
       <c r="T228">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="U228">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V228">
-        <v>2.05</v>
+        <v>1.9</v>
       </c>
       <c r="W228">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="X228">
         <v>-1</v>
       </c>
       <c r="Y228">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="Z228">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA228">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB228">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC228">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="229" spans="1:29">
@@ -20819,7 +20819,7 @@
         <v>227</v>
       </c>
       <c r="B229">
-        <v>6078263</v>
+        <v>6077767</v>
       </c>
       <c r="C229" t="s">
         <v>28</v>
@@ -20831,76 +20831,76 @@
         <v>45263.75</v>
       </c>
       <c r="F229" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G229" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H229">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I229">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J229" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K229">
-        <v>2.05</v>
+        <v>2.75</v>
       </c>
       <c r="L229">
         <v>3.4</v>
       </c>
       <c r="M229">
-        <v>3.5</v>
+        <v>2.45</v>
       </c>
       <c r="N229">
+        <v>2.875</v>
+      </c>
+      <c r="O229">
+        <v>3.3</v>
+      </c>
+      <c r="P229">
+        <v>2.5</v>
+      </c>
+      <c r="Q229">
+        <v>0</v>
+      </c>
+      <c r="R229">
         <v>2.05</v>
-      </c>
-      <c r="O229">
-        <v>3.6</v>
-      </c>
-      <c r="P229">
-        <v>3.5</v>
-      </c>
-      <c r="Q229">
-        <v>-0.5</v>
-      </c>
-      <c r="R229">
-        <v>2</v>
       </c>
       <c r="S229">
         <v>1.8</v>
       </c>
       <c r="T229">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="U229">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V229">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="W229">
+        <v>-1</v>
+      </c>
+      <c r="X229">
+        <v>-1</v>
+      </c>
+      <c r="Y229">
+        <v>1.5</v>
+      </c>
+      <c r="Z229">
+        <v>-1</v>
+      </c>
+      <c r="AA229">
+        <v>0.8</v>
+      </c>
+      <c r="AB229">
+        <v>-1</v>
+      </c>
+      <c r="AC229">
         <v>1.05</v>
-      </c>
-      <c r="X229">
-        <v>-1</v>
-      </c>
-      <c r="Y229">
-        <v>-1</v>
-      </c>
-      <c r="Z229">
-        <v>1</v>
-      </c>
-      <c r="AA229">
-        <v>-1</v>
-      </c>
-      <c r="AB229">
-        <v>0.8999999999999999</v>
-      </c>
-      <c r="AC229">
-        <v>-1</v>
       </c>
     </row>
     <row r="230" spans="1:29">
@@ -20908,7 +20908,7 @@
         <v>228</v>
       </c>
       <c r="B230">
-        <v>6078267</v>
+        <v>6078997</v>
       </c>
       <c r="C230" t="s">
         <v>28</v>
@@ -20920,13 +20920,13 @@
         <v>45268.75</v>
       </c>
       <c r="F230" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G230" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H230">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I230">
         <v>0</v>
@@ -20935,28 +20935,28 @@
         <v>47</v>
       </c>
       <c r="K230">
-        <v>1.5</v>
+        <v>3.8</v>
       </c>
       <c r="L230">
-        <v>4.333</v>
+        <v>3.6</v>
       </c>
       <c r="M230">
-        <v>6</v>
+        <v>1.909</v>
       </c>
       <c r="N230">
-        <v>1.444</v>
+        <v>2.7</v>
       </c>
       <c r="O230">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="P230">
-        <v>7</v>
+        <v>2.45</v>
       </c>
       <c r="Q230">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="R230">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="S230">
         <v>1.825</v>
@@ -20965,13 +20965,13 @@
         <v>2.75</v>
       </c>
       <c r="U230">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="V230">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="W230">
-        <v>0.444</v>
+        <v>1.7</v>
       </c>
       <c r="X230">
         <v>-1</v>
@@ -20980,16 +20980,16 @@
         <v>-1</v>
       </c>
       <c r="Z230">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AA230">
+        <v>-1</v>
+      </c>
+      <c r="AB230">
+        <v>-1</v>
+      </c>
+      <c r="AC230">
         <v>1.025</v>
-      </c>
-      <c r="AA230">
-        <v>-1</v>
-      </c>
-      <c r="AB230">
-        <v>-1</v>
-      </c>
-      <c r="AC230">
-        <v>1.05</v>
       </c>
     </row>
     <row r="231" spans="1:29">
@@ -20997,7 +20997,7 @@
         <v>229</v>
       </c>
       <c r="B231">
-        <v>6143704</v>
+        <v>6078267</v>
       </c>
       <c r="C231" t="s">
         <v>28</v>
@@ -21009,67 +21009,67 @@
         <v>45268.75</v>
       </c>
       <c r="F231" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G231" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H231">
+        <v>2</v>
+      </c>
+      <c r="I231">
         <v>0</v>
       </c>
-      <c r="I231">
-        <v>1</v>
-      </c>
       <c r="J231" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K231">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="L231">
+        <v>4.333</v>
+      </c>
+      <c r="M231">
+        <v>6</v>
+      </c>
+      <c r="N231">
+        <v>1.444</v>
+      </c>
+      <c r="O231">
         <v>4.75</v>
       </c>
-      <c r="M231">
-        <v>1.4</v>
-      </c>
-      <c r="N231">
-        <v>12</v>
-      </c>
-      <c r="O231">
-        <v>8.5</v>
-      </c>
       <c r="P231">
-        <v>1.166</v>
+        <v>7</v>
       </c>
       <c r="Q231">
-        <v>2</v>
+        <v>-1.25</v>
       </c>
       <c r="R231">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="S231">
+        <v>1.825</v>
+      </c>
+      <c r="T231">
+        <v>2.75</v>
+      </c>
+      <c r="U231">
         <v>1.8</v>
       </c>
-      <c r="T231">
-        <v>3.25</v>
-      </c>
-      <c r="U231">
-        <v>1.875</v>
-      </c>
       <c r="V231">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="W231">
-        <v>-1</v>
+        <v>0.444</v>
       </c>
       <c r="X231">
         <v>-1</v>
       </c>
       <c r="Y231">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z231">
-        <v>1</v>
+        <v>1.025</v>
       </c>
       <c r="AA231">
         <v>-1</v>
@@ -21078,7 +21078,7 @@
         <v>-1</v>
       </c>
       <c r="AC231">
-        <v>0.925</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="232" spans="1:29">
@@ -21086,7 +21086,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>6078997</v>
+        <v>6143704</v>
       </c>
       <c r="C232" t="s">
         <v>28</v>
@@ -21098,67 +21098,67 @@
         <v>45268.75</v>
       </c>
       <c r="F232" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G232" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="H232">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J232" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K232">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
       <c r="L232">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="M232">
-        <v>1.909</v>
+        <v>1.4</v>
       </c>
       <c r="N232">
-        <v>2.7</v>
+        <v>12</v>
       </c>
       <c r="O232">
-        <v>3.6</v>
+        <v>8.5</v>
       </c>
       <c r="P232">
-        <v>2.45</v>
+        <v>1.166</v>
       </c>
       <c r="Q232">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R232">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S232">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T232">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U232">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="V232">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W232">
-        <v>1.7</v>
+        <v>-1</v>
       </c>
       <c r="X232">
         <v>-1</v>
       </c>
       <c r="Y232">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="Z232">
-        <v>0.9750000000000001</v>
+        <v>1</v>
       </c>
       <c r="AA232">
         <v>-1</v>
@@ -21167,7 +21167,7 @@
         <v>-1</v>
       </c>
       <c r="AC232">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="233" spans="1:29">
@@ -21175,7 +21175,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>6077499</v>
+        <v>6077768</v>
       </c>
       <c r="C233" t="s">
         <v>28</v>
@@ -21187,76 +21187,76 @@
         <v>45269.75</v>
       </c>
       <c r="F233" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G233" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H233">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I233">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J233" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K233">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="L233">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M233">
         <v>3.4</v>
       </c>
       <c r="N233">
-        <v>2.9</v>
+        <v>2.05</v>
       </c>
       <c r="O233">
+        <v>3.6</v>
+      </c>
+      <c r="P233">
         <v>3.4</v>
       </c>
-      <c r="P233">
-        <v>2.4</v>
-      </c>
       <c r="Q233">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R233">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="S233">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="T233">
         <v>2.75</v>
       </c>
       <c r="U233">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V233">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W233">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="X233">
         <v>-1</v>
       </c>
       <c r="Y233">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z233">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA233">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB233">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AC233">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="234" spans="1:29">
@@ -21264,7 +21264,7 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>6078269</v>
+        <v>6077499</v>
       </c>
       <c r="C234" t="s">
         <v>28</v>
@@ -21276,58 +21276,58 @@
         <v>45269.75</v>
       </c>
       <c r="F234" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G234" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H234">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J234" t="s">
         <v>47</v>
       </c>
       <c r="K234">
-        <v>1.85</v>
+        <v>2.1</v>
       </c>
       <c r="L234">
         <v>3.4</v>
       </c>
       <c r="M234">
-        <v>4.333</v>
+        <v>3.4</v>
       </c>
       <c r="N234">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="O234">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="P234">
-        <v>4.5</v>
+        <v>2.4</v>
       </c>
       <c r="Q234">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R234">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="S234">
-        <v>1.925</v>
+        <v>2.1</v>
       </c>
       <c r="T234">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U234">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V234">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W234">
-        <v>0.8</v>
+        <v>1.9</v>
       </c>
       <c r="X234">
         <v>-1</v>
@@ -21336,16 +21336,16 @@
         <v>-1</v>
       </c>
       <c r="Z234">
-        <v>0.925</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA234">
         <v>-1</v>
       </c>
       <c r="AB234">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AC234">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:29">
@@ -21353,7 +21353,7 @@
         <v>233</v>
       </c>
       <c r="B235">
-        <v>6078268</v>
+        <v>6078998</v>
       </c>
       <c r="C235" t="s">
         <v>28</v>
@@ -21365,55 +21365,55 @@
         <v>45269.75</v>
       </c>
       <c r="F235" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G235" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H235">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I235">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J235" t="s">
         <v>45</v>
       </c>
       <c r="K235">
+        <v>1.909</v>
+      </c>
+      <c r="L235">
+        <v>3.6</v>
+      </c>
+      <c r="M235">
+        <v>3.8</v>
+      </c>
+      <c r="N235">
+        <v>2.15</v>
+      </c>
+      <c r="O235">
+        <v>3.75</v>
+      </c>
+      <c r="P235">
         <v>3.1</v>
       </c>
-      <c r="L235">
-        <v>3.3</v>
-      </c>
-      <c r="M235">
-        <v>2.3</v>
-      </c>
-      <c r="N235">
-        <v>2.9</v>
-      </c>
-      <c r="O235">
-        <v>3.4</v>
-      </c>
-      <c r="P235">
-        <v>2.375</v>
-      </c>
       <c r="Q235">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R235">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S235">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="T235">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U235">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V235">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="W235">
         <v>-1</v>
@@ -21422,19 +21422,19 @@
         <v>-1</v>
       </c>
       <c r="Y235">
-        <v>1.375</v>
+        <v>2.1</v>
       </c>
       <c r="Z235">
         <v>-1</v>
       </c>
       <c r="AA235">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="AB235">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC235">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="236" spans="1:29">
@@ -21442,7 +21442,7 @@
         <v>234</v>
       </c>
       <c r="B236">
-        <v>6077768</v>
+        <v>6078268</v>
       </c>
       <c r="C236" t="s">
         <v>28</v>
@@ -21454,40 +21454,40 @@
         <v>45269.75</v>
       </c>
       <c r="F236" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G236" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H236">
         <v>0</v>
       </c>
       <c r="I236">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J236" t="s">
         <v>45</v>
       </c>
       <c r="K236">
-        <v>2.05</v>
+        <v>3.1</v>
       </c>
       <c r="L236">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M236">
+        <v>2.3</v>
+      </c>
+      <c r="N236">
+        <v>2.9</v>
+      </c>
+      <c r="O236">
         <v>3.4</v>
       </c>
-      <c r="N236">
-        <v>2.05</v>
-      </c>
-      <c r="O236">
-        <v>3.6</v>
-      </c>
       <c r="P236">
-        <v>3.4</v>
+        <v>2.375</v>
       </c>
       <c r="Q236">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="R236">
         <v>1.8</v>
@@ -21499,10 +21499,10 @@
         <v>2.75</v>
       </c>
       <c r="U236">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="V236">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="W236">
         <v>-1</v>
@@ -21511,7 +21511,7 @@
         <v>-1</v>
       </c>
       <c r="Y236">
-        <v>2.4</v>
+        <v>1.375</v>
       </c>
       <c r="Z236">
         <v>-1</v>
@@ -21520,10 +21520,10 @@
         <v>1</v>
       </c>
       <c r="AB236">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AC236">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="237" spans="1:29">
@@ -21531,7 +21531,7 @@
         <v>235</v>
       </c>
       <c r="B237">
-        <v>6078998</v>
+        <v>6078269</v>
       </c>
       <c r="C237" t="s">
         <v>28</v>
@@ -21543,73 +21543,73 @@
         <v>45269.75</v>
       </c>
       <c r="F237" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G237" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H237">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I237">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J237" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K237">
-        <v>1.909</v>
+        <v>1.85</v>
       </c>
       <c r="L237">
+        <v>3.4</v>
+      </c>
+      <c r="M237">
+        <v>4.333</v>
+      </c>
+      <c r="N237">
+        <v>1.8</v>
+      </c>
+      <c r="O237">
         <v>3.6</v>
       </c>
-      <c r="M237">
-        <v>3.8</v>
-      </c>
-      <c r="N237">
-        <v>2.15</v>
-      </c>
-      <c r="O237">
-        <v>3.75</v>
-      </c>
       <c r="P237">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="Q237">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R237">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S237">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="T237">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U237">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="V237">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W237">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X237">
         <v>-1</v>
       </c>
       <c r="Y237">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z237">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA237">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB237">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AC237">
         <v>-1</v>

</xml_diff>